<commit_message>
Encode filters in URL #922 in views (e.g. directory) create criteria from url and update filter components when going into case keep the criteria in the vaadin session cache add reset button do this for cases directory
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -273,7 +273,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.10.0-SNAPSHOT</t>
+    <t>1.11.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -2347,8 +2347,8 @@
       <c r="E35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>20</v>
+      <c r="F35" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>20</v>
@@ -2515,8 +2515,8 @@
       <c r="E38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>20</v>
+      <c r="F38" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
#900 reactivated automatic generation of caption properties and fixed genColumn entries
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="98">
   <si>
     <t>User Right</t>
   </si>
@@ -291,10 +291,22 @@
     <t>TREATMENT_DELETE</t>
   </si>
   <si>
+    <t>CLINICAL_COURSE_VIEW</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_CREATE</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_EDIT</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_DELETE</t>
+  </si>
+  <si>
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.12.0-SNAPSHOT</t>
+    <t>1.13.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -422,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S73"/>
+  <dimension ref="A1:S77"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4536,6 +4548,230 @@
         <v>20</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="B74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="B75" t="s">
+        <v>93</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R75" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R76" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="B77" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -4551,12 +4787,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1277 - Added content to the aggregate reports app view, added save and retrieval logic, overhauled disease configuration cache and disease configuration facade, added aggregate diseases, added caseBased property to disease
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="123">
   <si>
     <t>User Right</t>
   </si>
@@ -369,10 +369,19 @@
     <t>POPULATION_MANAGE</t>
   </si>
   <si>
+    <t>LINE_LISTING_CONFIGURE</t>
+  </si>
+  <si>
+    <t>LINE_LISTING_CONFIGURE_NATION</t>
+  </si>
+  <si>
+    <t>AGGREGATE_REPORT_VIEW</t>
+  </si>
+  <si>
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.30.0-SNAPSHOT</t>
+    <t>1.31.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -500,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W95"/>
+  <dimension ref="A1:W98"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -6990,6 +6999,210 @@
         <v>24</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="s" s="3">
+        <v>118</v>
+      </c>
+      <c r="B96" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U96" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V96" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="3">
+        <v>119</v>
+      </c>
+      <c r="B97" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U97" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V97" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="3">
+        <v>120</v>
+      </c>
+      <c r="B98" t="s">
+        <v>120</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O98" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V98" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -7005,12 +7218,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1637: Change facility selection
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -63,7 +63,7 @@
     <t>National Observer</t>
   </si>
   <si>
-    <t>State Observer</t>
+    <t>Region Observer</t>
   </si>
   <si>
     <t>District Observer</t>
@@ -108,7 +108,7 @@
     <t>District</t>
   </si>
   <si>
-    <t>Health facility</t>
+    <t>Facility</t>
   </si>
   <si>
     <t>Community</t>
@@ -492,7 +492,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.44.0-SNAPSHOT</t>
+    <t>1.45.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
#1637: finish web part and consider facility type in imports
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="163">
   <si>
     <t>User Right</t>
   </si>
@@ -63,7 +63,7 @@
     <t>National Observer</t>
   </si>
   <si>
-    <t>State Observer</t>
+    <t>Region Observer</t>
   </si>
   <si>
     <t>District Observer</t>
@@ -108,7 +108,7 @@
     <t>District</t>
   </si>
   <si>
-    <t>Health facility</t>
+    <t>Facility</t>
   </si>
   <si>
     <t>Community</t>
@@ -255,7 +255,7 @@
     <t>CONTACT_REASSIGN_CASE</t>
   </si>
   <si>
-    <t>CONTACT_CREATE_PIA_ACCOUNT</t>
+    <t>MANAGE_EXTERNAL_SYMPTOM_JOURNAL</t>
   </si>
   <si>
     <t>VISIT_CREATE</t>
@@ -288,6 +288,15 @@
     <t>TASK_DELETE</t>
   </si>
   <si>
+    <t>ACTION_CREATE</t>
+  </si>
+  <si>
+    <t>ACTION_DELETE</t>
+  </si>
+  <si>
+    <t>ACTION_EDIT</t>
+  </si>
+  <si>
     <t>EVENT_CREATE</t>
   </si>
   <si>
@@ -492,7 +501,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.45.0-SNAPSHOT</t>
+    <t>1.46.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z122"/>
+  <dimension ref="A1:Z125"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2076,8 +2085,8 @@
       <c r="L19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>38</v>
+      <c r="M19" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>37</v>
@@ -2230,8 +2239,8 @@
       <c r="L21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M21" s="2" t="s">
-        <v>38</v>
+      <c r="M21" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>37</v>
@@ -2307,8 +2316,8 @@
       <c r="L22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>38</v>
+      <c r="M22" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>38</v>
@@ -2692,8 +2701,8 @@
       <c r="L27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="2" t="s">
-        <v>38</v>
+      <c r="M27" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>37</v>
@@ -2769,8 +2778,8 @@
       <c r="L28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M28" s="2" t="s">
-        <v>38</v>
+      <c r="M28" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>37</v>
@@ -4975,35 +4984,35 @@
       <c r="C57" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>37</v>
+      <c r="D57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>38</v>
@@ -5011,23 +5020,23 @@
       <c r="O57" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T57" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U57" s="1" t="s">
-        <v>37</v>
+      <c r="P57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V57" s="2" t="s">
         <v>38</v>
@@ -5135,8 +5144,8 @@
       <c r="E59" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>38</v>
+      <c r="F59" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>38</v>
@@ -5144,23 +5153,23 @@
       <c r="H59" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>37</v>
+      <c r="I59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>37</v>
+      <c r="K59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M59" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>37</v>
+      <c r="M59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>38</v>
@@ -5174,17 +5183,17 @@
       <c r="R59" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S59" s="1" t="s">
-        <v>37</v>
+      <c r="S59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T59" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U59" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V59" s="1" t="s">
-        <v>37</v>
+      <c r="U59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V59" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W59" s="2" t="s">
         <v>38</v>
@@ -5206,35 +5215,35 @@
       <c r="C60" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>38</v>
+      <c r="D60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>38</v>
@@ -5242,23 +5251,23 @@
       <c r="O60" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U60" s="2" t="s">
-        <v>38</v>
+      <c r="P60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V60" s="2" t="s">
         <v>38</v>
@@ -5286,11 +5295,11 @@
       <c r="D61" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>38</v>
+      <c r="E61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>38</v>
@@ -5310,8 +5319,8 @@
       <c r="L61" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M61" s="2" t="s">
-        <v>38</v>
+      <c r="M61" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>38</v>
@@ -5363,8 +5372,8 @@
       <c r="D62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>38</v>
+      <c r="E62" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>38</v>
@@ -5390,20 +5399,20 @@
       <c r="M62" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N62" s="2" t="s">
-        <v>38</v>
+      <c r="N62" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P62" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R62" s="1" t="s">
-        <v>37</v>
+      <c r="P62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R62" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="S62" s="1" t="s">
         <v>37</v>
@@ -5437,14 +5446,14 @@
       <c r="C63" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>37</v>
+      <c r="D63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>38</v>
@@ -5464,8 +5473,8 @@
       <c r="L63" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M63" s="1" t="s">
-        <v>37</v>
+      <c r="M63" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>38</v>
@@ -5517,11 +5526,11 @@
       <c r="D64" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>37</v>
+      <c r="E64" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>38</v>
@@ -5541,8 +5550,8 @@
       <c r="L64" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M64" s="1" t="s">
-        <v>37</v>
+      <c r="M64" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>38</v>
@@ -5606,14 +5615,14 @@
       <c r="H65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I65" s="2" t="s">
-        <v>38</v>
+      <c r="I65" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K65" s="2" t="s">
-        <v>38</v>
+      <c r="K65" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>38</v>
@@ -5627,26 +5636,26 @@
       <c r="O65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P65" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q65" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R65" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S65" s="2" t="s">
-        <v>38</v>
+      <c r="P65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T65" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U65" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V65" s="2" t="s">
-        <v>38</v>
+      <c r="U65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V65" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W65" s="2" t="s">
         <v>38</v>
@@ -5665,23 +5674,23 @@
       <c r="B66" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>38</v>
+      <c r="C66" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>37</v>
+      <c r="G66" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>38</v>
@@ -5695,8 +5704,8 @@
       <c r="L66" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M66" s="2" t="s">
-        <v>38</v>
+      <c r="M66" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>38</v>
@@ -5754,26 +5763,26 @@
       <c r="F67" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>37</v>
+      <c r="G67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K67" s="1" t="s">
-        <v>37</v>
+      <c r="K67" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M67" s="2" t="s">
-        <v>38</v>
+      <c r="M67" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>38</v>
@@ -5781,17 +5790,17 @@
       <c r="O67" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S67" s="1" t="s">
-        <v>37</v>
+      <c r="P67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T67" s="2" t="s">
         <v>38</v>
@@ -5822,8 +5831,8 @@
       <c r="C68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>38</v>
+      <c r="D68" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>38</v>
@@ -5896,8 +5905,8 @@
       <c r="B69" t="s">
         <v>104</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>37</v>
+      <c r="C69" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>38</v>
@@ -5905,14 +5914,14 @@
       <c r="E69" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>38</v>
+      <c r="F69" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>38</v>
@@ -5976,29 +5985,29 @@
       <c r="C70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>38</v>
+      <c r="D70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K70" s="2" t="s">
-        <v>38</v>
+      <c r="K70" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>38</v>
@@ -6012,17 +6021,17 @@
       <c r="O70" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S70" s="2" t="s">
-        <v>38</v>
+      <c r="P70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T70" s="2" t="s">
         <v>38</v>
@@ -6053,11 +6062,11 @@
       <c r="C71" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>37</v>
+      <c r="D71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>38</v>
@@ -6089,26 +6098,26 @@
       <c r="O71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P71" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q71" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R71" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S71" s="1" t="s">
-        <v>37</v>
+      <c r="P71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U71" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V71" s="1" t="s">
-        <v>37</v>
+      <c r="U71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V71" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W71" s="2" t="s">
         <v>38</v>
@@ -6130,8 +6139,8 @@
       <c r="C72" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>37</v>
+      <c r="D72" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>38</v>
@@ -6204,14 +6213,14 @@
       <c r="B73" t="s">
         <v>108</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>38</v>
+      <c r="C73" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>37</v>
+      <c r="E73" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>38</v>
@@ -6299,14 +6308,14 @@
       <c r="H74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I74" s="1" t="s">
-        <v>37</v>
+      <c r="I74" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>37</v>
+      <c r="K74" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>38</v>
@@ -6314,8 +6323,8 @@
       <c r="M74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N74" s="1" t="s">
-        <v>37</v>
+      <c r="N74" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>38</v>
@@ -6364,8 +6373,8 @@
       <c r="D75" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>37</v>
+      <c r="E75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>38</v>
@@ -6376,14 +6385,14 @@
       <c r="H75" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I75" s="1" t="s">
-        <v>37</v>
+      <c r="I75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>37</v>
+      <c r="K75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>38</v>
@@ -6391,8 +6400,8 @@
       <c r="M75" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N75" s="1" t="s">
-        <v>37</v>
+      <c r="N75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>38</v>
@@ -6406,17 +6415,17 @@
       <c r="R75" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S75" s="1" t="s">
-        <v>37</v>
+      <c r="S75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T75" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U75" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V75" s="1" t="s">
-        <v>37</v>
+      <c r="U75" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V75" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W75" s="2" t="s">
         <v>38</v>
@@ -6435,14 +6444,14 @@
       <c r="B76" t="s">
         <v>111</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>38</v>
+      <c r="C76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>38</v>
@@ -6515,11 +6524,11 @@
       <c r="C77" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>38</v>
+      <c r="D77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>38</v>
@@ -6530,14 +6539,14 @@
       <c r="H77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I77" s="2" t="s">
-        <v>38</v>
+      <c r="I77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K77" s="2" t="s">
-        <v>38</v>
+      <c r="K77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>38</v>
@@ -6545,32 +6554,32 @@
       <c r="M77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N77" s="2" t="s">
-        <v>38</v>
+      <c r="N77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S77" s="2" t="s">
-        <v>38</v>
+      <c r="P77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V77" s="2" t="s">
-        <v>38</v>
+      <c r="U77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V77" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W77" s="2" t="s">
         <v>38</v>
@@ -6592,11 +6601,11 @@
       <c r="C78" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>38</v>
+      <c r="D78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>38</v>
@@ -6607,14 +6616,14 @@
       <c r="H78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I78" s="2" t="s">
-        <v>38</v>
+      <c r="I78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K78" s="2" t="s">
-        <v>38</v>
+      <c r="K78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>38</v>
@@ -6622,8 +6631,8 @@
       <c r="M78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N78" s="2" t="s">
-        <v>38</v>
+      <c r="N78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O78" s="2" t="s">
         <v>38</v>
@@ -6637,17 +6646,17 @@
       <c r="R78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S78" s="2" t="s">
-        <v>38</v>
+      <c r="S78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T78" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U78" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V78" s="2" t="s">
-        <v>38</v>
+      <c r="U78" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V78" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W78" s="2" t="s">
         <v>38</v>
@@ -6669,8 +6678,8 @@
       <c r="C79" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>38</v>
+      <c r="D79" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -6746,11 +6755,11 @@
       <c r="C80" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>37</v>
+      <c r="D80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>38</v>
@@ -6782,26 +6791,26 @@
       <c r="O80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S80" s="1" t="s">
-        <v>37</v>
+      <c r="P80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S80" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U80" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V80" s="1" t="s">
-        <v>37</v>
+      <c r="U80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V80" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W80" s="2" t="s">
         <v>38</v>
@@ -6823,8 +6832,8 @@
       <c r="C81" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>37</v>
+      <c r="D81" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>38</v>
@@ -6859,8 +6868,8 @@
       <c r="O81" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P81" s="1" t="s">
-        <v>37</v>
+      <c r="P81" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="Q81" s="2" t="s">
         <v>38</v>
@@ -6900,11 +6909,11 @@
       <c r="C82" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>37</v>
+      <c r="D82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>38</v>
@@ -6945,17 +6954,17 @@
       <c r="R82" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S82" s="1" t="s">
-        <v>37</v>
+      <c r="S82" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T82" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U82" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V82" s="1" t="s">
-        <v>37</v>
+      <c r="U82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V82" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W82" s="2" t="s">
         <v>38</v>
@@ -6977,11 +6986,11 @@
       <c r="C83" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>38</v>
+      <c r="D83" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>38</v>
@@ -7013,26 +7022,26 @@
       <c r="O83" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P83" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q83" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R83" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S83" s="2" t="s">
-        <v>38</v>
+      <c r="P83" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S83" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T83" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U83" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V83" s="2" t="s">
-        <v>38</v>
+      <c r="U83" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V83" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W83" s="2" t="s">
         <v>38</v>
@@ -7090,8 +7099,8 @@
       <c r="O84" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P84" s="2" t="s">
-        <v>38</v>
+      <c r="P84" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="Q84" s="2" t="s">
         <v>38</v>
@@ -7131,11 +7140,11 @@
       <c r="C85" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>38</v>
+      <c r="D85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>38</v>
@@ -7176,17 +7185,17 @@
       <c r="R85" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S85" s="2" t="s">
-        <v>38</v>
+      <c r="S85" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T85" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U85" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V85" s="2" t="s">
-        <v>38</v>
+      <c r="U85" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V85" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W85" s="2" t="s">
         <v>38</v>
@@ -7208,14 +7217,14 @@
       <c r="C86" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>37</v>
+      <c r="D86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>38</v>
@@ -7223,47 +7232,47 @@
       <c r="H86" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N86" s="1" t="s">
-        <v>37</v>
+      <c r="I86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N86" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S86" s="1" t="s">
-        <v>37</v>
+      <c r="P86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T86" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U86" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V86" s="1" t="s">
-        <v>37</v>
+      <c r="U86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V86" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W86" s="2" t="s">
         <v>38</v>
@@ -7288,11 +7297,11 @@
       <c r="D87" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>37</v>
+      <c r="E87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>38</v>
@@ -7300,11 +7309,11 @@
       <c r="H87" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>37</v>
+      <c r="I87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>38</v>
@@ -7312,35 +7321,35 @@
       <c r="L87" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N87" s="1" t="s">
-        <v>37</v>
+      <c r="M87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S87" s="1" t="s">
-        <v>37</v>
+      <c r="P87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T87" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U87" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V87" s="1" t="s">
-        <v>37</v>
+      <c r="U87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V87" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W87" s="2" t="s">
         <v>38</v>
@@ -7362,8 +7371,8 @@
       <c r="C88" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>37</v>
+      <c r="D88" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>38</v>
@@ -7383,11 +7392,11 @@
       <c r="J88" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K88" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L88" s="1" t="s">
-        <v>37</v>
+      <c r="K88" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>38</v>
@@ -7398,14 +7407,14 @@
       <c r="O88" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P88" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q88" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R88" s="1" t="s">
-        <v>37</v>
+      <c r="P88" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q88" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R88" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="S88" s="2" t="s">
         <v>38</v>
@@ -7442,11 +7451,11 @@
       <c r="D89" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>38</v>
+      <c r="E89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>38</v>
@@ -7454,23 +7463,23 @@
       <c r="H89" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>38</v>
+      <c r="I89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N89" s="2" t="s">
-        <v>38</v>
+      <c r="L89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>38</v>
@@ -7484,17 +7493,17 @@
       <c r="R89" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S89" s="2" t="s">
-        <v>38</v>
+      <c r="S89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T89" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U89" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V89" s="2" t="s">
-        <v>38</v>
+      <c r="U89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W89" s="2" t="s">
         <v>38</v>
@@ -7516,14 +7525,14 @@
       <c r="C90" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>38</v>
+      <c r="D90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>38</v>
@@ -7543,8 +7552,8 @@
       <c r="L90" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M90" s="2" t="s">
-        <v>38</v>
+      <c r="M90" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>37</v>
@@ -7552,14 +7561,14 @@
       <c r="O90" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R90" s="2" t="s">
-        <v>38</v>
+      <c r="P90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="S90" s="1" t="s">
         <v>37</v>
@@ -7567,11 +7576,11 @@
       <c r="T90" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U90" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V90" s="2" t="s">
-        <v>38</v>
+      <c r="U90" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V90" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W90" s="2" t="s">
         <v>38</v>
@@ -7593,8 +7602,8 @@
       <c r="C91" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>38</v>
+      <c r="D91" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>38</v>
@@ -7608,17 +7617,17 @@
       <c r="H91" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I91" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L91" s="2" t="s">
-        <v>38</v>
+      <c r="I91" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>38</v>
@@ -7629,17 +7638,17 @@
       <c r="O91" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P91" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q91" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R91" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S91" s="1" t="s">
-        <v>37</v>
+      <c r="P91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R91" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T91" s="2" t="s">
         <v>38</v>
@@ -7670,8 +7679,8 @@
       <c r="C92" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>38</v>
+      <c r="D92" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>38</v>
@@ -7685,14 +7694,14 @@
       <c r="H92" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I92" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>38</v>
+      <c r="I92" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>38</v>
@@ -7706,17 +7715,17 @@
       <c r="O92" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P92" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q92" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R92" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S92" s="1" t="s">
-        <v>37</v>
+      <c r="P92" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q92" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R92" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S92" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T92" s="2" t="s">
         <v>38</v>
@@ -7777,8 +7786,8 @@
       <c r="M93" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N93" s="2" t="s">
-        <v>38</v>
+      <c r="N93" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>38</v>
@@ -7842,8 +7851,8 @@
       <c r="I94" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J94" s="2" t="s">
-        <v>38</v>
+      <c r="J94" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>38</v>
@@ -8304,8 +8313,8 @@
       <c r="I100" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J100" s="1" t="s">
-        <v>37</v>
+      <c r="J100" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>38</v>
@@ -8458,8 +8467,8 @@
       <c r="I102" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J102" s="2" t="s">
-        <v>38</v>
+      <c r="J102" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>38</v>
@@ -8517,20 +8526,20 @@
       <c r="C103" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>37</v>
+      <c r="D103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>37</v>
@@ -8538,41 +8547,41 @@
       <c r="J103" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N103" s="1" t="s">
-        <v>37</v>
+      <c r="K103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N103" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R103" s="1" t="s">
-        <v>37</v>
+      <c r="P103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R103" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="S103" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V103" s="1" t="s">
-        <v>37</v>
+      <c r="T103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U103" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V103" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W103" s="2" t="s">
         <v>38</v>
@@ -8594,14 +8603,14 @@
       <c r="C104" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>37</v>
+      <c r="D104" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>38</v>
@@ -8609,11 +8618,11 @@
       <c r="H104" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I104" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>38</v>
+      <c r="I104" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>38</v>
@@ -8642,14 +8651,14 @@
       <c r="S104" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T104" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U104" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V104" s="1" t="s">
-        <v>37</v>
+      <c r="T104" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U104" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V104" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W104" s="2" t="s">
         <v>38</v>
@@ -8686,8 +8695,8 @@
       <c r="H105" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>38</v>
+      <c r="I105" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>38</v>
@@ -8716,8 +8725,8 @@
       <c r="R105" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S105" s="2" t="s">
-        <v>38</v>
+      <c r="S105" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T105" s="2" t="s">
         <v>38</v>
@@ -8754,56 +8763,56 @@
       <c r="E106" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>38</v>
+      <c r="F106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="O106" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U106" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V106" s="2" t="s">
-        <v>38</v>
+      <c r="P106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V106" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W106" s="2" t="s">
         <v>38</v>
@@ -8828,11 +8837,11 @@
       <c r="D107" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>38</v>
+      <c r="E107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>38</v>
@@ -8870,17 +8879,17 @@
       <c r="R107" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S107" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T107" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U107" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V107" s="2" t="s">
-        <v>38</v>
+      <c r="S107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V107" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W107" s="2" t="s">
         <v>38</v>
@@ -8902,29 +8911,29 @@
       <c r="C108" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>37</v>
+      <c r="D108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I108" s="1" t="s">
-        <v>37</v>
+      <c r="I108" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J108" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K108" s="1" t="s">
-        <v>37</v>
+      <c r="K108" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>38</v>
@@ -8938,26 +8947,26 @@
       <c r="O108" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U108" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V108" s="1" t="s">
-        <v>37</v>
+      <c r="P108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U108" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V108" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W108" s="2" t="s">
         <v>38</v>
@@ -8994,14 +9003,14 @@
       <c r="H109" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I109" s="1" t="s">
-        <v>37</v>
+      <c r="I109" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K109" s="1" t="s">
-        <v>37</v>
+      <c r="K109" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>38</v>
@@ -9024,17 +9033,17 @@
       <c r="R109" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S109" s="1" t="s">
-        <v>37</v>
+      <c r="S109" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="T109" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U109" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V109" s="1" t="s">
-        <v>37</v>
+      <c r="U109" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V109" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W109" s="2" t="s">
         <v>38</v>
@@ -9059,26 +9068,26 @@
       <c r="D110" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>37</v>
+      <c r="E110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G110" s="1" t="s">
-        <v>37</v>
+      <c r="G110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H110" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I110" s="1" t="s">
-        <v>37</v>
+      <c r="I110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K110" s="1" t="s">
-        <v>37</v>
+      <c r="K110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L110" s="2" t="s">
         <v>38</v>
@@ -9092,26 +9101,26 @@
       <c r="O110" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V110" s="1" t="s">
-        <v>37</v>
+      <c r="P110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W110" s="2" t="s">
         <v>38</v>
@@ -9130,8 +9139,8 @@
       <c r="B111" t="s">
         <v>146</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>38</v>
+      <c r="C111" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>37</v>
@@ -9145,23 +9154,23 @@
       <c r="G111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H111" s="1" t="s">
-        <v>37</v>
+      <c r="H111" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J111" s="1" t="s">
-        <v>37</v>
+      <c r="J111" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L111" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M111" s="1" t="s">
-        <v>37</v>
+      <c r="L111" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M111" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>38</v>
@@ -9169,17 +9178,17 @@
       <c r="O111" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S111" s="2" t="s">
-        <v>38</v>
+      <c r="P111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S111" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T111" s="1" t="s">
         <v>37</v>
@@ -9207,14 +9216,14 @@
       <c r="B112" t="s">
         <v>147</v>
       </c>
-      <c r="C112" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>38</v>
+      <c r="C112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>38</v>
@@ -9225,14 +9234,14 @@
       <c r="H112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I112" s="2" t="s">
-        <v>38</v>
+      <c r="I112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K112" s="2" t="s">
-        <v>38</v>
+      <c r="K112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>38</v>
@@ -9255,17 +9264,17 @@
       <c r="R112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S112" s="2" t="s">
-        <v>38</v>
+      <c r="S112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U112" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V112" s="2" t="s">
-        <v>38</v>
+      <c r="U112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W112" s="2" t="s">
         <v>38</v>
@@ -9284,8 +9293,8 @@
       <c r="B113" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>38</v>
+      <c r="C113" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>37</v>
@@ -9293,29 +9302,29 @@
       <c r="E113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>37</v>
+      <c r="F113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H113" s="1" t="s">
-        <v>37</v>
+      <c r="H113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J113" s="1" t="s">
-        <v>37</v>
+      <c r="J113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M113" s="1" t="s">
-        <v>37</v>
+      <c r="L113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>38</v>
@@ -9323,17 +9332,17 @@
       <c r="O113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S113" s="2" t="s">
-        <v>38</v>
+      <c r="P113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S113" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T113" s="1" t="s">
         <v>37</v>
@@ -9364,35 +9373,35 @@
       <c r="C114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M114" s="2" t="s">
-        <v>38</v>
+      <c r="D114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N114" s="2" t="s">
         <v>38</v>
@@ -9412,14 +9421,14 @@
       <c r="S114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V114" s="2" t="s">
-        <v>38</v>
+      <c r="T114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V114" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W114" s="2" t="s">
         <v>38</v>
@@ -9438,17 +9447,17 @@
       <c r="B115" t="s">
         <v>150</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>37</v>
+      <c r="C115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>38</v>
@@ -9456,20 +9465,20 @@
       <c r="H115" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>37</v>
+      <c r="I115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>38</v>
@@ -9492,8 +9501,8 @@
       <c r="T115" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U115" s="1" t="s">
-        <v>37</v>
+      <c r="U115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V115" s="2" t="s">
         <v>38</v>
@@ -9515,38 +9524,38 @@
       <c r="B116" t="s">
         <v>151</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>37</v>
+      <c r="C116" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M116" s="2" t="s">
-        <v>38</v>
+      <c r="E116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>38</v>
@@ -9566,14 +9575,14 @@
       <c r="S116" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V116" s="2" t="s">
-        <v>38</v>
+      <c r="T116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W116" s="2" t="s">
         <v>38</v>
@@ -9592,11 +9601,11 @@
       <c r="B117" t="s">
         <v>152</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>37</v>
+      <c r="C117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>38</v>
@@ -9672,14 +9681,14 @@
       <c r="C118" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>38</v>
+      <c r="D118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>38</v>
@@ -9687,20 +9696,20 @@
       <c r="H118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M118" s="2" t="s">
-        <v>38</v>
+      <c r="I118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N118" s="2" t="s">
         <v>38</v>
@@ -9723,8 +9732,8 @@
       <c r="T118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U118" s="2" t="s">
-        <v>38</v>
+      <c r="U118" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V118" s="2" t="s">
         <v>38</v>
@@ -9752,11 +9761,11 @@
       <c r="D119" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>37</v>
+      <c r="E119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>38</v>
@@ -9764,20 +9773,20 @@
       <c r="H119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M119" s="1" t="s">
-        <v>37</v>
+      <c r="I119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>38</v>
@@ -9800,8 +9809,8 @@
       <c r="T119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U119" s="1" t="s">
-        <v>37</v>
+      <c r="U119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V119" s="2" t="s">
         <v>38</v>
@@ -9829,8 +9838,8 @@
       <c r="D120" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>37</v>
+      <c r="E120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>38</v>
@@ -9841,14 +9850,14 @@
       <c r="H120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I120" s="1" t="s">
-        <v>37</v>
+      <c r="I120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K120" s="1" t="s">
-        <v>37</v>
+      <c r="K120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>38</v>
@@ -9877,8 +9886,8 @@
       <c r="T120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U120" s="1" t="s">
-        <v>37</v>
+      <c r="U120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V120" s="2" t="s">
         <v>38</v>
@@ -9903,8 +9912,8 @@
       <c r="C121" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>37</v>
+      <c r="D121" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>38</v>
@@ -9980,14 +9989,14 @@
       <c r="C122" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>38</v>
+      <c r="D122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>38</v>
@@ -9995,20 +10004,20 @@
       <c r="H122" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L122" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M122" s="2" t="s">
-        <v>38</v>
+      <c r="I122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N122" s="2" t="s">
         <v>38</v>
@@ -10031,8 +10040,8 @@
       <c r="T122" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U122" s="2" t="s">
-        <v>38</v>
+      <c r="U122" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V122" s="2" t="s">
         <v>38</v>
@@ -10044,6 +10053,237 @@
         <v>38</v>
       </c>
       <c r="Y122" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="3">
+        <v>158</v>
+      </c>
+      <c r="B123" t="s">
+        <v>158</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U123" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y123" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="3">
+        <v>159</v>
+      </c>
+      <c r="B124" t="s">
+        <v>159</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y124" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="B125" t="s">
+        <v>160</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X125" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y125" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10062,12 +10302,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quarantine order for contacts (#9) Fix I18N test
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3177" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="166">
   <si>
     <t>User Right</t>
   </si>
@@ -450,6 +450,9 @@
     <t>POPULATION_MANAGE</t>
   </si>
   <si>
+    <t>DOCUMENT_TEMPLATE_MANAGEMENT</t>
+  </si>
+  <si>
     <t>LINE_LISTING_CONFIGURE</t>
   </si>
   <si>
@@ -507,7 +510,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.49.0-SNAPSHOT</t>
+    <t>1.50.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z127"/>
+  <dimension ref="A1:Z128"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -9071,11 +9074,11 @@
       <c r="C110" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>37</v>
+      <c r="D110" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>38</v>
@@ -9151,8 +9154,8 @@
       <c r="D111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>38</v>
+      <c r="E111" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>38</v>
@@ -9228,26 +9231,26 @@
       <c r="D112" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>37</v>
+      <c r="E112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I112" s="1" t="s">
-        <v>37</v>
+      <c r="I112" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K112" s="1" t="s">
-        <v>37</v>
+      <c r="K112" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>38</v>
@@ -9261,26 +9264,26 @@
       <c r="O112" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U112" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V112" s="1" t="s">
-        <v>37</v>
+      <c r="P112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U112" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V112" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W112" s="2" t="s">
         <v>38</v>
@@ -9308,11 +9311,11 @@
       <c r="E113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>38</v>
+      <c r="F113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>38</v>
@@ -9338,20 +9341,20 @@
       <c r="O113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q113" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R113" s="2" t="s">
-        <v>38</v>
+      <c r="P113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="S113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T113" s="2" t="s">
-        <v>38</v>
+      <c r="T113" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="U113" s="1" t="s">
         <v>37</v>
@@ -9388,8 +9391,8 @@
       <c r="F114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G114" s="1" t="s">
-        <v>37</v>
+      <c r="G114" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>38</v>
@@ -9415,20 +9418,20 @@
       <c r="O114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P114" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q114" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R114" s="1" t="s">
-        <v>37</v>
+      <c r="P114" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q114" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R114" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T114" s="1" t="s">
-        <v>37</v>
+      <c r="T114" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="U114" s="1" t="s">
         <v>37</v>
@@ -9453,8 +9456,8 @@
       <c r="B115" t="s">
         <v>150</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>38</v>
+      <c r="C115" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>37</v>
@@ -9462,29 +9465,29 @@
       <c r="E115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>37</v>
+      <c r="F115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H115" s="1" t="s">
-        <v>37</v>
+      <c r="H115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J115" s="1" t="s">
-        <v>37</v>
+      <c r="J115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>37</v>
+      <c r="L115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>38</v>
@@ -9492,17 +9495,17 @@
       <c r="O115" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P115" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q115" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R115" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S115" s="2" t="s">
-        <v>38</v>
+      <c r="P115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T115" s="1" t="s">
         <v>37</v>
@@ -9533,35 +9536,35 @@
       <c r="C116" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M116" s="2" t="s">
-        <v>38</v>
+      <c r="D116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>38</v>
@@ -9581,14 +9584,14 @@
       <c r="S116" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V116" s="2" t="s">
-        <v>38</v>
+      <c r="T116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W116" s="2" t="s">
         <v>38</v>
@@ -9610,35 +9613,35 @@
       <c r="C117" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M117" s="1" t="s">
-        <v>37</v>
+      <c r="D117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>38</v>
@@ -9658,14 +9661,14 @@
       <c r="S117" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U117" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V117" s="1" t="s">
-        <v>37</v>
+      <c r="T117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V117" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W117" s="2" t="s">
         <v>38</v>
@@ -9687,35 +9690,35 @@
       <c r="C118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M118" s="2" t="s">
-        <v>38</v>
+      <c r="D118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N118" s="2" t="s">
         <v>38</v>
@@ -9735,14 +9738,14 @@
       <c r="S118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U118" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V118" s="2" t="s">
-        <v>38</v>
+      <c r="T118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U118" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V118" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W118" s="2" t="s">
         <v>38</v>
@@ -9761,17 +9764,17 @@
       <c r="B119" t="s">
         <v>154</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>37</v>
+      <c r="C119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>38</v>
@@ -9779,20 +9782,20 @@
       <c r="H119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M119" s="1" t="s">
-        <v>37</v>
+      <c r="I119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>38</v>
@@ -9815,8 +9818,8 @@
       <c r="T119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U119" s="1" t="s">
-        <v>37</v>
+      <c r="U119" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V119" s="2" t="s">
         <v>38</v>
@@ -9844,11 +9847,11 @@
       <c r="D120" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>38</v>
+      <c r="E120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>38</v>
@@ -9856,20 +9859,20 @@
       <c r="H120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I120" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L120" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M120" s="2" t="s">
-        <v>38</v>
+      <c r="I120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>38</v>
@@ -9892,8 +9895,8 @@
       <c r="T120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U120" s="2" t="s">
-        <v>38</v>
+      <c r="U120" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V120" s="2" t="s">
         <v>38</v>
@@ -9995,8 +9998,8 @@
       <c r="C122" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>38</v>
+      <c r="D122" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>38</v>
@@ -10072,14 +10075,14 @@
       <c r="C123" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>37</v>
+      <c r="D123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>38</v>
@@ -10087,20 +10090,20 @@
       <c r="H123" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L123" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M123" s="1" t="s">
-        <v>37</v>
+      <c r="I123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>38</v>
@@ -10123,8 +10126,8 @@
       <c r="T123" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U123" s="1" t="s">
-        <v>37</v>
+      <c r="U123" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V123" s="2" t="s">
         <v>38</v>
@@ -10155,8 +10158,8 @@
       <c r="E124" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F124" s="2" t="s">
-        <v>38</v>
+      <c r="F124" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>38</v>
@@ -10167,17 +10170,17 @@
       <c r="I124" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J124" s="2" t="s">
-        <v>38</v>
+      <c r="J124" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L124" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M124" s="2" t="s">
-        <v>38</v>
+      <c r="L124" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N124" s="2" t="s">
         <v>38</v>
@@ -10229,8 +10232,8 @@
       <c r="D125" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>38</v>
+      <c r="E125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>38</v>
@@ -10241,14 +10244,14 @@
       <c r="H125" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I125" s="2" t="s">
-        <v>38</v>
+      <c r="I125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K125" s="2" t="s">
-        <v>38</v>
+      <c r="K125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>38</v>
@@ -10277,8 +10280,8 @@
       <c r="T125" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U125" s="2" t="s">
-        <v>38</v>
+      <c r="U125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V125" s="2" t="s">
         <v>38</v>
@@ -10303,8 +10306,8 @@
       <c r="C126" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>38</v>
+      <c r="D126" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>38</v>
@@ -10380,11 +10383,11 @@
       <c r="C127" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>37</v>
+      <c r="D127" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>38</v>
@@ -10395,14 +10398,14 @@
       <c r="H127" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I127" s="1" t="s">
-        <v>37</v>
+      <c r="I127" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J127" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K127" s="1" t="s">
-        <v>37</v>
+      <c r="K127" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>38</v>
@@ -10431,8 +10434,8 @@
       <c r="T127" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U127" s="1" t="s">
-        <v>37</v>
+      <c r="U127" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V127" s="2" t="s">
         <v>38</v>
@@ -10444,6 +10447,83 @@
         <v>38</v>
       </c>
       <c r="Y127" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="3">
+        <v>163</v>
+      </c>
+      <c r="B128" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y128" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10462,12 +10542,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup Strings and Captions (#9)
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3227" uniqueCount="167">
   <si>
     <t>User Right</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>DOCUMENT_TEMPLATE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>QUARANTINE_ORDER_CREATE</t>
   </si>
   <si>
     <t>LINE_LISTING_CONFIGURE</t>
@@ -638,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z128"/>
+  <dimension ref="A1:Z129"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -9151,8 +9154,8 @@
       <c r="C111" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>37</v>
+      <c r="D111" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>37</v>
@@ -9166,17 +9169,17 @@
       <c r="H111" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K111" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L111" s="2" t="s">
-        <v>38</v>
+      <c r="I111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="M111" s="2" t="s">
         <v>38</v>
@@ -9231,8 +9234,8 @@
       <c r="D112" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>38</v>
+      <c r="E112" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>38</v>
@@ -9308,26 +9311,26 @@
       <c r="D113" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>37</v>
+      <c r="E113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I113" s="1" t="s">
-        <v>37</v>
+      <c r="I113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K113" s="1" t="s">
-        <v>37</v>
+      <c r="K113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L113" s="2" t="s">
         <v>38</v>
@@ -9341,26 +9344,26 @@
       <c r="O113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U113" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V113" s="1" t="s">
-        <v>37</v>
+      <c r="P113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U113" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V113" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W113" s="2" t="s">
         <v>38</v>
@@ -9388,11 +9391,11 @@
       <c r="E114" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>38</v>
+      <c r="F114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>38</v>
@@ -9418,20 +9421,20 @@
       <c r="O114" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q114" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R114" s="2" t="s">
-        <v>38</v>
+      <c r="P114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q114" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="S114" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T114" s="2" t="s">
-        <v>38</v>
+      <c r="T114" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="U114" s="1" t="s">
         <v>37</v>
@@ -9468,8 +9471,8 @@
       <c r="F115" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G115" s="1" t="s">
-        <v>37</v>
+      <c r="G115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>38</v>
@@ -9495,20 +9498,20 @@
       <c r="O115" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q115" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R115" s="1" t="s">
-        <v>37</v>
+      <c r="P115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q115" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="S115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T115" s="1" t="s">
-        <v>37</v>
+      <c r="T115" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="U115" s="1" t="s">
         <v>37</v>
@@ -9533,8 +9536,8 @@
       <c r="B116" t="s">
         <v>151</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>38</v>
+      <c r="C116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>37</v>
@@ -9542,29 +9545,29 @@
       <c r="E116" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>37</v>
+      <c r="F116" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H116" s="1" t="s">
-        <v>37</v>
+      <c r="H116" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="I116" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J116" s="1" t="s">
-        <v>37</v>
+      <c r="J116" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="K116" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L116" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M116" s="1" t="s">
-        <v>37</v>
+      <c r="L116" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M116" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>38</v>
@@ -9572,17 +9575,17 @@
       <c r="O116" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R116" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S116" s="2" t="s">
-        <v>38</v>
+      <c r="P116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T116" s="1" t="s">
         <v>37</v>
@@ -9613,35 +9616,35 @@
       <c r="C117" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M117" s="2" t="s">
-        <v>38</v>
+      <c r="D117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>38</v>
@@ -9661,14 +9664,14 @@
       <c r="S117" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U117" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V117" s="2" t="s">
-        <v>38</v>
+      <c r="T117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V117" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W117" s="2" t="s">
         <v>38</v>
@@ -9690,35 +9693,35 @@
       <c r="C118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M118" s="1" t="s">
-        <v>37</v>
+      <c r="D118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M118" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N118" s="2" t="s">
         <v>38</v>
@@ -9738,14 +9741,14 @@
       <c r="S118" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U118" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V118" s="1" t="s">
-        <v>37</v>
+      <c r="T118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U118" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V118" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="W118" s="2" t="s">
         <v>38</v>
@@ -9767,35 +9770,35 @@
       <c r="C119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M119" s="2" t="s">
-        <v>38</v>
+      <c r="D119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>38</v>
@@ -9815,14 +9818,14 @@
       <c r="S119" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U119" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V119" s="2" t="s">
-        <v>38</v>
+      <c r="T119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U119" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V119" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="W119" s="2" t="s">
         <v>38</v>
@@ -9841,17 +9844,17 @@
       <c r="B120" t="s">
         <v>155</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>37</v>
+      <c r="C120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>38</v>
@@ -9859,20 +9862,20 @@
       <c r="H120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L120" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M120" s="1" t="s">
-        <v>37</v>
+      <c r="I120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>38</v>
@@ -9895,8 +9898,8 @@
       <c r="T120" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U120" s="1" t="s">
-        <v>37</v>
+      <c r="U120" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V120" s="2" t="s">
         <v>38</v>
@@ -9924,11 +9927,11 @@
       <c r="D121" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>38</v>
+      <c r="E121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>38</v>
@@ -9936,20 +9939,20 @@
       <c r="H121" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I121" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J121" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L121" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M121" s="2" t="s">
-        <v>38</v>
+      <c r="I121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>38</v>
@@ -9972,8 +9975,8 @@
       <c r="T121" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U121" s="2" t="s">
-        <v>38</v>
+      <c r="U121" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V121" s="2" t="s">
         <v>38</v>
@@ -10075,8 +10078,8 @@
       <c r="C123" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>38</v>
+      <c r="D123" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>38</v>
@@ -10152,14 +10155,14 @@
       <c r="C124" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>37</v>
+      <c r="D124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>38</v>
@@ -10167,20 +10170,20 @@
       <c r="H124" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L124" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M124" s="1" t="s">
-        <v>37</v>
+      <c r="I124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M124" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="N124" s="2" t="s">
         <v>38</v>
@@ -10203,8 +10206,8 @@
       <c r="T124" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U124" s="1" t="s">
-        <v>37</v>
+      <c r="U124" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V124" s="2" t="s">
         <v>38</v>
@@ -10235,8 +10238,8 @@
       <c r="E125" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F125" s="2" t="s">
-        <v>38</v>
+      <c r="F125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>38</v>
@@ -10247,17 +10250,17 @@
       <c r="I125" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J125" s="2" t="s">
-        <v>38</v>
+      <c r="J125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L125" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M125" s="2" t="s">
-        <v>38</v>
+      <c r="L125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>38</v>
@@ -10309,8 +10312,8 @@
       <c r="D126" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>38</v>
+      <c r="E126" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>38</v>
@@ -10321,14 +10324,14 @@
       <c r="H126" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I126" s="2" t="s">
-        <v>38</v>
+      <c r="I126" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J126" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K126" s="2" t="s">
-        <v>38</v>
+      <c r="K126" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>38</v>
@@ -10357,8 +10360,8 @@
       <c r="T126" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U126" s="2" t="s">
-        <v>38</v>
+      <c r="U126" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V126" s="2" t="s">
         <v>38</v>
@@ -10383,8 +10386,8 @@
       <c r="C127" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>38</v>
+      <c r="D127" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>38</v>
@@ -10460,11 +10463,11 @@
       <c r="C128" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>37</v>
+      <c r="D128" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>38</v>
@@ -10475,14 +10478,14 @@
       <c r="H128" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I128" s="1" t="s">
-        <v>37</v>
+      <c r="I128" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J128" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K128" s="1" t="s">
-        <v>37</v>
+      <c r="K128" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>38</v>
@@ -10511,8 +10514,8 @@
       <c r="T128" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U128" s="1" t="s">
-        <v>37</v>
+      <c r="U128" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="V128" s="2" t="s">
         <v>38</v>
@@ -10524,6 +10527,83 @@
         <v>38</v>
       </c>
       <c r="Y128" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="3">
+        <v>164</v>
+      </c>
+      <c r="B129" t="s">
+        <v>164</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y129" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10542,12 +10622,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SORMAS_Data_Dictionary.xlsx and SORMAS_User_Rights.xlsx (#9)
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3382" uniqueCount="169">
   <si>
     <t>User Right</t>
   </si>
@@ -453,6 +453,12 @@
     <t>POPULATION_MANAGE</t>
   </si>
   <si>
+    <t>DOCUMENT_TEMPLATE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>QUARANTINE_ORDER_CREATE</t>
+  </si>
+  <si>
     <t>LINE_LISTING_CONFIGURE</t>
   </si>
   <si>
@@ -513,7 +519,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.50.0-SNAPSHOT</t>
+    <t>1.51.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA128"/>
+  <dimension ref="A1:AA130"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -9405,11 +9411,11 @@
       <c r="C110" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>38</v>
+      <c r="D110" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>39</v>
@@ -9482,14 +9488,14 @@
       <c r="B111" t="s">
         <v>147</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>39</v>
+      <c r="C111" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>39</v>
@@ -9500,17 +9506,17 @@
       <c r="H111" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I111" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K111" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L111" s="2" t="s">
-        <v>39</v>
+      <c r="I111" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="M111" s="2" t="s">
         <v>39</v>
@@ -9571,23 +9577,23 @@
       <c r="E112" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>38</v>
+      <c r="F112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I112" s="1" t="s">
-        <v>38</v>
+      <c r="I112" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K112" s="1" t="s">
-        <v>38</v>
+      <c r="K112" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>39</v>
@@ -9601,26 +9607,26 @@
       <c r="O112" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U112" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V112" s="1" t="s">
-        <v>38</v>
+      <c r="P112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U112" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V112" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W112" s="2" t="s">
         <v>39</v>
@@ -9648,8 +9654,8 @@
       <c r="D113" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>38</v>
+      <c r="E113" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>39</v>
@@ -9660,14 +9666,14 @@
       <c r="H113" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I113" s="1" t="s">
-        <v>38</v>
+      <c r="I113" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K113" s="1" t="s">
-        <v>38</v>
+      <c r="K113" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L113" s="2" t="s">
         <v>39</v>
@@ -9690,17 +9696,17 @@
       <c r="R113" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S113" s="1" t="s">
-        <v>38</v>
+      <c r="S113" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="T113" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U113" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V113" s="1" t="s">
-        <v>38</v>
+      <c r="U113" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V113" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W113" s="2" t="s">
         <v>39</v>
@@ -9731,8 +9737,8 @@
       <c r="E114" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>39</v>
+      <c r="F114" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>38</v>
@@ -9802,8 +9808,8 @@
       <c r="B115" t="s">
         <v>151</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>39</v>
+      <c r="C115" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>38</v>
@@ -9811,29 +9817,29 @@
       <c r="E115" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>38</v>
+      <c r="F115" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J115" s="1" t="s">
-        <v>38</v>
+      <c r="J115" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L115" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>38</v>
+      <c r="L115" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>39</v>
@@ -9850,11 +9856,11 @@
       <c r="R115" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S115" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T115" s="1" t="s">
-        <v>38</v>
+      <c r="S115" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T115" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="U115" s="1" t="s">
         <v>38</v>
@@ -9882,32 +9888,32 @@
       <c r="B116" t="s">
         <v>152</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>39</v>
+      <c r="C116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G116" s="2" t="s">
-        <v>39</v>
+      <c r="G116" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I116" s="2" t="s">
-        <v>39</v>
+      <c r="I116" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K116" s="2" t="s">
-        <v>39</v>
+      <c r="K116" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>39</v>
@@ -9921,26 +9927,26 @@
       <c r="O116" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U116" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V116" s="2" t="s">
-        <v>39</v>
+      <c r="P116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U116" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="W116" s="2" t="s">
         <v>39</v>
@@ -10122,8 +10128,8 @@
       <c r="B119" t="s">
         <v>155</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>38</v>
+      <c r="C119" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>38</v>
@@ -10134,11 +10140,11 @@
       <c r="F119" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G119" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H119" s="2" t="s">
-        <v>39</v>
+      <c r="G119" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>38</v>
@@ -10173,14 +10179,14 @@
       <c r="S119" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T119" s="2" t="s">
-        <v>39</v>
+      <c r="T119" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="U119" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="V119" s="2" t="s">
-        <v>39</v>
+      <c r="V119" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="W119" s="2" t="s">
         <v>39</v>
@@ -10202,11 +10208,11 @@
       <c r="B120" t="s">
         <v>156</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>38</v>
+      <c r="C120" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>39</v>
@@ -10288,11 +10294,11 @@
       <c r="D121" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>39</v>
+      <c r="E121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>39</v>
@@ -10300,20 +10306,20 @@
       <c r="H121" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I121" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J121" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L121" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M121" s="2" t="s">
-        <v>39</v>
+      <c r="I121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>39</v>
@@ -10336,8 +10342,8 @@
       <c r="T121" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U121" s="2" t="s">
-        <v>39</v>
+      <c r="U121" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="V121" s="2" t="s">
         <v>39</v>
@@ -10365,8 +10371,8 @@
       <c r="C122" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>39</v>
+      <c r="D122" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>39</v>
@@ -10448,11 +10454,11 @@
       <c r="D123" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>38</v>
+      <c r="E123" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>39</v>
@@ -10460,20 +10466,20 @@
       <c r="H123" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L123" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M123" s="1" t="s">
-        <v>38</v>
+      <c r="I123" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>39</v>
@@ -10496,8 +10502,8 @@
       <c r="T123" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U123" s="1" t="s">
-        <v>38</v>
+      <c r="U123" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="V123" s="2" t="s">
         <v>39</v>
@@ -10525,11 +10531,11 @@
       <c r="C124" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>38</v>
+      <c r="D124" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>39</v>
@@ -10540,14 +10546,14 @@
       <c r="H124" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I124" s="1" t="s">
-        <v>38</v>
+      <c r="I124" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J124" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K124" s="1" t="s">
-        <v>38</v>
+      <c r="K124" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>39</v>
@@ -10576,8 +10582,8 @@
       <c r="T124" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U124" s="1" t="s">
-        <v>38</v>
+      <c r="U124" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="V124" s="2" t="s">
         <v>39</v>
@@ -10608,11 +10614,11 @@
       <c r="D125" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>39</v>
+      <c r="E125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>39</v>
@@ -10620,20 +10626,20 @@
       <c r="H125" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M125" s="2" t="s">
-        <v>39</v>
+      <c r="I125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>39</v>
@@ -10656,8 +10662,8 @@
       <c r="T125" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U125" s="2" t="s">
-        <v>39</v>
+      <c r="U125" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="V125" s="2" t="s">
         <v>39</v>
@@ -10685,11 +10691,11 @@
       <c r="C126" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>39</v>
+      <c r="D126" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>39</v>
@@ -10700,14 +10706,14 @@
       <c r="H126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I126" s="2" t="s">
-        <v>39</v>
+      <c r="I126" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="J126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K126" s="2" t="s">
-        <v>39</v>
+      <c r="K126" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>39</v>
@@ -10736,8 +10742,8 @@
       <c r="T126" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U126" s="2" t="s">
-        <v>39</v>
+      <c r="U126" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="V126" s="2" t="s">
         <v>39</v>
@@ -10768,8 +10774,8 @@
       <c r="D127" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>38</v>
+      <c r="E127" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>39</v>
@@ -10780,14 +10786,14 @@
       <c r="H127" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I127" s="1" t="s">
-        <v>38</v>
+      <c r="I127" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J127" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K127" s="1" t="s">
-        <v>38</v>
+      <c r="K127" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>39</v>
@@ -10816,8 +10822,8 @@
       <c r="T127" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U127" s="1" t="s">
-        <v>38</v>
+      <c r="U127" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="V127" s="2" t="s">
         <v>39</v>
@@ -10845,11 +10851,11 @@
       <c r="C128" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>38</v>
+      <c r="D128" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>39</v>
@@ -10860,14 +10866,14 @@
       <c r="H128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I128" s="1" t="s">
-        <v>38</v>
+      <c r="I128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K128" s="1" t="s">
-        <v>38</v>
+      <c r="K128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>39</v>
@@ -10875,8 +10881,8 @@
       <c r="M128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N128" s="1" t="s">
-        <v>38</v>
+      <c r="N128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="O128" s="2" t="s">
         <v>39</v>
@@ -10890,17 +10896,17 @@
       <c r="R128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S128" s="1" t="s">
-        <v>38</v>
+      <c r="S128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="T128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U128" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V128" s="1" t="s">
-        <v>38</v>
+      <c r="U128" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V128" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="W128" s="2" t="s">
         <v>39</v>
@@ -10912,6 +10918,166 @@
         <v>39</v>
       </c>
       <c r="Z128" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="3">
+        <v>165</v>
+      </c>
+      <c r="B129" t="s">
+        <v>165</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y129" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z129" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="3">
+        <v>166</v>
+      </c>
+      <c r="B130" t="s">
+        <v>166</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y130" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z130" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -10930,12 +11096,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2137 - Only display cases and contacts from the user's jurisdiction by default
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3512" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="171">
   <si>
     <t>User Right</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>BAG_EXPORT</t>
+  </si>
+  <si>
+    <t>SORMAS_TO_SORMAS_SHARE</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -650,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AB130"/>
+  <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1614,8 +1617,8 @@
       <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>40</v>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>40</v>
@@ -10522,8 +10525,8 @@
       <c r="N119" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O119" s="2" t="s">
-        <v>40</v>
+      <c r="O119" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="P119" s="2" t="s">
         <v>40</v>
@@ -11472,6 +11475,89 @@
         <v>40</v>
       </c>
       <c r="AA130" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="3">
+        <v>168</v>
+      </c>
+      <c r="B131" t="s">
+        <v>168</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA131" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -11490,12 +11576,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2996: Display "External ID" field for switzerland
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -525,7 +525,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.51.0-SNAPSHOT</t>
+    <t>${project.version}</t>
   </si>
 </sst>
 </file>
@@ -6929,8 +6929,8 @@
       <c r="E76" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>39</v>
+      <c r="F76" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>40</v>
@@ -9828,14 +9828,14 @@
       <c r="C111" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>39</v>
+      <c r="D111" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>39</v>
+      <c r="F111" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>40</v>
@@ -9917,8 +9917,8 @@
       <c r="E112" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>39</v>
+      <c r="F112" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>40</v>
@@ -11494,8 +11494,8 @@
       <c r="E131" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F131" s="1" t="s">
-        <v>39</v>
+      <c r="F131" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
#3925 update data dictionary and user rights
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -537,7 +537,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.53.0-SNAPSHOT</t>
+    <t>1.54.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -11008,14 +11008,14 @@
       <c r="X120" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y120" s="2" t="s">
-        <v>41</v>
+      <c r="Y120" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="Z120" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA120" s="2" t="s">
-        <v>41</v>
+      <c r="AA120" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AB120" s="2" t="s">
         <v>41</v>
@@ -11094,14 +11094,14 @@
       <c r="X121" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y121" s="2" t="s">
-        <v>41</v>
+      <c r="Y121" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="Z121" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA121" s="2" t="s">
-        <v>41</v>
+      <c r="AA121" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AB121" s="2" t="s">
         <v>41</v>
@@ -11180,14 +11180,14 @@
       <c r="X122" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y122" s="2" t="s">
-        <v>41</v>
+      <c r="Y122" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="Z122" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA122" s="2" t="s">
-        <v>41</v>
+      <c r="AA122" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AB122" s="2" t="s">
         <v>41</v>
@@ -11266,14 +11266,14 @@
       <c r="X123" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y123" s="2" t="s">
-        <v>41</v>
+      <c r="Y123" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="Z123" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AA123" s="2" t="s">
-        <v>41</v>
+      <c r="AA123" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AB123" s="2" t="s">
         <v>41</v>
@@ -11375,8 +11375,8 @@
       <c r="C125" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>40</v>
+      <c r="D125" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
detect charset for import (#4050)
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4033" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4062" uniqueCount="182">
   <si>
     <t>User Right</t>
   </si>
@@ -330,6 +330,9 @@
     <t>EVENT_EDIT</t>
   </si>
   <si>
+    <t>EVENT_IMPORT</t>
+  </si>
+  <si>
     <t>EVENT_EXPORT</t>
   </si>
   <si>
@@ -555,7 +558,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.57.0-SNAPSHOT</t>
+    <t>1.58.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AD139"/>
+  <dimension ref="A1:AD140"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -6515,14 +6518,14 @@
       <c r="C66" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>41</v>
+      <c r="D66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>42</v>
@@ -6536,14 +6539,14 @@
       <c r="J66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K66" s="1" t="s">
-        <v>41</v>
+      <c r="K66" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M66" s="1" t="s">
-        <v>41</v>
+      <c r="M66" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>42</v>
@@ -6551,8 +6554,8 @@
       <c r="O66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P66" s="1" t="s">
-        <v>41</v>
+      <c r="P66" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q66" s="2" t="s">
         <v>42</v>
@@ -6566,20 +6569,20 @@
       <c r="T66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U66" s="1" t="s">
-        <v>41</v>
+      <c r="U66" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V66" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y66" s="2" t="s">
-        <v>42</v>
+      <c r="W66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y66" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Z66" s="2" t="s">
         <v>42</v>
@@ -6604,14 +6607,14 @@
       <c r="C67" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>42</v>
+      <c r="D67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>42</v>
@@ -6625,14 +6628,14 @@
       <c r="J67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K67" s="2" t="s">
-        <v>42</v>
+      <c r="K67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="2" t="s">
-        <v>42</v>
+      <c r="M67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>42</v>
@@ -6640,8 +6643,8 @@
       <c r="O67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P67" s="2" t="s">
-        <v>42</v>
+      <c r="P67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>42</v>
@@ -6655,17 +6658,17 @@
       <c r="T67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U67" s="2" t="s">
-        <v>42</v>
+      <c r="U67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X67" s="2" t="s">
-        <v>42</v>
+      <c r="W67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X67" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y67" s="2" t="s">
         <v>42</v>
@@ -6693,8 +6696,8 @@
       <c r="C68" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>41</v>
+      <c r="D68" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>42</v>
@@ -6803,14 +6806,14 @@
       <c r="J69" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K69" s="1" t="s">
-        <v>41</v>
+      <c r="K69" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M69" s="1" t="s">
-        <v>41</v>
+      <c r="M69" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>42</v>
@@ -6824,26 +6827,26 @@
       <c r="Q69" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U69" s="1" t="s">
-        <v>41</v>
+      <c r="R69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U69" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V69" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X69" s="1" t="s">
-        <v>41</v>
+      <c r="W69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X69" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y69" s="2" t="s">
         <v>42</v>
@@ -6874,38 +6877,38 @@
       <c r="D70" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>41</v>
+      <c r="E70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I70" s="1" t="s">
-        <v>41</v>
+      <c r="I70" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K70" s="2" t="s">
-        <v>42</v>
+      <c r="K70" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M70" s="2" t="s">
-        <v>42</v>
+      <c r="M70" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O70" s="1" t="s">
-        <v>41</v>
+      <c r="O70" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P70" s="2" t="s">
         <v>42</v>
@@ -6913,26 +6916,26 @@
       <c r="Q70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U70" s="2" t="s">
-        <v>42</v>
+      <c r="R70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U70" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X70" s="2" t="s">
-        <v>42</v>
+      <c r="W70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X70" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y70" s="2" t="s">
         <v>42</v>
@@ -7052,20 +7055,20 @@
       <c r="D72" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>42</v>
+      <c r="E72" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>42</v>
+      <c r="I72" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>42</v>
@@ -7082,8 +7085,8 @@
       <c r="N72" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O72" s="2" t="s">
-        <v>42</v>
+      <c r="O72" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P72" s="2" t="s">
         <v>42</v>
@@ -7141,20 +7144,20 @@
       <c r="D73" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>41</v>
+      <c r="E73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I73" s="1" t="s">
-        <v>41</v>
+      <c r="I73" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>42</v>
@@ -7171,8 +7174,8 @@
       <c r="N73" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O73" s="1" t="s">
-        <v>41</v>
+      <c r="O73" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>42</v>
@@ -7201,8 +7204,8 @@
       <c r="X73" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Y73" s="1" t="s">
-        <v>41</v>
+      <c r="Y73" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Z73" s="2" t="s">
         <v>42</v>
@@ -7224,29 +7227,29 @@
       <c r="B74" t="s">
         <v>113</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>42</v>
+      <c r="C74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>41</v>
+      <c r="H74" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>41</v>
+      <c r="J74" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>42</v>
@@ -7260,8 +7263,8 @@
       <c r="N74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O74" s="2" t="s">
-        <v>42</v>
+      <c r="O74" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P74" s="2" t="s">
         <v>42</v>
@@ -7290,8 +7293,8 @@
       <c r="X74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Y74" s="2" t="s">
-        <v>42</v>
+      <c r="Y74" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Z74" s="2" t="s">
         <v>42</v>
@@ -7313,17 +7316,17 @@
       <c r="B75" t="s">
         <v>114</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>41</v>
+      <c r="C75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>41</v>
@@ -7337,14 +7340,14 @@
       <c r="J75" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>41</v>
+      <c r="K75" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M75" s="1" t="s">
-        <v>41</v>
+      <c r="M75" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>42</v>
@@ -7358,17 +7361,17 @@
       <c r="Q75" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U75" s="1" t="s">
-        <v>41</v>
+      <c r="R75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U75" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V75" s="2" t="s">
         <v>42</v>
@@ -7405,35 +7408,35 @@
       <c r="C76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>42</v>
+      <c r="D76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M76" s="2" t="s">
-        <v>42</v>
+      <c r="M76" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>42</v>
@@ -7447,17 +7450,17 @@
       <c r="Q76" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U76" s="2" t="s">
-        <v>42</v>
+      <c r="R76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U76" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V76" s="2" t="s">
         <v>42</v>
@@ -7672,14 +7675,14 @@
       <c r="C79" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>41</v>
+      <c r="D79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>42</v>
@@ -7714,26 +7717,26 @@
       <c r="Q79" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U79" s="1" t="s">
-        <v>41</v>
+      <c r="R79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U79" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V79" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W79" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X79" s="1" t="s">
-        <v>41</v>
+      <c r="W79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X79" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y79" s="2" t="s">
         <v>42</v>
@@ -7764,11 +7767,11 @@
       <c r="D80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>42</v>
+      <c r="E80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>42</v>
@@ -7803,26 +7806,26 @@
       <c r="Q80" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U80" s="2" t="s">
-        <v>42</v>
+      <c r="R80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U80" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V80" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X80" s="2" t="s">
-        <v>42</v>
+      <c r="W80" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X80" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y80" s="2" t="s">
         <v>42</v>
@@ -7847,17 +7850,17 @@
       <c r="B81" t="s">
         <v>120</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>41</v>
+      <c r="C81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>42</v>
@@ -7936,17 +7939,17 @@
       <c r="B82" t="s">
         <v>121</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>42</v>
+      <c r="C82" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>42</v>
@@ -8031,11 +8034,11 @@
       <c r="D83" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>41</v>
+      <c r="E83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>42</v>
@@ -8049,14 +8052,14 @@
       <c r="J83" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K83" s="1" t="s">
-        <v>41</v>
+      <c r="K83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M83" s="1" t="s">
-        <v>41</v>
+      <c r="M83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N83" s="2" t="s">
         <v>42</v>
@@ -8064,32 +8067,32 @@
       <c r="O83" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P83" s="1" t="s">
-        <v>41</v>
+      <c r="P83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q83" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U83" s="1" t="s">
-        <v>41</v>
+      <c r="R83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V83" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W83" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X83" s="1" t="s">
-        <v>41</v>
+      <c r="W83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X83" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y83" s="2" t="s">
         <v>42</v>
@@ -8159,14 +8162,14 @@
       <c r="Q84" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R84" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S84" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T84" s="2" t="s">
-        <v>42</v>
+      <c r="R84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="U84" s="1" t="s">
         <v>41</v>
@@ -8209,11 +8212,11 @@
       <c r="D85" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>42</v>
+      <c r="E85" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>42</v>
@@ -8227,14 +8230,14 @@
       <c r="J85" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K85" s="2" t="s">
-        <v>42</v>
+      <c r="K85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M85" s="2" t="s">
-        <v>42</v>
+      <c r="M85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>42</v>
@@ -8242,8 +8245,8 @@
       <c r="O85" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P85" s="2" t="s">
-        <v>42</v>
+      <c r="P85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q85" s="2" t="s">
         <v>42</v>
@@ -8257,17 +8260,17 @@
       <c r="T85" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U85" s="2" t="s">
-        <v>42</v>
+      <c r="U85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V85" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W85" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X85" s="2" t="s">
-        <v>42</v>
+      <c r="W85" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X85" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y85" s="2" t="s">
         <v>42</v>
@@ -8295,8 +8298,8 @@
       <c r="C86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>42</v>
+      <c r="D86" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>42</v>
@@ -8384,14 +8387,14 @@
       <c r="C87" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>41</v>
+      <c r="D87" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>41</v>
+      <c r="F87" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>42</v>
@@ -8473,8 +8476,8 @@
       <c r="C88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>42</v>
+      <c r="D88" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>42</v>
@@ -8568,8 +8571,8 @@
       <c r="E89" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>42</v>
+      <c r="F89" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>42</v>
@@ -8740,14 +8743,14 @@
       <c r="C91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>41</v>
+      <c r="D91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>42</v>
@@ -8782,26 +8785,26 @@
       <c r="Q91" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U91" s="1" t="s">
-        <v>41</v>
+      <c r="R91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U91" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V91" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X91" s="1" t="s">
-        <v>41</v>
+      <c r="W91" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X91" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y91" s="2" t="s">
         <v>42</v>
@@ -8832,11 +8835,11 @@
       <c r="D92" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>42</v>
+      <c r="E92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>42</v>
@@ -8874,23 +8877,23 @@
       <c r="R92" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S92" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T92" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U92" s="2" t="s">
-        <v>42</v>
+      <c r="S92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U92" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V92" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W92" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X92" s="2" t="s">
-        <v>42</v>
+      <c r="W92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X92" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y92" s="2" t="s">
         <v>42</v>
@@ -8921,11 +8924,11 @@
       <c r="D93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>41</v>
+      <c r="E93" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>42</v>
@@ -8960,8 +8963,8 @@
       <c r="Q93" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R93" s="2" t="s">
-        <v>42</v>
+      <c r="R93" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>42</v>
@@ -8969,17 +8972,17 @@
       <c r="T93" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U93" s="1" t="s">
-        <v>41</v>
+      <c r="U93" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V93" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X93" s="1" t="s">
-        <v>41</v>
+      <c r="W93" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X93" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y93" s="2" t="s">
         <v>42</v>
@@ -9007,14 +9010,14 @@
       <c r="C94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>42</v>
+      <c r="D94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>42</v>
@@ -9058,17 +9061,17 @@
       <c r="T94" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U94" s="2" t="s">
-        <v>42</v>
+      <c r="U94" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V94" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W94" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X94" s="2" t="s">
-        <v>42</v>
+      <c r="W94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X94" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y94" s="2" t="s">
         <v>42</v>
@@ -9096,8 +9099,8 @@
       <c r="C95" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>41</v>
+      <c r="D95" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>42</v>
@@ -9185,8 +9188,8 @@
       <c r="C96" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>42</v>
+      <c r="D96" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>42</v>
@@ -9274,32 +9277,32 @@
       <c r="C97" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>41</v>
+      <c r="D97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I97" s="1" t="s">
-        <v>41</v>
+      <c r="I97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L97" s="1" t="s">
-        <v>41</v>
+      <c r="K97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>42</v>
@@ -9307,35 +9310,35 @@
       <c r="N97" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P97" s="1" t="s">
-        <v>41</v>
+      <c r="O97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q97" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U97" s="1" t="s">
-        <v>41</v>
+      <c r="R97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V97" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X97" s="1" t="s">
-        <v>41</v>
+      <c r="W97" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X97" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y97" s="2" t="s">
         <v>42</v>
@@ -9366,14 +9369,14 @@
       <c r="D98" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>42</v>
+      <c r="E98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>42</v>
@@ -9384,23 +9387,23 @@
       <c r="J98" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M98" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N98" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P98" s="2" t="s">
-        <v>42</v>
+      <c r="K98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M98" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N98" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q98" s="2" t="s">
         <v>42</v>
@@ -9414,17 +9417,17 @@
       <c r="T98" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U98" s="2" t="s">
-        <v>42</v>
+      <c r="U98" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V98" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X98" s="2" t="s">
-        <v>42</v>
+      <c r="W98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X98" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y98" s="2" t="s">
         <v>42</v>
@@ -9467,8 +9470,8 @@
       <c r="H99" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I99" s="2" t="s">
-        <v>42</v>
+      <c r="I99" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>42</v>
@@ -9482,8 +9485,8 @@
       <c r="M99" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N99" s="2" t="s">
-        <v>42</v>
+      <c r="N99" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>42</v>
@@ -9544,38 +9547,38 @@
       <c r="D100" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>41</v>
+      <c r="E100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>41</v>
+      <c r="I100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="M100" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N100" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O100" s="1" t="s">
-        <v>41</v>
+      <c r="N100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O100" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P100" s="2" t="s">
         <v>42</v>
@@ -9583,14 +9586,14 @@
       <c r="Q100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T100" s="2" t="s">
-        <v>42</v>
+      <c r="R100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T100" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="U100" s="2" t="s">
         <v>42</v>
@@ -9598,8 +9601,8 @@
       <c r="V100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W100" s="1" t="s">
-        <v>41</v>
+      <c r="W100" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="X100" s="2" t="s">
         <v>42</v>
@@ -9630,26 +9633,26 @@
       <c r="C101" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>42</v>
+      <c r="D101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>42</v>
+      <c r="I101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>41</v>
@@ -9657,17 +9660,17 @@
       <c r="L101" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P101" s="1" t="s">
-        <v>41</v>
+      <c r="M101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P101" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q101" s="2" t="s">
         <v>42</v>
@@ -9681,14 +9684,14 @@
       <c r="T101" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U101" s="1" t="s">
-        <v>41</v>
+      <c r="U101" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V101" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W101" s="2" t="s">
-        <v>42</v>
+      <c r="W101" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="X101" s="2" t="s">
         <v>42</v>
@@ -9755,8 +9758,8 @@
       <c r="O102" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P102" s="2" t="s">
-        <v>42</v>
+      <c r="P102" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q102" s="2" t="s">
         <v>42</v>
@@ -10010,8 +10013,8 @@
       <c r="K105" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L105" s="2" t="s">
-        <v>42</v>
+      <c r="L105" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>42</v>
@@ -10099,8 +10102,8 @@
       <c r="K106" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L106" s="1" t="s">
-        <v>41</v>
+      <c r="L106" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="M106" s="2" t="s">
         <v>42</v>
@@ -10277,8 +10280,8 @@
       <c r="K108" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L108" s="2" t="s">
-        <v>42</v>
+      <c r="L108" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>42</v>
@@ -10366,8 +10369,8 @@
       <c r="K109" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L109" s="1" t="s">
-        <v>41</v>
+      <c r="L109" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="M109" s="2" t="s">
         <v>42</v>
@@ -10722,8 +10725,8 @@
       <c r="K113" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L113" s="2" t="s">
-        <v>42</v>
+      <c r="L113" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="M113" s="2" t="s">
         <v>42</v>
@@ -10787,68 +10790,68 @@
       <c r="C114" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J114" s="1" t="s">
-        <v>41</v>
+      <c r="D114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P114" s="1" t="s">
-        <v>41</v>
+      <c r="L114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P114" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q114" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T114" s="1" t="s">
-        <v>41</v>
+      <c r="R114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T114" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="U114" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W114" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X114" s="1" t="s">
-        <v>41</v>
+      <c r="V114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X114" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y114" s="2" t="s">
         <v>42</v>
@@ -10888,44 +10891,44 @@
       <c r="G115" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H115" s="2" t="s">
-        <v>42</v>
+      <c r="H115" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P115" s="2" t="s">
-        <v>42</v>
+      <c r="J115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P115" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q115" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T115" s="2" t="s">
-        <v>42</v>
+      <c r="R115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T115" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="U115" s="1" t="s">
         <v>41</v>
@@ -10965,23 +10968,23 @@
       <c r="C116" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>42</v>
+      <c r="D116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I116" s="2" t="s">
-        <v>42</v>
+      <c r="I116" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>42</v>
@@ -11016,17 +11019,17 @@
       <c r="T116" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X116" s="2" t="s">
-        <v>42</v>
+      <c r="U116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W116" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X116" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y116" s="2" t="s">
         <v>42</v>
@@ -11140,17 +11143,17 @@
       <c r="B118" t="s">
         <v>157</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>41</v>
+      <c r="C118" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>42</v>
@@ -11158,23 +11161,23 @@
       <c r="H118" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I118" s="1" t="s">
-        <v>41</v>
+      <c r="I118" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J118" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K118" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L118" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M118" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N118" s="1" t="s">
-        <v>41</v>
+      <c r="K118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N118" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>42</v>
@@ -11229,8 +11232,8 @@
       <c r="B119" t="s">
         <v>158</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>41</v>
+      <c r="C119" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>41</v>
@@ -11247,23 +11250,23 @@
       <c r="H119" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I119" s="2" t="s">
-        <v>42</v>
+      <c r="I119" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N119" s="2" t="s">
-        <v>42</v>
+      <c r="K119" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="O119" s="2" t="s">
         <v>42</v>
@@ -11324,11 +11327,11 @@
       <c r="D120" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>42</v>
+      <c r="E120" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>42</v>
@@ -11413,32 +11416,32 @@
       <c r="D121" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>41</v>
+      <c r="E121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J121" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K121" s="1" t="s">
-        <v>41</v>
+      <c r="K121" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M121" s="1" t="s">
-        <v>41</v>
+      <c r="M121" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>42</v>
@@ -11452,26 +11455,26 @@
       <c r="Q121" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W121" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X121" s="1" t="s">
-        <v>41</v>
+      <c r="R121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X121" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y121" s="2" t="s">
         <v>42</v>
@@ -11508,14 +11511,14 @@
       <c r="F122" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I122" s="2" t="s">
-        <v>42</v>
+      <c r="G122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J122" s="2" t="s">
         <v>42</v>
@@ -11541,20 +11544,20 @@
       <c r="Q122" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T122" s="2" t="s">
-        <v>42</v>
+      <c r="R122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="U122" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V122" s="2" t="s">
-        <v>42</v>
+      <c r="V122" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="W122" s="1" t="s">
         <v>41</v>
@@ -11600,8 +11603,8 @@
       <c r="G123" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H123" s="1" t="s">
-        <v>41</v>
+      <c r="H123" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="I123" s="2" t="s">
         <v>42</v>
@@ -11630,20 +11633,20 @@
       <c r="Q123" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R123" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S123" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T123" s="1" t="s">
-        <v>41</v>
+      <c r="R123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T123" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="U123" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V123" s="1" t="s">
-        <v>41</v>
+      <c r="V123" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="W123" s="1" t="s">
         <v>41</v>
@@ -11674,8 +11677,8 @@
       <c r="B124" t="s">
         <v>163</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>42</v>
+      <c r="C124" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>41</v>
@@ -11686,32 +11689,32 @@
       <c r="F124" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G124" s="1" t="s">
-        <v>41</v>
+      <c r="G124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I124" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J124" s="1" t="s">
-        <v>41</v>
+      <c r="I124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L124" s="1" t="s">
-        <v>41</v>
+      <c r="L124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="M124" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N124" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O124" s="1" t="s">
-        <v>41</v>
+      <c r="N124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P124" s="2" t="s">
         <v>42</v>
@@ -11719,17 +11722,17 @@
       <c r="Q124" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R124" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S124" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T124" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U124" s="2" t="s">
-        <v>42</v>
+      <c r="R124" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T124" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U124" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V124" s="1" t="s">
         <v>41</v>
@@ -11743,14 +11746,14 @@
       <c r="Y124" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Z124" s="1" t="s">
-        <v>41</v>
+      <c r="Z124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="AA124" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AB124" s="1" t="s">
-        <v>41</v>
+      <c r="AB124" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="AC124" s="2" t="s">
         <v>42</v>
@@ -11766,41 +11769,41 @@
       <c r="C125" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O125" s="2" t="s">
-        <v>42</v>
+      <c r="D125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O125" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P125" s="2" t="s">
         <v>42</v>
@@ -11820,14 +11823,14 @@
       <c r="U125" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X125" s="2" t="s">
-        <v>42</v>
+      <c r="V125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X125" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y125" s="2" t="s">
         <v>42</v>
@@ -11855,44 +11858,44 @@
       <c r="C126" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P126" s="1" t="s">
-        <v>41</v>
+      <c r="D126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P126" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Q126" s="2" t="s">
         <v>42</v>
@@ -11909,14 +11912,14 @@
       <c r="U126" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W126" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X126" s="1" t="s">
-        <v>41</v>
+      <c r="V126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X126" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y126" s="2" t="s">
         <v>42</v>
@@ -11944,44 +11947,44 @@
       <c r="C127" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P127" s="2" t="s">
-        <v>42</v>
+      <c r="D127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Q127" s="2" t="s">
         <v>42</v>
@@ -11998,14 +12001,14 @@
       <c r="U127" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="V127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W127" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X127" s="2" t="s">
-        <v>42</v>
+      <c r="V127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X127" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y127" s="2" t="s">
         <v>42</v>
@@ -12030,44 +12033,44 @@
       <c r="B128" t="s">
         <v>167</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>41</v>
+      <c r="C128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I128" s="1" t="s">
-        <v>41</v>
+      <c r="I128" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J128" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N128" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O128" s="1" t="s">
-        <v>41</v>
+      <c r="K128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O128" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P128" s="2" t="s">
         <v>42</v>
@@ -12090,8 +12093,8 @@
       <c r="V128" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W128" s="1" t="s">
-        <v>41</v>
+      <c r="W128" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="X128" s="2" t="s">
         <v>42</v>
@@ -12099,14 +12102,14 @@
       <c r="Y128" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Z128" s="2" t="s">
-        <v>42</v>
+      <c r="Z128" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="AA128" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AB128" s="2" t="s">
-        <v>42</v>
+      <c r="AB128" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="AC128" s="2" t="s">
         <v>42</v>
@@ -12122,41 +12125,41 @@
       <c r="C129" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G129" s="2" t="s">
-        <v>42</v>
+      <c r="D129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H129" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I129" s="2" t="s">
-        <v>42</v>
+      <c r="I129" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J129" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N129" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O129" s="2" t="s">
-        <v>42</v>
+      <c r="K129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P129" s="2" t="s">
         <v>42</v>
@@ -12179,8 +12182,8 @@
       <c r="V129" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W129" s="2" t="s">
-        <v>42</v>
+      <c r="W129" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="X129" s="2" t="s">
         <v>42</v>
@@ -12211,8 +12214,8 @@
       <c r="C130" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>41</v>
+      <c r="D130" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>42</v>
@@ -12300,8 +12303,8 @@
       <c r="C131" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>42</v>
+      <c r="D131" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>42</v>
@@ -12389,41 +12392,41 @@
       <c r="C132" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>41</v>
+      <c r="D132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I132" s="1" t="s">
-        <v>41</v>
+      <c r="I132" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J132" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N132" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O132" s="1" t="s">
-        <v>41</v>
+      <c r="K132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O132" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P132" s="2" t="s">
         <v>42</v>
@@ -12446,8 +12449,8 @@
       <c r="V132" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W132" s="1" t="s">
-        <v>41</v>
+      <c r="W132" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="X132" s="2" t="s">
         <v>42</v>
@@ -12487,14 +12490,14 @@
       <c r="F133" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>42</v>
+      <c r="G133" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I133" s="2" t="s">
-        <v>42</v>
+      <c r="I133" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J133" s="2" t="s">
         <v>42</v>
@@ -12502,17 +12505,17 @@
       <c r="K133" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L133" s="2" t="s">
-        <v>42</v>
+      <c r="L133" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="M133" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N133" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O133" s="2" t="s">
-        <v>42</v>
+      <c r="N133" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P133" s="2" t="s">
         <v>42</v>
@@ -12570,11 +12573,11 @@
       <c r="D134" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E134" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>42</v>
+      <c r="E134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>42</v>
@@ -12588,14 +12591,14 @@
       <c r="J134" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K134" s="2" t="s">
-        <v>42</v>
+      <c r="K134" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L134" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M134" s="2" t="s">
-        <v>42</v>
+      <c r="M134" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N134" s="2" t="s">
         <v>42</v>
@@ -12624,8 +12627,8 @@
       <c r="V134" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W134" s="2" t="s">
-        <v>42</v>
+      <c r="W134" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="X134" s="2" t="s">
         <v>42</v>
@@ -12656,8 +12659,8 @@
       <c r="C135" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>42</v>
+      <c r="D135" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>42</v>
@@ -12745,14 +12748,14 @@
       <c r="C136" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>41</v>
+      <c r="D136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>42</v>
@@ -12766,14 +12769,14 @@
       <c r="J136" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K136" s="1" t="s">
-        <v>41</v>
+      <c r="K136" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="L136" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M136" s="1" t="s">
-        <v>41</v>
+      <c r="M136" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N136" s="2" t="s">
         <v>42</v>
@@ -12802,8 +12805,8 @@
       <c r="V136" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W136" s="1" t="s">
-        <v>41</v>
+      <c r="W136" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="X136" s="2" t="s">
         <v>42</v>
@@ -12831,17 +12834,17 @@
       <c r="B137" t="s">
         <v>176</v>
       </c>
-      <c r="C137" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>42</v>
+      <c r="C137" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>42</v>
@@ -12855,14 +12858,14 @@
       <c r="J137" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K137" s="2" t="s">
-        <v>42</v>
+      <c r="K137" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M137" s="2" t="s">
-        <v>42</v>
+      <c r="M137" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="N137" s="2" t="s">
         <v>42</v>
@@ -12891,8 +12894,8 @@
       <c r="V137" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W137" s="2" t="s">
-        <v>42</v>
+      <c r="W137" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="X137" s="2" t="s">
         <v>42</v>
@@ -12909,8 +12912,8 @@
       <c r="AB137" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AC137" s="1" t="s">
-        <v>41</v>
+      <c r="AC137" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="138">
@@ -12920,44 +12923,44 @@
       <c r="B138" t="s">
         <v>177</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>41</v>
+      <c r="C138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I138" s="1" t="s">
-        <v>41</v>
+      <c r="I138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O138" s="1" t="s">
-        <v>41</v>
+      <c r="K138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="P138" s="2" t="s">
         <v>42</v>
@@ -12965,26 +12968,26 @@
       <c r="Q138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U138" s="1" t="s">
-        <v>41</v>
+      <c r="R138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="V138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W138" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X138" s="1" t="s">
-        <v>41</v>
+      <c r="W138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X138" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="Y138" s="2" t="s">
         <v>42</v>
@@ -12998,8 +13001,8 @@
       <c r="AB138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AC138" s="2" t="s">
-        <v>42</v>
+      <c r="AC138" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="139">
@@ -13009,8 +13012,8 @@
       <c r="B139" t="s">
         <v>178</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>42</v>
+      <c r="C139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>41</v>
@@ -13018,35 +13021,35 @@
       <c r="E139" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>42</v>
+      <c r="F139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I139" s="2" t="s">
-        <v>42</v>
+      <c r="I139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J139" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O139" s="2" t="s">
-        <v>42</v>
+      <c r="K139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="P139" s="2" t="s">
         <v>42</v>
@@ -13054,26 +13057,26 @@
       <c r="Q139" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U139" s="2" t="s">
-        <v>42</v>
+      <c r="R139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="V139" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W139" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X139" s="2" t="s">
-        <v>42</v>
+      <c r="W139" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X139" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="Y139" s="2" t="s">
         <v>42</v>
@@ -13088,6 +13091,95 @@
         <v>42</v>
       </c>
       <c r="AC139" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="3">
+        <v>179</v>
+      </c>
+      <c r="B140" t="s">
+        <v>179</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC140" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -13106,12 +13198,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#7246 - merge development
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4497" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4526" uniqueCount="352">
   <si>
     <t>User Right</t>
   </si>
@@ -1057,6 +1057,12 @@
   </si>
   <si>
     <t>Archive travel entries</t>
+  </si>
+  <si>
+    <t>EXPORT_DATA_PROTECTION_DATA</t>
+  </si>
+  <si>
+    <t>Export data protection data</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -1190,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AD155"/>
+  <dimension ref="A1:AD156"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -15022,6 +15028,95 @@
         <v>43</v>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" t="s" s="3">
+        <v>348</v>
+      </c>
+      <c r="B156" t="s">
+        <v>349</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB156" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC156" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -15037,12 +15132,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#7249 - Archived entities should always be read-only - changes after review
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4526" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="353">
   <si>
     <t>User Right</t>
   </si>
@@ -1054,6 +1054,18 @@
   </si>
   <si>
     <t>Edit outbreaks</t>
+  </si>
+  <si>
+    <t>SORMAS_REST</t>
+  </si>
+  <si>
+    <t>SORMAS_UI</t>
+  </si>
+  <si>
+    <t>SORMAS_TO_SORMAS_CLIENT</t>
+  </si>
+  <si>
+    <t>EXTERNAL_VISITS</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -1187,7 +1199,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AC156"/>
+  <dimension ref="A1:AC160"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -15108,6 +15120,362 @@
         <v>43</v>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" t="s" s="3">
+        <v>347</v>
+      </c>
+      <c r="B157" t="s">
+        <v>347</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y157" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC157" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="3">
+        <v>348</v>
+      </c>
+      <c r="B158" t="s">
+        <v>348</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X158" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC158" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="3">
+        <v>349</v>
+      </c>
+      <c r="B159" t="s">
+        <v>349</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA159" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC159" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="3">
+        <v>350</v>
+      </c>
+      <c r="B160" t="s">
+        <v>350</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC160" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -15123,12 +15491,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2804 reverted user rights that were added to user
removed java 11 dependency from pom
replaced FILTERED_GRID_BULK_ACTION UserRIght with PERFORM_BULK_OPERATIONS_PSEUDONYM
Used jurisdictions instead of user rights and roles in a lot of places
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -735,6 +735,9 @@
     <t>Perform bulk operations on case samples</t>
   </si>
   <si>
+    <t>PERFORM_BULK_OPERATIONS_PSEUDONYM</t>
+  </si>
+  <si>
     <t>INFRASTRUCTURE_CREATE</t>
   </si>
   <si>
@@ -1096,9 +1099,6 @@
   </si>
   <si>
     <t>DEV_MODE</t>
-  </si>
-  <si>
-    <t>FILTERED_GRID_BULK_ACTION</t>
   </si>
   <si>
     <t>SORMAS Version</t>
@@ -10263,7 +10263,7 @@
         <v>240</v>
       </c>
       <c r="B102" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>42</v>
@@ -10349,10 +10349,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="3">
+        <v>241</v>
+      </c>
+      <c r="B103" t="s">
         <v>242</v>
-      </c>
-      <c r="B103" t="s">
-        <v>243</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>42</v>
@@ -10438,22 +10438,22 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="3">
+        <v>243</v>
+      </c>
+      <c r="B104" t="s">
         <v>244</v>
       </c>
-      <c r="B104" t="s">
-        <v>245</v>
-      </c>
       <c r="C104" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>42</v>
+      <c r="D104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>43</v>
@@ -10488,26 +10488,26 @@
       <c r="Q104" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U104" s="1" t="s">
-        <v>42</v>
+      <c r="R104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U104" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="V104" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W104" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X104" s="1" t="s">
-        <v>42</v>
+      <c r="W104" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X104" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y104" s="2" t="s">
         <v>43</v>
@@ -10527,11 +10527,11 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="3">
+        <v>245</v>
+      </c>
+      <c r="B105" t="s">
         <v>246</v>
       </c>
-      <c r="B105" t="s">
-        <v>247</v>
-      </c>
       <c r="C105" s="1" t="s">
         <v>42</v>
       </c>
@@ -10577,14 +10577,14 @@
       <c r="Q105" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R105" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S105" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T105" s="2" t="s">
-        <v>43</v>
+      <c r="R105" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S105" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T105" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>42</v>
@@ -10616,22 +10616,22 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="3">
+        <v>247</v>
+      </c>
+      <c r="B106" t="s">
         <v>248</v>
       </c>
-      <c r="B106" t="s">
-        <v>249</v>
-      </c>
       <c r="C106" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>43</v>
+      <c r="D106" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>43</v>
@@ -10675,17 +10675,17 @@
       <c r="T106" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U106" s="2" t="s">
-        <v>43</v>
+      <c r="U106" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V106" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W106" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X106" s="2" t="s">
-        <v>43</v>
+      <c r="W106" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X106" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y106" s="2" t="s">
         <v>43</v>
@@ -10705,16 +10705,16 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="3">
+        <v>249</v>
+      </c>
+      <c r="B107" t="s">
         <v>250</v>
       </c>
-      <c r="B107" t="s">
-        <v>251</v>
-      </c>
       <c r="C107" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>42</v>
+      <c r="D107" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>43</v>
@@ -10794,40 +10794,40 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="3">
+        <v>251</v>
+      </c>
+      <c r="B108" t="s">
         <v>252</v>
       </c>
-      <c r="B108" t="s">
-        <v>253</v>
-      </c>
       <c r="C108" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>42</v>
+      <c r="E108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I108" s="1" t="s">
-        <v>42</v>
+      <c r="I108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J108" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L108" s="1" t="s">
-        <v>42</v>
+      <c r="K108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>43</v>
@@ -10835,35 +10835,35 @@
       <c r="N108" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P108" s="1" t="s">
-        <v>42</v>
+      <c r="O108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q108" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U108" s="1" t="s">
-        <v>42</v>
+      <c r="R108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="V108" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X108" s="1" t="s">
-        <v>42</v>
+      <c r="W108" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X108" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y108" s="2" t="s">
         <v>43</v>
@@ -10883,25 +10883,25 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="3">
+        <v>253</v>
+      </c>
+      <c r="B109" t="s">
         <v>254</v>
       </c>
-      <c r="B109" t="s">
-        <v>255</v>
-      </c>
       <c r="C109" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>43</v>
+      <c r="E109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H109" s="2" t="s">
         <v>43</v>
@@ -10912,23 +10912,23 @@
       <c r="J109" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M109" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N109" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P109" s="2" t="s">
-        <v>43</v>
+      <c r="K109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M109" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N109" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P109" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q109" s="2" t="s">
         <v>43</v>
@@ -10942,17 +10942,17 @@
       <c r="T109" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U109" s="2" t="s">
-        <v>43</v>
+      <c r="U109" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V109" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X109" s="2" t="s">
-        <v>43</v>
+      <c r="W109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X109" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y109" s="2" t="s">
         <v>43</v>
@@ -10972,11 +10972,11 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="3">
+        <v>255</v>
+      </c>
+      <c r="B110" t="s">
         <v>256</v>
       </c>
-      <c r="B110" t="s">
-        <v>257</v>
-      </c>
       <c r="C110" s="1" t="s">
         <v>42</v>
       </c>
@@ -10995,8 +10995,8 @@
       <c r="H110" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I110" s="2" t="s">
-        <v>43</v>
+      <c r="I110" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>43</v>
@@ -11010,8 +11010,8 @@
       <c r="M110" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N110" s="2" t="s">
-        <v>43</v>
+      <c r="N110" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="O110" s="2" t="s">
         <v>43</v>
@@ -11061,49 +11061,49 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="3">
+        <v>257</v>
+      </c>
+      <c r="B111" t="s">
         <v>258</v>
       </c>
-      <c r="B111" t="s">
-        <v>259</v>
-      </c>
       <c r="C111" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>42</v>
+      <c r="E111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H111" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L111" s="1" t="s">
-        <v>42</v>
+      <c r="I111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M111" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O111" s="1" t="s">
-        <v>42</v>
+      <c r="N111" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="P111" s="2" t="s">
         <v>43</v>
@@ -11111,14 +11111,14 @@
       <c r="Q111" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R111" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S111" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T111" s="2" t="s">
-        <v>43</v>
+      <c r="R111" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S111" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T111" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="U111" s="2" t="s">
         <v>43</v>
@@ -11126,8 +11126,8 @@
       <c r="V111" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W111" s="1" t="s">
-        <v>42</v>
+      <c r="W111" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="X111" s="2" t="s">
         <v>43</v>
@@ -11150,34 +11150,34 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="3">
+        <v>259</v>
+      </c>
+      <c r="B112" t="s">
         <v>260</v>
       </c>
-      <c r="B112" t="s">
-        <v>261</v>
-      </c>
       <c r="C112" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>43</v>
+      <c r="D112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>43</v>
+      <c r="I112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>42</v>
@@ -11185,17 +11185,17 @@
       <c r="L112" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O112" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P112" s="1" t="s">
-        <v>42</v>
+      <c r="M112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P112" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q112" s="2" t="s">
         <v>43</v>
@@ -11209,14 +11209,14 @@
       <c r="T112" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U112" s="1" t="s">
-        <v>42</v>
+      <c r="U112" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="V112" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W112" s="2" t="s">
-        <v>43</v>
+      <c r="W112" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="X112" s="2" t="s">
         <v>43</v>
@@ -11239,11 +11239,11 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="3">
+        <v>261</v>
+      </c>
+      <c r="B113" t="s">
         <v>262</v>
       </c>
-      <c r="B113" t="s">
-        <v>263</v>
-      </c>
       <c r="C113" s="1" t="s">
         <v>42</v>
       </c>
@@ -11283,8 +11283,8 @@
       <c r="O113" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P113" s="2" t="s">
-        <v>43</v>
+      <c r="P113" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q113" s="2" t="s">
         <v>43</v>
@@ -11328,10 +11328,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="3">
+        <v>263</v>
+      </c>
+      <c r="B114" t="s">
         <v>264</v>
-      </c>
-      <c r="B114" t="s">
-        <v>265</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>42</v>
@@ -11417,10 +11417,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="3">
+        <v>265</v>
+      </c>
+      <c r="B115" t="s">
         <v>266</v>
-      </c>
-      <c r="B115" t="s">
-        <v>267</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>42</v>
@@ -11506,11 +11506,11 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="3">
+        <v>267</v>
+      </c>
+      <c r="B116" t="s">
         <v>268</v>
       </c>
-      <c r="B116" t="s">
-        <v>269</v>
-      </c>
       <c r="C116" s="1" t="s">
         <v>42</v>
       </c>
@@ -11538,8 +11538,8 @@
       <c r="K116" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L116" s="2" t="s">
-        <v>43</v>
+      <c r="L116" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="M116" s="2" t="s">
         <v>43</v>
@@ -11595,11 +11595,11 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="3">
+        <v>269</v>
+      </c>
+      <c r="B117" t="s">
         <v>270</v>
       </c>
-      <c r="B117" t="s">
-        <v>271</v>
-      </c>
       <c r="C117" s="1" t="s">
         <v>42</v>
       </c>
@@ -11627,8 +11627,8 @@
       <c r="K117" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L117" s="1" t="s">
-        <v>42</v>
+      <c r="L117" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M117" s="2" t="s">
         <v>43</v>
@@ -11684,10 +11684,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="3">
+        <v>271</v>
+      </c>
+      <c r="B118" t="s">
         <v>272</v>
-      </c>
-      <c r="B118" t="s">
-        <v>273</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>42</v>
@@ -11773,11 +11773,11 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="3">
+        <v>273</v>
+      </c>
+      <c r="B119" t="s">
         <v>274</v>
       </c>
-      <c r="B119" t="s">
-        <v>275</v>
-      </c>
       <c r="C119" s="1" t="s">
         <v>42</v>
       </c>
@@ -11805,8 +11805,8 @@
       <c r="K119" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L119" s="2" t="s">
-        <v>43</v>
+      <c r="L119" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="M119" s="2" t="s">
         <v>43</v>
@@ -11862,11 +11862,11 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="3">
+        <v>275</v>
+      </c>
+      <c r="B120" t="s">
         <v>276</v>
       </c>
-      <c r="B120" t="s">
-        <v>277</v>
-      </c>
       <c r="C120" s="1" t="s">
         <v>42</v>
       </c>
@@ -11894,8 +11894,8 @@
       <c r="K120" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L120" s="1" t="s">
-        <v>42</v>
+      <c r="L120" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M120" s="2" t="s">
         <v>43</v>
@@ -11951,10 +11951,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="3">
+        <v>277</v>
+      </c>
+      <c r="B121" t="s">
         <v>278</v>
-      </c>
-      <c r="B121" t="s">
-        <v>279</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>42</v>
@@ -12040,10 +12040,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="3">
+        <v>279</v>
+      </c>
+      <c r="B122" t="s">
         <v>280</v>
-      </c>
-      <c r="B122" t="s">
-        <v>281</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>42</v>
@@ -12129,10 +12129,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="3">
+        <v>281</v>
+      </c>
+      <c r="B123" t="s">
         <v>282</v>
-      </c>
-      <c r="B123" t="s">
-        <v>283</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>42</v>
@@ -12218,11 +12218,11 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="3">
+        <v>283</v>
+      </c>
+      <c r="B124" t="s">
         <v>284</v>
       </c>
-      <c r="B124" t="s">
-        <v>285</v>
-      </c>
       <c r="C124" s="1" t="s">
         <v>42</v>
       </c>
@@ -12250,8 +12250,8 @@
       <c r="K124" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L124" s="2" t="s">
-        <v>43</v>
+      <c r="L124" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="M124" s="2" t="s">
         <v>43</v>
@@ -12307,76 +12307,76 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="3">
+        <v>285</v>
+      </c>
+      <c r="B125" t="s">
         <v>286</v>
       </c>
-      <c r="B125" t="s">
-        <v>287</v>
-      </c>
       <c r="C125" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J125" s="1" t="s">
-        <v>42</v>
+      <c r="D125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P125" s="1" t="s">
-        <v>42</v>
+      <c r="L125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P125" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q125" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T125" s="1" t="s">
-        <v>42</v>
+      <c r="R125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T125" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="U125" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W125" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X125" s="1" t="s">
-        <v>42</v>
+      <c r="V125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W125" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X125" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y125" s="2" t="s">
         <v>43</v>
@@ -12396,11 +12396,11 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="3">
+        <v>287</v>
+      </c>
+      <c r="B126" t="s">
         <v>288</v>
       </c>
-      <c r="B126" t="s">
-        <v>289</v>
-      </c>
       <c r="C126" s="1" t="s">
         <v>42</v>
       </c>
@@ -12416,44 +12416,44 @@
       <c r="G126" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H126" s="2" t="s">
-        <v>43</v>
+      <c r="H126" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P126" s="2" t="s">
-        <v>43</v>
+      <c r="J126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q126" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S126" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T126" s="2" t="s">
-        <v>43</v>
+      <c r="R126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S126" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T126" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="U126" s="1" t="s">
         <v>42</v>
@@ -12485,31 +12485,31 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="3">
+        <v>289</v>
+      </c>
+      <c r="B127" t="s">
         <v>290</v>
       </c>
-      <c r="B127" t="s">
-        <v>291</v>
-      </c>
       <c r="C127" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>43</v>
+      <c r="D127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I127" s="2" t="s">
-        <v>43</v>
+      <c r="I127" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J127" s="2" t="s">
         <v>43</v>
@@ -12544,17 +12544,17 @@
       <c r="T127" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W127" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X127" s="2" t="s">
-        <v>43</v>
+      <c r="U127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X127" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y127" s="2" t="s">
         <v>43</v>
@@ -12574,10 +12574,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="3">
+        <v>291</v>
+      </c>
+      <c r="B128" t="s">
         <v>292</v>
-      </c>
-      <c r="B128" t="s">
-        <v>293</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>42</v>
@@ -12663,22 +12663,22 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="3">
+        <v>293</v>
+      </c>
+      <c r="B129" t="s">
         <v>294</v>
       </c>
-      <c r="B129" t="s">
-        <v>295</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>42</v>
+      <c r="C129" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>43</v>
@@ -12686,23 +12686,23 @@
       <c r="H129" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I129" s="1" t="s">
-        <v>42</v>
+      <c r="I129" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J129" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K129" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L129" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M129" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N129" s="1" t="s">
-        <v>42</v>
+      <c r="K129" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M129" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="O129" s="2" t="s">
         <v>43</v>
@@ -12752,13 +12752,13 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="3">
+        <v>295</v>
+      </c>
+      <c r="B130" t="s">
         <v>296</v>
       </c>
-      <c r="B130" t="s">
-        <v>297</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>42</v>
+      <c r="C130" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>42</v>
@@ -12775,23 +12775,23 @@
       <c r="H130" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I130" s="2" t="s">
-        <v>43</v>
+      <c r="I130" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J130" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K130" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L130" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M130" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N130" s="2" t="s">
-        <v>43</v>
+      <c r="K130" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>43</v>
@@ -12841,11 +12841,11 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="3">
+        <v>297</v>
+      </c>
+      <c r="B131" t="s">
         <v>298</v>
       </c>
-      <c r="B131" t="s">
-        <v>299</v>
-      </c>
       <c r="C131" s="1" t="s">
         <v>42</v>
       </c>
@@ -12858,26 +12858,26 @@
       <c r="F131" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>42</v>
+      <c r="G131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J131" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K131" s="1" t="s">
-        <v>42</v>
+      <c r="K131" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M131" s="1" t="s">
-        <v>42</v>
+      <c r="M131" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N131" s="2" t="s">
         <v>43</v>
@@ -12891,26 +12891,26 @@
       <c r="Q131" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W131" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X131" s="1" t="s">
-        <v>42</v>
+      <c r="R131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X131" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y131" s="2" t="s">
         <v>43</v>
@@ -12930,11 +12930,11 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="3">
+        <v>299</v>
+      </c>
+      <c r="B132" t="s">
         <v>300</v>
       </c>
-      <c r="B132" t="s">
-        <v>301</v>
-      </c>
       <c r="C132" s="1" t="s">
         <v>42</v>
       </c>
@@ -12947,14 +12947,14 @@
       <c r="F132" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G132" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I132" s="2" t="s">
-        <v>43</v>
+      <c r="G132" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J132" s="2" t="s">
         <v>43</v>
@@ -12980,20 +12980,20 @@
       <c r="Q132" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R132" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S132" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T132" s="2" t="s">
-        <v>43</v>
+      <c r="R132" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S132" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T132" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="U132" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V132" s="2" t="s">
-        <v>43</v>
+      <c r="V132" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="W132" s="1" t="s">
         <v>42</v>
@@ -13019,11 +13019,11 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="3">
+        <v>301</v>
+      </c>
+      <c r="B133" t="s">
         <v>302</v>
       </c>
-      <c r="B133" t="s">
-        <v>303</v>
-      </c>
       <c r="C133" s="1" t="s">
         <v>42</v>
       </c>
@@ -13039,8 +13039,8 @@
       <c r="G133" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H133" s="1" t="s">
-        <v>42</v>
+      <c r="H133" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="I133" s="2" t="s">
         <v>43</v>
@@ -13069,20 +13069,20 @@
       <c r="Q133" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R133" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S133" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T133" s="1" t="s">
-        <v>42</v>
+      <c r="R133" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S133" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T133" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="U133" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V133" s="1" t="s">
-        <v>42</v>
+      <c r="V133" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="W133" s="1" t="s">
         <v>42</v>
@@ -13108,13 +13108,13 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="3">
+        <v>303</v>
+      </c>
+      <c r="B134" t="s">
         <v>304</v>
       </c>
-      <c r="B134" t="s">
-        <v>305</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>43</v>
+      <c r="C134" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>42</v>
@@ -13125,50 +13125,50 @@
       <c r="F134" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G134" s="1" t="s">
-        <v>42</v>
+      <c r="G134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I134" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J134" s="1" t="s">
-        <v>42</v>
+      <c r="I134" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L134" s="1" t="s">
-        <v>42</v>
+      <c r="L134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M134" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N134" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O134" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P134" s="1" t="s">
-        <v>42</v>
+      <c r="N134" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O134" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q134" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R134" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S134" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T134" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U134" s="2" t="s">
-        <v>43</v>
+      <c r="R134" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V134" s="1" t="s">
         <v>42</v>
@@ -13182,14 +13182,14 @@
       <c r="Y134" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z134" s="1" t="s">
-        <v>42</v>
+      <c r="Z134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="AA134" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AB134" s="1" t="s">
-        <v>42</v>
+      <c r="AB134" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="AC134" s="2" t="s">
         <v>43</v>
@@ -13197,52 +13197,52 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="3">
+        <v>305</v>
+      </c>
+      <c r="B135" t="s">
         <v>306</v>
       </c>
-      <c r="B135" t="s">
-        <v>307</v>
-      </c>
       <c r="C135" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P135" s="2" t="s">
-        <v>43</v>
+      <c r="D135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q135" s="2" t="s">
         <v>43</v>
@@ -13259,14 +13259,14 @@
       <c r="U135" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W135" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X135" s="2" t="s">
-        <v>43</v>
+      <c r="V135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X135" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y135" s="2" t="s">
         <v>43</v>
@@ -13286,52 +13286,52 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="3">
+        <v>307</v>
+      </c>
+      <c r="B136" t="s">
         <v>308</v>
       </c>
-      <c r="B136" t="s">
-        <v>309</v>
-      </c>
       <c r="C136" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P136" s="1" t="s">
-        <v>42</v>
+      <c r="D136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P136" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q136" s="2" t="s">
         <v>43</v>
@@ -13348,14 +13348,14 @@
       <c r="U136" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X136" s="1" t="s">
-        <v>42</v>
+      <c r="V136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W136" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X136" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y136" s="2" t="s">
         <v>43</v>
@@ -13375,52 +13375,52 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="3">
+        <v>309</v>
+      </c>
+      <c r="B137" t="s">
         <v>310</v>
       </c>
-      <c r="B137" t="s">
-        <v>311</v>
-      </c>
       <c r="C137" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P137" s="2" t="s">
-        <v>43</v>
+      <c r="D137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q137" s="2" t="s">
         <v>43</v>
@@ -13437,14 +13437,14 @@
       <c r="U137" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W137" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X137" s="2" t="s">
-        <v>43</v>
+      <c r="V137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W137" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X137" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y137" s="2" t="s">
         <v>43</v>
@@ -13464,49 +13464,49 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="3">
+        <v>311</v>
+      </c>
+      <c r="B138" t="s">
         <v>312</v>
       </c>
-      <c r="B138" t="s">
-        <v>313</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>42</v>
+      <c r="C138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I138" s="1" t="s">
-        <v>42</v>
+      <c r="I138" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J138" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N138" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O138" s="1" t="s">
-        <v>42</v>
+      <c r="K138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N138" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O138" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="P138" s="2" t="s">
         <v>43</v>
@@ -13529,8 +13529,8 @@
       <c r="V138" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W138" s="1" t="s">
-        <v>42</v>
+      <c r="W138" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="X138" s="2" t="s">
         <v>43</v>
@@ -13538,14 +13538,14 @@
       <c r="Y138" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z138" s="2" t="s">
-        <v>43</v>
+      <c r="Z138" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AA138" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AB138" s="2" t="s">
-        <v>43</v>
+      <c r="AB138" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AC138" s="2" t="s">
         <v>43</v>
@@ -13553,49 +13553,49 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="3">
+        <v>313</v>
+      </c>
+      <c r="B139" t="s">
         <v>314</v>
       </c>
-      <c r="B139" t="s">
-        <v>315</v>
-      </c>
       <c r="C139" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>43</v>
+      <c r="D139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I139" s="2" t="s">
-        <v>43</v>
+      <c r="I139" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J139" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O139" s="2" t="s">
-        <v>43</v>
+      <c r="K139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P139" s="2" t="s">
         <v>43</v>
@@ -13618,8 +13618,8 @@
       <c r="V139" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W139" s="2" t="s">
-        <v>43</v>
+      <c r="W139" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="X139" s="2" t="s">
         <v>43</v>
@@ -13642,16 +13642,16 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="3">
+        <v>315</v>
+      </c>
+      <c r="B140" t="s">
         <v>316</v>
       </c>
-      <c r="B140" t="s">
-        <v>317</v>
-      </c>
       <c r="C140" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>42</v>
+      <c r="D140" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>43</v>
@@ -13731,16 +13731,16 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="3">
+        <v>317</v>
+      </c>
+      <c r="B141" t="s">
         <v>318</v>
       </c>
-      <c r="B141" t="s">
-        <v>319</v>
-      </c>
       <c r="C141" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D141" s="2" t="s">
-        <v>43</v>
+      <c r="D141" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>43</v>
@@ -13820,49 +13820,49 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="3">
+        <v>319</v>
+      </c>
+      <c r="B142" t="s">
         <v>320</v>
       </c>
-      <c r="B142" t="s">
-        <v>321</v>
-      </c>
       <c r="C142" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>42</v>
+      <c r="D142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I142" s="1" t="s">
-        <v>42</v>
+      <c r="I142" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J142" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N142" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O142" s="1" t="s">
-        <v>42</v>
+      <c r="K142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N142" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O142" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="P142" s="2" t="s">
         <v>43</v>
@@ -13885,8 +13885,8 @@
       <c r="V142" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W142" s="1" t="s">
-        <v>42</v>
+      <c r="W142" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="X142" s="2" t="s">
         <v>43</v>
@@ -13909,10 +13909,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="3">
+        <v>321</v>
+      </c>
+      <c r="B143" t="s">
         <v>322</v>
-      </c>
-      <c r="B143" t="s">
-        <v>323</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>42</v>
@@ -13998,49 +13998,49 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="3">
+        <v>323</v>
+      </c>
+      <c r="B144" t="s">
         <v>324</v>
       </c>
-      <c r="B144" t="s">
-        <v>325</v>
-      </c>
       <c r="C144" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>43</v>
+      <c r="E144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H144" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I144" s="2" t="s">
-        <v>43</v>
+      <c r="I144" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J144" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N144" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O144" s="2" t="s">
-        <v>43</v>
+      <c r="K144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P144" s="2" t="s">
         <v>43</v>
@@ -14063,8 +14063,8 @@
       <c r="V144" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W144" s="2" t="s">
-        <v>43</v>
+      <c r="W144" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="X144" s="2" t="s">
         <v>43</v>
@@ -14087,16 +14087,16 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="3">
+        <v>325</v>
+      </c>
+      <c r="B145" t="s">
         <v>326</v>
       </c>
-      <c r="B145" t="s">
-        <v>327</v>
-      </c>
       <c r="C145" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>43</v>
+      <c r="D145" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>43</v>
@@ -14176,22 +14176,22 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="3">
+        <v>327</v>
+      </c>
+      <c r="B146" t="s">
         <v>328</v>
       </c>
-      <c r="B146" t="s">
-        <v>329</v>
-      </c>
       <c r="C146" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>42</v>
+      <c r="D146" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>43</v>
@@ -14205,14 +14205,14 @@
       <c r="J146" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K146" s="1" t="s">
-        <v>42</v>
+      <c r="K146" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M146" s="1" t="s">
-        <v>42</v>
+      <c r="M146" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N146" s="2" t="s">
         <v>43</v>
@@ -14241,8 +14241,8 @@
       <c r="V146" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W146" s="1" t="s">
-        <v>42</v>
+      <c r="W146" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="X146" s="2" t="s">
         <v>43</v>
@@ -14265,22 +14265,22 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="3">
+        <v>329</v>
+      </c>
+      <c r="B147" t="s">
         <v>330</v>
       </c>
-      <c r="B147" t="s">
-        <v>331</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>43</v>
+      <c r="C147" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>43</v>
@@ -14294,14 +14294,14 @@
       <c r="J147" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K147" s="2" t="s">
-        <v>43</v>
+      <c r="K147" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M147" s="2" t="s">
-        <v>43</v>
+      <c r="M147" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="N147" s="2" t="s">
         <v>43</v>
@@ -14330,8 +14330,8 @@
       <c r="V147" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W147" s="2" t="s">
-        <v>43</v>
+      <c r="W147" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="X147" s="2" t="s">
         <v>43</v>
@@ -14348,55 +14348,55 @@
       <c r="AB147" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AC147" s="1" t="s">
-        <v>42</v>
+      <c r="AC147" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s" s="3">
+        <v>331</v>
+      </c>
+      <c r="B148" t="s">
         <v>332</v>
       </c>
-      <c r="B148" t="s">
-        <v>333</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>42</v>
+      <c r="C148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I148" s="1" t="s">
-        <v>42</v>
+      <c r="I148" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J148" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>42</v>
+      <c r="K148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O148" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="P148" s="2" t="s">
         <v>43</v>
@@ -14404,26 +14404,26 @@
       <c r="Q148" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U148" s="1" t="s">
-        <v>42</v>
+      <c r="R148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U148" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="V148" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X148" s="1" t="s">
-        <v>42</v>
+      <c r="W148" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X148" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y148" s="2" t="s">
         <v>43</v>
@@ -14437,19 +14437,19 @@
       <c r="AB148" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AC148" s="2" t="s">
-        <v>43</v>
+      <c r="AC148" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s" s="3">
+        <v>333</v>
+      </c>
+      <c r="B149" t="s">
         <v>334</v>
       </c>
-      <c r="B149" t="s">
-        <v>335</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>43</v>
+      <c r="C149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>42</v>
@@ -14457,35 +14457,35 @@
       <c r="E149" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G149" s="2" t="s">
-        <v>43</v>
+      <c r="F149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H149" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I149" s="2" t="s">
-        <v>43</v>
+      <c r="I149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J149" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O149" s="2" t="s">
-        <v>43</v>
+      <c r="K149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P149" s="2" t="s">
         <v>43</v>
@@ -14493,26 +14493,26 @@
       <c r="Q149" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U149" s="2" t="s">
-        <v>43</v>
+      <c r="R149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V149" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W149" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X149" s="2" t="s">
-        <v>43</v>
+      <c r="W149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X149" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y149" s="2" t="s">
         <v>43</v>
@@ -14532,19 +14532,19 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="3">
+        <v>335</v>
+      </c>
+      <c r="B150" t="s">
         <v>336</v>
       </c>
-      <c r="B150" t="s">
-        <v>337</v>
-      </c>
       <c r="C150" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E150" s="2" t="s">
-        <v>43</v>
+      <c r="E150" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>43</v>
@@ -14621,76 +14621,76 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="3">
+        <v>337</v>
+      </c>
+      <c r="B151" t="s">
         <v>338</v>
       </c>
-      <c r="B151" t="s">
-        <v>339</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>42</v>
+      <c r="C151" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P151" s="1" t="s">
-        <v>42</v>
+      <c r="E151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P151" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Q151" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W151" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X151" s="1" t="s">
-        <v>42</v>
+      <c r="R151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W151" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X151" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y151" s="2" t="s">
         <v>43</v>
@@ -14710,10 +14710,10 @@
     </row>
     <row r="152">
       <c r="A152" t="s" s="3">
+        <v>339</v>
+      </c>
+      <c r="B152" t="s">
         <v>340</v>
-      </c>
-      <c r="B152" t="s">
-        <v>341</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>42</v>
@@ -14799,11 +14799,11 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="3">
+        <v>341</v>
+      </c>
+      <c r="B153" t="s">
         <v>342</v>
       </c>
-      <c r="B153" t="s">
-        <v>343</v>
-      </c>
       <c r="C153" s="1" t="s">
         <v>42</v>
       </c>
@@ -14849,14 +14849,14 @@
       <c r="Q153" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R153" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S153" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T153" s="2" t="s">
-        <v>43</v>
+      <c r="R153" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S153" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T153" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="U153" s="1" t="s">
         <v>42</v>
@@ -14888,10 +14888,10 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="3">
+        <v>343</v>
+      </c>
+      <c r="B154" t="s">
         <v>344</v>
-      </c>
-      <c r="B154" t="s">
-        <v>345</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>42</v>
@@ -14977,52 +14977,52 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="3">
+        <v>345</v>
+      </c>
+      <c r="B155" t="s">
         <v>346</v>
       </c>
-      <c r="B155" t="s">
-        <v>347</v>
-      </c>
       <c r="C155" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E155" s="2" t="s">
-        <v>43</v>
+      <c r="E155" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P155" s="2" t="s">
-        <v>43</v>
+      <c r="G155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q155" s="2" t="s">
         <v>43</v>
@@ -15036,17 +15036,17 @@
       <c r="T155" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W155" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X155" s="2" t="s">
-        <v>43</v>
+      <c r="U155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W155" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X155" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y155" s="2" t="s">
         <v>43</v>
@@ -15066,22 +15066,22 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="3">
+        <v>347</v>
+      </c>
+      <c r="B156" t="s">
         <v>348</v>
       </c>
-      <c r="B156" t="s">
-        <v>349</v>
-      </c>
       <c r="C156" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D156" s="2" t="s">
-        <v>43</v>
+      <c r="D156" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F156" s="2" t="s">
-        <v>43</v>
+      <c r="F156" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>43</v>
@@ -15155,10 +15155,10 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="3">
+        <v>349</v>
+      </c>
+      <c r="B157" t="s">
         <v>350</v>
-      </c>
-      <c r="B157" t="s">
-        <v>351</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>42</v>
@@ -15244,22 +15244,22 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="3">
+        <v>351</v>
+      </c>
+      <c r="B158" t="s">
         <v>352</v>
       </c>
-      <c r="B158" t="s">
-        <v>353</v>
-      </c>
       <c r="C158" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>42</v>
+      <c r="D158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G158" s="2" t="s">
         <v>43</v>
@@ -15294,26 +15294,26 @@
       <c r="Q158" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U158" s="1" t="s">
-        <v>42</v>
+      <c r="R158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U158" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="V158" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W158" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X158" s="1" t="s">
-        <v>42</v>
+      <c r="W158" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X158" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y158" s="2" t="s">
         <v>43</v>
@@ -15333,11 +15333,11 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="3">
+        <v>353</v>
+      </c>
+      <c r="B159" t="s">
         <v>354</v>
       </c>
-      <c r="B159" t="s">
-        <v>355</v>
-      </c>
       <c r="C159" s="1" t="s">
         <v>42</v>
       </c>
@@ -15383,26 +15383,26 @@
       <c r="Q159" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R159" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S159" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T159" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U159" s="2" t="s">
-        <v>43</v>
+      <c r="R159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U159" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V159" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W159" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X159" s="2" t="s">
-        <v>43</v>
+      <c r="W159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X159" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y159" s="2" t="s">
         <v>43</v>
@@ -15422,31 +15422,31 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="3">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B160" t="s">
         <v>356</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H160" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I160" s="1" t="s">
-        <v>42</v>
+      <c r="C160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I160" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J160" s="2" t="s">
         <v>43</v>
@@ -15454,14 +15454,14 @@
       <c r="K160" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L160" s="1" t="s">
-        <v>42</v>
+      <c r="L160" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="M160" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N160" s="1" t="s">
-        <v>42</v>
+      <c r="N160" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="O160" s="2" t="s">
         <v>43</v>
@@ -15484,8 +15484,8 @@
       <c r="U160" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V160" s="1" t="s">
-        <v>42</v>
+      <c r="V160" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="W160" s="2" t="s">
         <v>43</v>
@@ -15496,17 +15496,17 @@
       <c r="Y160" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z160" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA160" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB160" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC160" s="1" t="s">
-        <v>42</v>
+      <c r="Z160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB160" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC160" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="161">
@@ -15516,17 +15516,17 @@
       <c r="B161" t="s">
         <v>357</v>
       </c>
-      <c r="C161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>42</v>
+      <c r="C161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G161" s="1" t="s">
         <v>42</v>
@@ -15537,65 +15537,65 @@
       <c r="I161" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K161" s="1" t="s">
-        <v>42</v>
+      <c r="J161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K161" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M161" s="1" t="s">
-        <v>42</v>
+      <c r="M161" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N161" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V161" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="W161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X161" s="1" t="s">
-        <v>42</v>
+      <c r="O161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V161" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W161" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X161" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="Y161" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z161" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA161" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB161" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC161" s="2" t="s">
-        <v>43</v>
+      <c r="Z161" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA161" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB161" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC161" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="162">
@@ -15605,71 +15605,71 @@
       <c r="B162" t="s">
         <v>358</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U162" s="2" t="s">
-        <v>43</v>
+      <c r="C162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U162" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="V162" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="W162" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X162" s="2" t="s">
-        <v>43</v>
+      <c r="W162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X162" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Y162" s="2" t="s">
         <v>43</v>
@@ -15680,8 +15680,8 @@
       <c r="AA162" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AB162" s="1" t="s">
-        <v>42</v>
+      <c r="AB162" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="AC162" s="2" t="s">
         <v>43</v>
@@ -15763,14 +15763,14 @@
       <c r="Y163" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z163" s="1" t="s">
-        <v>42</v>
+      <c r="Z163" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="AA163" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AB163" s="2" t="s">
-        <v>43</v>
+      <c r="AB163" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AC163" s="2" t="s">
         <v>43</v>
@@ -15783,8 +15783,8 @@
       <c r="B164" t="s">
         <v>360</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>42</v>
+      <c r="C164" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>43</v>
@@ -15852,8 +15852,8 @@
       <c r="Y164" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z164" s="2" t="s">
-        <v>43</v>
+      <c r="Z164" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="AA164" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
#4461: Fixed failing tests
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -1502,11 +1502,11 @@
       <c r="N3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>42</v>
+      <c r="O3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>43</v>
@@ -1591,11 +1591,11 @@
       <c r="N4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>42</v>
+      <c r="O4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>43</v>
@@ -1680,11 +1680,11 @@
       <c r="N5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>42</v>
+      <c r="O5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>43</v>
@@ -1787,11 +1787,11 @@
       <c r="T6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>42</v>
+      <c r="U6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>43</v>
@@ -1840,11 +1840,11 @@
       <c r="H7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>42</v>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
@@ -1876,11 +1876,11 @@
       <c r="T7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>42</v>
+      <c r="U7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>43</v>
@@ -1965,11 +1965,11 @@
       <c r="T8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>42</v>
+      <c r="U8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>43</v>
@@ -2036,11 +2036,11 @@
       <c r="N9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>42</v>
+      <c r="O9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>42</v>
@@ -2054,11 +2054,11 @@
       <c r="T9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>42</v>
+      <c r="U9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>43</v>
@@ -2143,11 +2143,11 @@
       <c r="T10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>42</v>
+      <c r="U10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>42</v>
@@ -2214,11 +2214,11 @@
       <c r="N11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>42</v>
+      <c r="O11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>43</v>
@@ -2232,11 +2232,11 @@
       <c r="T11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>42</v>
+      <c r="U11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>42</v>
@@ -2365,11 +2365,11 @@
       <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>43</v>
+      <c r="F13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>42</v>
@@ -2463,11 +2463,11 @@
       <c r="H14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>42</v>
+      <c r="I14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>43</v>
@@ -2481,11 +2481,11 @@
       <c r="N14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>42</v>
+      <c r="O14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>42</v>
@@ -2493,17 +2493,17 @@
       <c r="R14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>42</v>
+      <c r="S14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W14" s="2" t="s">
         <v>42</v>
@@ -2552,11 +2552,11 @@
       <c r="H15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>42</v>
+      <c r="I15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>43</v>
@@ -2582,17 +2582,17 @@
       <c r="R15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>42</v>
+      <c r="S15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W15" s="2" t="s">
         <v>42</v>
@@ -2926,11 +2926,11 @@
       <c r="N19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>42</v>
+      <c r="O19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>43</v>
@@ -3015,11 +3015,11 @@
       <c r="N20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>42</v>
+      <c r="O20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>43</v>
@@ -3104,11 +3104,11 @@
       <c r="N21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>42</v>
+      <c r="O21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>43</v>
@@ -3371,11 +3371,11 @@
       <c r="N24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>42</v>
+      <c r="O24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>43</v>
@@ -3460,11 +3460,11 @@
       <c r="N25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>42</v>
+      <c r="O25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>43</v>
@@ -3816,11 +3816,11 @@
       <c r="N29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>42</v>
+      <c r="O29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>43</v>
@@ -3828,11 +3828,11 @@
       <c r="R29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>43</v>
+      <c r="S29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>43</v>
@@ -4006,11 +4006,11 @@
       <c r="R31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>43</v>
+      <c r="S31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="U31" s="1" t="s">
         <v>43</v>
@@ -4279,11 +4279,11 @@
       <c r="T34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V34" s="2" t="s">
-        <v>42</v>
+      <c r="U34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W34" s="2" t="s">
         <v>42</v>
@@ -4350,11 +4350,11 @@
       <c r="N35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>42</v>
+      <c r="O35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>42</v>
@@ -4362,17 +4362,17 @@
       <c r="R35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V35" s="2" t="s">
-        <v>42</v>
+      <c r="S35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W35" s="2" t="s">
         <v>42</v>
@@ -4457,11 +4457,11 @@
       <c r="T36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V36" s="2" t="s">
-        <v>42</v>
+      <c r="U36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W36" s="1" t="s">
         <v>43</v>
@@ -4546,11 +4546,11 @@
       <c r="T37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V37" s="2" t="s">
-        <v>42</v>
+      <c r="U37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>43</v>
@@ -4718,17 +4718,17 @@
       <c r="R39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V39" s="2" t="s">
-        <v>42</v>
+      <c r="S39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W39" s="2" t="s">
         <v>42</v>
@@ -4807,17 +4807,17 @@
       <c r="R40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V40" s="2" t="s">
-        <v>42</v>
+      <c r="S40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W40" s="2" t="s">
         <v>42</v>
@@ -4896,17 +4896,17 @@
       <c r="R41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>42</v>
+      <c r="S41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W41" s="2" t="s">
         <v>42</v>
@@ -5074,11 +5074,11 @@
       <c r="R43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T43" s="2" t="s">
-        <v>42</v>
+      <c r="S43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>42</v>
@@ -5124,11 +5124,11 @@
       <c r="E44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>43</v>
+      <c r="F44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>42</v>
@@ -5240,11 +5240,11 @@
       <c r="N45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>42</v>
+      <c r="O45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>43</v>
@@ -5252,17 +5252,17 @@
       <c r="R45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>42</v>
+      <c r="S45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>43</v>
@@ -5430,11 +5430,11 @@
       <c r="R47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>42</v>
+      <c r="S47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>42</v>
@@ -5507,11 +5507,11 @@
       <c r="N48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>42</v>
+      <c r="O48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>42</v>
@@ -5519,11 +5519,11 @@
       <c r="R48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T48" s="2" t="s">
-        <v>42</v>
+      <c r="S48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U48" s="2" t="s">
         <v>42</v>
@@ -5697,11 +5697,11 @@
       <c r="R50" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T50" s="2" t="s">
-        <v>42</v>
+      <c r="S50" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T50" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>42</v>
@@ -5786,11 +5786,11 @@
       <c r="R51" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S51" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T51" s="2" t="s">
-        <v>42</v>
+      <c r="S51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U51" s="2" t="s">
         <v>42</v>
@@ -5863,11 +5863,11 @@
       <c r="N52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>42</v>
+      <c r="O52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>42</v>
@@ -5875,17 +5875,17 @@
       <c r="R52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V52" s="2" t="s">
-        <v>42</v>
+      <c r="S52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W52" s="2" t="s">
         <v>42</v>
@@ -5964,11 +5964,11 @@
       <c r="R53" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S53" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T53" s="2" t="s">
-        <v>42</v>
+      <c r="S53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U53" s="2" t="s">
         <v>42</v>
@@ -6231,11 +6231,11 @@
       <c r="R56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S56" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T56" s="2" t="s">
-        <v>42</v>
+      <c r="S56" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U56" s="2" t="s">
         <v>42</v>
@@ -6320,11 +6320,11 @@
       <c r="R57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S57" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>42</v>
+      <c r="S57" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U57" s="2" t="s">
         <v>42</v>
@@ -6409,11 +6409,11 @@
       <c r="R58" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S58" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T58" s="2" t="s">
-        <v>42</v>
+      <c r="S58" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T58" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U58" s="2" t="s">
         <v>42</v>
@@ -6575,11 +6575,11 @@
       <c r="N60" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O60" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P60" s="2" t="s">
-        <v>42</v>
+      <c r="O60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q60" s="2" t="s">
         <v>42</v>
@@ -6587,17 +6587,17 @@
       <c r="R60" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S60" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T60" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V60" s="2" t="s">
-        <v>42</v>
+      <c r="S60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W60" s="2" t="s">
         <v>42</v>
@@ -6646,11 +6646,11 @@
       <c r="H61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>42</v>
+      <c r="I61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>43</v>
@@ -6664,11 +6664,11 @@
       <c r="N61" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O61" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P61" s="2" t="s">
-        <v>42</v>
+      <c r="O61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q61" s="2" t="s">
         <v>42</v>
@@ -6676,17 +6676,17 @@
       <c r="R61" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S61" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T61" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V61" s="2" t="s">
-        <v>42</v>
+      <c r="S61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>43</v>
@@ -6913,11 +6913,11 @@
       <c r="H64" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>42</v>
+      <c r="I64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>43</v>
@@ -6931,11 +6931,11 @@
       <c r="N64" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P64" s="2" t="s">
-        <v>42</v>
+      <c r="O64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q64" s="2" t="s">
         <v>42</v>
@@ -6943,17 +6943,17 @@
       <c r="R64" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T64" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V64" s="2" t="s">
-        <v>42</v>
+      <c r="S64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V64" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W64" s="1" t="s">
         <v>43</v>
@@ -7554,11 +7554,11 @@
       <c r="N71" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O71" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P71" s="2" t="s">
-        <v>42</v>
+      <c r="O71" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q71" s="1" t="s">
         <v>43</v>
@@ -7655,11 +7655,11 @@
       <c r="R72" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S72" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T72" s="2" t="s">
-        <v>42</v>
+      <c r="S72" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T72" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U72" s="2" t="s">
         <v>42</v>
@@ -7705,11 +7705,11 @@
       <c r="E73" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>43</v>
+      <c r="F73" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>42</v>
@@ -7803,11 +7803,11 @@
       <c r="H74" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>42</v>
+      <c r="I74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>43</v>
@@ -7821,11 +7821,11 @@
       <c r="N74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>42</v>
+      <c r="O74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q74" s="2" t="s">
         <v>42</v>
@@ -7833,17 +7833,17 @@
       <c r="R74" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T74" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V74" s="2" t="s">
-        <v>42</v>
+      <c r="S74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T74" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V74" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W74" s="2" t="s">
         <v>42</v>
@@ -7922,11 +7922,11 @@
       <c r="R75" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S75" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T75" s="2" t="s">
-        <v>42</v>
+      <c r="S75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T75" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U75" s="2" t="s">
         <v>42</v>
@@ -8355,11 +8355,11 @@
       <c r="N80" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O80" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P80" s="2" t="s">
-        <v>42</v>
+      <c r="O80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q80" s="1" t="s">
         <v>43</v>
@@ -8506,11 +8506,11 @@
       <c r="E82" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>43</v>
+      <c r="F82" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>42</v>
@@ -8622,11 +8622,11 @@
       <c r="N83" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P83" s="2" t="s">
-        <v>42</v>
+      <c r="O83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q83" s="1" t="s">
         <v>43</v>
@@ -8723,11 +8723,11 @@
       <c r="R84" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S84" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T84" s="2" t="s">
-        <v>42</v>
+      <c r="S84" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U84" s="2" t="s">
         <v>42</v>
@@ -8901,11 +8901,11 @@
       <c r="R86" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S86" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T86" s="2" t="s">
-        <v>42</v>
+      <c r="S86" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T86" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U86" s="2" t="s">
         <v>42</v>
@@ -9174,11 +9174,11 @@
       <c r="T89" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U89" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V89" s="1" t="s">
-        <v>43</v>
+      <c r="U89" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V89" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>43</v>
@@ -9257,11 +9257,11 @@
       <c r="R90" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S90" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T90" s="2" t="s">
-        <v>42</v>
+      <c r="S90" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T90" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U90" s="1" t="s">
         <v>43</v>
@@ -9672,11 +9672,11 @@
       <c r="H95" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>42</v>
+      <c r="I95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>43</v>
@@ -9690,11 +9690,11 @@
       <c r="N95" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P95" s="2" t="s">
-        <v>42</v>
+      <c r="O95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q95" s="2" t="s">
         <v>42</v>
@@ -9702,17 +9702,17 @@
       <c r="R95" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T95" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V95" s="2" t="s">
-        <v>42</v>
+      <c r="S95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V95" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W95" s="1" t="s">
         <v>43</v>
@@ -9761,11 +9761,11 @@
       <c r="H96" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I96" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>42</v>
+      <c r="I96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>43</v>
@@ -9779,11 +9779,11 @@
       <c r="N96" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O96" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P96" s="2" t="s">
-        <v>42</v>
+      <c r="O96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q96" s="2" t="s">
         <v>42</v>
@@ -9791,17 +9791,17 @@
       <c r="R96" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S96" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T96" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U96" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V96" s="2" t="s">
-        <v>42</v>
+      <c r="S96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U96" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V96" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>43</v>
@@ -10058,11 +10058,11 @@
       <c r="R99" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S99" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T99" s="2" t="s">
-        <v>42</v>
+      <c r="S99" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T99" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U99" s="2" t="s">
         <v>42</v>
@@ -10147,11 +10147,11 @@
       <c r="R100" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S100" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T100" s="2" t="s">
-        <v>42</v>
+      <c r="S100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T100" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U100" s="2" t="s">
         <v>42</v>
@@ -10651,11 +10651,11 @@
       <c r="H106" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I106" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>42</v>
+      <c r="I106" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>43</v>
@@ -10740,11 +10740,11 @@
       <c r="H107" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>42</v>
+      <c r="I107" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>43</v>
@@ -11007,11 +11007,11 @@
       <c r="H110" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I110" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>42</v>
+      <c r="I110" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>43</v>
@@ -11025,11 +11025,11 @@
       <c r="N110" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O110" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P110" s="2" t="s">
-        <v>42</v>
+      <c r="O110" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P110" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q110" s="1" t="s">
         <v>43</v>
@@ -11037,17 +11037,17 @@
       <c r="R110" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S110" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T110" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U110" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V110" s="2" t="s">
-        <v>42</v>
+      <c r="S110" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T110" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U110" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V110" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>43</v>
@@ -11126,11 +11126,11 @@
       <c r="R111" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T111" s="2" t="s">
-        <v>42</v>
+      <c r="S111" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T111" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U111" s="2" t="s">
         <v>42</v>
@@ -11215,11 +11215,11 @@
       <c r="R112" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S112" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T112" s="2" t="s">
-        <v>42</v>
+      <c r="S112" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T112" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="U112" s="2" t="s">
         <v>42</v>
@@ -11274,11 +11274,11 @@
       <c r="H113" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I113" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>42</v>
+      <c r="I113" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>42</v>
@@ -11381,11 +11381,11 @@
       <c r="N114" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O114" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P114" s="2" t="s">
-        <v>42</v>
+      <c r="O114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q114" s="2" t="s">
         <v>42</v>
@@ -11393,17 +11393,17 @@
       <c r="R114" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S114" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T114" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U114" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V114" s="2" t="s">
-        <v>42</v>
+      <c r="S114" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U114" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V114" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W114" s="2" t="s">
         <v>42</v>
@@ -11482,17 +11482,17 @@
       <c r="R115" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S115" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T115" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U115" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V115" s="2" t="s">
-        <v>42</v>
+      <c r="S115" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U115" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V115" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W115" s="2" t="s">
         <v>42</v>
@@ -11571,17 +11571,17 @@
       <c r="R116" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S116" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T116" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U116" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V116" s="2" t="s">
-        <v>42</v>
+      <c r="S116" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T116" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U116" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W116" s="2" t="s">
         <v>42</v>
@@ -11660,17 +11660,17 @@
       <c r="R117" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S117" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T117" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U117" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V117" s="2" t="s">
-        <v>42</v>
+      <c r="S117" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T117" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U117" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V117" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W117" s="2" t="s">
         <v>42</v>
@@ -11755,11 +11755,11 @@
       <c r="T118" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U118" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V118" s="2" t="s">
-        <v>42</v>
+      <c r="U118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V118" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W118" s="2" t="s">
         <v>42</v>
@@ -11838,17 +11838,17 @@
       <c r="R119" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S119" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V119" s="2" t="s">
-        <v>42</v>
+      <c r="S119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T119" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U119" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V119" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W119" s="2" t="s">
         <v>42</v>
@@ -11927,17 +11927,17 @@
       <c r="R120" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S120" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T120" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U120" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V120" s="2" t="s">
-        <v>42</v>
+      <c r="S120" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T120" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U120" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V120" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W120" s="2" t="s">
         <v>42</v>
@@ -12022,11 +12022,11 @@
       <c r="T121" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U121" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V121" s="2" t="s">
-        <v>42</v>
+      <c r="U121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V121" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W121" s="2" t="s">
         <v>42</v>
@@ -12105,17 +12105,17 @@
       <c r="R122" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T122" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U122" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V122" s="2" t="s">
-        <v>42</v>
+      <c r="S122" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T122" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U122" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V122" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W122" s="2" t="s">
         <v>42</v>
@@ -12194,17 +12194,17 @@
       <c r="R123" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S123" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T123" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U123" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V123" s="2" t="s">
-        <v>42</v>
+      <c r="S123" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V123" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W123" s="2" t="s">
         <v>42</v>
@@ -12283,17 +12283,17 @@
       <c r="R124" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S124" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T124" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U124" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V124" s="2" t="s">
-        <v>42</v>
+      <c r="S124" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V124" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W124" s="2" t="s">
         <v>42</v>
@@ -12372,17 +12372,17 @@
       <c r="R125" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S125" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T125" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U125" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V125" s="2" t="s">
-        <v>42</v>
+      <c r="S125" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T125" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U125" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V125" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W125" s="2" t="s">
         <v>42</v>
@@ -12467,11 +12467,11 @@
       <c r="T126" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U126" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V126" s="2" t="s">
-        <v>42</v>
+      <c r="U126" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V126" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W126" s="2" t="s">
         <v>42</v>
@@ -12538,11 +12538,11 @@
       <c r="N127" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O127" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P127" s="2" t="s">
-        <v>42</v>
+      <c r="O127" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q127" s="1" t="s">
         <v>43</v>
@@ -12912,11 +12912,11 @@
       <c r="T131" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U131" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V131" s="2" t="s">
-        <v>42</v>
+      <c r="U131" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W131" s="1" t="s">
         <v>43</v>
@@ -13084,17 +13084,17 @@
       <c r="R133" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S133" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T133" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U133" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V133" s="2" t="s">
-        <v>42</v>
+      <c r="S133" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T133" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U133" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V133" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W133" s="1" t="s">
         <v>43</v>
@@ -13143,11 +13143,11 @@
       <c r="H134" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I134" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>42</v>
+      <c r="I134" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>43</v>
@@ -13173,17 +13173,17 @@
       <c r="R134" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S134" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T134" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U134" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V134" s="2" t="s">
-        <v>42</v>
+      <c r="S134" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U134" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W134" s="2" t="s">
         <v>42</v>
@@ -13262,17 +13262,17 @@
       <c r="R135" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S135" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T135" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U135" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V135" s="2" t="s">
-        <v>42</v>
+      <c r="S135" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U135" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W135" s="2" t="s">
         <v>42</v>
@@ -13312,11 +13312,11 @@
       <c r="E136" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F136" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G136" s="2" t="s">
-        <v>42</v>
+      <c r="F136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>43</v>
@@ -13339,11 +13339,11 @@
       <c r="N136" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O136" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P136" s="2" t="s">
-        <v>42</v>
+      <c r="O136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q136" s="1" t="s">
         <v>43</v>
@@ -13401,11 +13401,11 @@
       <c r="E137" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F137" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>42</v>
+      <c r="F137" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H137" s="2" t="s">
         <v>42</v>
@@ -13490,11 +13490,11 @@
       <c r="E138" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F138" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>42</v>
+      <c r="F138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>43</v>
@@ -13517,11 +13517,11 @@
       <c r="N138" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O138" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P138" s="2" t="s">
-        <v>42</v>
+      <c r="O138" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q138" s="1" t="s">
         <v>43</v>
@@ -13579,11 +13579,11 @@
       <c r="E139" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F139" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>42</v>
+      <c r="F139" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>42</v>
@@ -13677,11 +13677,11 @@
       <c r="H140" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I140" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>42</v>
+      <c r="I140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>42</v>
@@ -13713,11 +13713,11 @@
       <c r="T140" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U140" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V140" s="2" t="s">
-        <v>42</v>
+      <c r="U140" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W140" s="1" t="s">
         <v>43</v>
@@ -14033,11 +14033,11 @@
       <c r="H144" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I144" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J144" s="2" t="s">
-        <v>42</v>
+      <c r="I144" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>42</v>
@@ -14069,11 +14069,11 @@
       <c r="T144" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U144" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V144" s="2" t="s">
-        <v>42</v>
+      <c r="U144" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V144" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W144" s="1" t="s">
         <v>43</v>
@@ -14122,11 +14122,11 @@
       <c r="H145" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I145" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J145" s="2" t="s">
-        <v>42</v>
+      <c r="I145" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>42</v>
@@ -14158,11 +14158,11 @@
       <c r="T145" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U145" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V145" s="2" t="s">
-        <v>42</v>
+      <c r="U145" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V145" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W145" s="1" t="s">
         <v>43</v>
@@ -14389,11 +14389,11 @@
       <c r="H148" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I148" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J148" s="2" t="s">
-        <v>42</v>
+      <c r="I148" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>42</v>
@@ -14419,17 +14419,17 @@
       <c r="R148" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S148" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T148" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U148" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V148" s="2" t="s">
-        <v>42</v>
+      <c r="S148" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T148" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U148" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V148" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W148" s="2" t="s">
         <v>42</v>
@@ -14567,11 +14567,11 @@
       <c r="H150" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I150" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J150" s="2" t="s">
-        <v>42</v>
+      <c r="I150" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>43</v>
@@ -14603,11 +14603,11 @@
       <c r="T150" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U150" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V150" s="2" t="s">
-        <v>42</v>
+      <c r="U150" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V150" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="W150" s="1" t="s">
         <v>43</v>
@@ -14852,11 +14852,11 @@
       <c r="N153" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O153" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P153" s="2" t="s">
-        <v>42</v>
+      <c r="O153" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P153" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q153" s="1" t="s">
         <v>43</v>
@@ -14941,11 +14941,11 @@
       <c r="N154" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O154" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P154" s="2" t="s">
-        <v>42</v>
+      <c r="O154" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P154" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q154" s="1" t="s">
         <v>43</v>
@@ -15030,11 +15030,11 @@
       <c r="N155" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O155" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P155" s="2" t="s">
-        <v>42</v>
+      <c r="O155" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q155" s="1" t="s">
         <v>43</v>
@@ -15119,11 +15119,11 @@
       <c r="N156" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O156" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P156" s="2" t="s">
-        <v>42</v>
+      <c r="O156" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P156" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Q156" s="1" t="s">
         <v>43</v>
@@ -15457,11 +15457,11 @@
       <c r="H160" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I160" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J160" s="2" t="s">
-        <v>42</v>
+      <c r="I160" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>43</v>
@@ -15626,20 +15626,20 @@
       <c r="E162" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F162" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G162" s="2" t="s">
-        <v>42</v>
+      <c r="F162" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H162" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I162" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J162" s="1" t="s">
-        <v>43</v>
+      <c r="I162" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J162" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>42</v>
@@ -15665,11 +15665,11 @@
       <c r="R162" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S162" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T162" s="1" t="s">
-        <v>43</v>
+      <c r="S162" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T162" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="U162" s="2" t="s">
         <v>42</v>
@@ -15724,11 +15724,11 @@
       <c r="H163" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I163" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J163" s="2" t="s">
-        <v>42</v>
+      <c r="I163" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>43</v>
@@ -15893,11 +15893,11 @@
       <c r="E165" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F165" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G165" s="2" t="s">
-        <v>42</v>
+      <c r="F165" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="H165" s="2" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
#4461: fixed some review findings
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -2004,11 +2004,11 @@
       <c r="N3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>45</v>
+      <c r="O3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>45</v>
@@ -2057,11 +2057,11 @@
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>44</v>
@@ -2093,11 +2093,11 @@
       <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>45</v>
+      <c r="O4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>45</v>
@@ -2182,11 +2182,11 @@
       <c r="N5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>45</v>
+      <c r="O5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>45</v>
@@ -2342,11 +2342,11 @@
       <c r="H7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>44</v>
+      <c r="I7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>45</v>
@@ -2538,11 +2538,11 @@
       <c r="N9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>45</v>
+      <c r="O9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>44</v>
@@ -2716,11 +2716,11 @@
       <c r="N11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>45</v>
+      <c r="O11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>45</v>
@@ -2965,11 +2965,11 @@
       <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>44</v>
+      <c r="I14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>45</v>
@@ -2983,11 +2983,11 @@
       <c r="N14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>45</v>
+      <c r="O14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>44</v>
@@ -3054,11 +3054,11 @@
       <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>44</v>
+      <c r="I15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>45</v>
@@ -3428,11 +3428,11 @@
       <c r="N19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>45</v>
+      <c r="O19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>45</v>
@@ -3517,11 +3517,11 @@
       <c r="N20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>45</v>
+      <c r="O20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>45</v>
@@ -3606,11 +3606,11 @@
       <c r="N21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>45</v>
+      <c r="O21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>45</v>
@@ -3873,11 +3873,11 @@
       <c r="N24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>45</v>
+      <c r="O24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>45</v>
@@ -3962,11 +3962,11 @@
       <c r="N25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>45</v>
+      <c r="O25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>45</v>
@@ -4318,11 +4318,11 @@
       <c r="N29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>45</v>
+      <c r="O29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>45</v>
@@ -4852,11 +4852,11 @@
       <c r="N35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>45</v>
+      <c r="O35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>44</v>
@@ -5742,11 +5742,11 @@
       <c r="N45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O45" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>45</v>
+      <c r="O45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>45</v>
@@ -6009,11 +6009,11 @@
       <c r="N48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>45</v>
+      <c r="O48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>44</v>
@@ -6365,11 +6365,11 @@
       <c r="N52" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O52" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>45</v>
+      <c r="O52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>44</v>
@@ -7077,11 +7077,11 @@
       <c r="N60" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O60" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>45</v>
+      <c r="O60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q60" s="2" t="s">
         <v>44</v>
@@ -7148,11 +7148,11 @@
       <c r="H61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>44</v>
+      <c r="I61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>45</v>
@@ -7166,11 +7166,11 @@
       <c r="N61" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O61" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>45</v>
+      <c r="O61" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q61" s="2" t="s">
         <v>44</v>
@@ -7415,11 +7415,11 @@
       <c r="H64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>44</v>
+      <c r="I64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>45</v>
@@ -7433,11 +7433,11 @@
       <c r="N64" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O64" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P64" s="1" t="s">
-        <v>45</v>
+      <c r="O64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P64" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q64" s="2" t="s">
         <v>44</v>
@@ -8056,11 +8056,11 @@
       <c r="N71" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O71" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P71" s="1" t="s">
-        <v>45</v>
+      <c r="O71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P71" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q71" s="1" t="s">
         <v>45</v>
@@ -8305,11 +8305,11 @@
       <c r="H74" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>44</v>
+      <c r="I74" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>45</v>
@@ -8323,11 +8323,11 @@
       <c r="N74" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O74" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P74" s="1" t="s">
-        <v>45</v>
+      <c r="O74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P74" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q74" s="2" t="s">
         <v>44</v>
@@ -8857,11 +8857,11 @@
       <c r="N80" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O80" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P80" s="1" t="s">
-        <v>45</v>
+      <c r="O80" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P80" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q80" s="1" t="s">
         <v>45</v>
@@ -9124,11 +9124,11 @@
       <c r="N83" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O83" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P83" s="1" t="s">
-        <v>45</v>
+      <c r="O83" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P83" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q83" s="1" t="s">
         <v>45</v>
@@ -10174,11 +10174,11 @@
       <c r="H95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I95" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>44</v>
+      <c r="I95" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>45</v>
@@ -10192,11 +10192,11 @@
       <c r="N95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O95" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P95" s="1" t="s">
-        <v>45</v>
+      <c r="O95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P95" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q95" s="2" t="s">
         <v>44</v>
@@ -10263,11 +10263,11 @@
       <c r="H96" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I96" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>44</v>
+      <c r="I96" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>45</v>
@@ -10281,11 +10281,11 @@
       <c r="N96" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O96" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P96" s="1" t="s">
-        <v>45</v>
+      <c r="O96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P96" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q96" s="2" t="s">
         <v>44</v>
@@ -11153,11 +11153,11 @@
       <c r="H106" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I106" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>44</v>
+      <c r="I106" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>45</v>
@@ -11242,11 +11242,11 @@
       <c r="H107" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>44</v>
+      <c r="I107" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>45</v>
@@ -11509,11 +11509,11 @@
       <c r="H110" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I110" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>44</v>
+      <c r="I110" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>45</v>
@@ -11527,11 +11527,11 @@
       <c r="N110" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O110" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P110" s="1" t="s">
-        <v>45</v>
+      <c r="O110" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P110" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q110" s="1" t="s">
         <v>45</v>
@@ -11776,11 +11776,11 @@
       <c r="H113" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I113" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>44</v>
+      <c r="I113" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>44</v>
@@ -11883,11 +11883,11 @@
       <c r="N114" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O114" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P114" s="1" t="s">
-        <v>45</v>
+      <c r="O114" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P114" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q114" s="2" t="s">
         <v>44</v>
@@ -13040,11 +13040,11 @@
       <c r="N127" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O127" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P127" s="1" t="s">
-        <v>45</v>
+      <c r="O127" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P127" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q127" s="1" t="s">
         <v>45</v>
@@ -13645,11 +13645,11 @@
       <c r="H134" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I134" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>44</v>
+      <c r="I134" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>45</v>
@@ -13805,17 +13805,17 @@
       <c r="B136" t="s">
         <v>440</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>45</v>
+      <c r="C136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>44</v>
@@ -13841,11 +13841,11 @@
       <c r="N136" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O136" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P136" s="1" t="s">
-        <v>45</v>
+      <c r="O136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P136" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q136" s="1" t="s">
         <v>45</v>
@@ -13894,17 +13894,17 @@
       <c r="B137" t="s">
         <v>443</v>
       </c>
-      <c r="C137" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>45</v>
+      <c r="C137" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>44</v>
@@ -13983,17 +13983,17 @@
       <c r="B138" t="s">
         <v>446</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>45</v>
+      <c r="C138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>44</v>
@@ -14019,11 +14019,11 @@
       <c r="N138" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O138" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P138" s="1" t="s">
-        <v>45</v>
+      <c r="O138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P138" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q138" s="1" t="s">
         <v>45</v>
@@ -14072,17 +14072,17 @@
       <c r="B139" t="s">
         <v>449</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>45</v>
+      <c r="C139" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>44</v>
@@ -14179,11 +14179,11 @@
       <c r="H140" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I140" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>44</v>
+      <c r="I140" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>44</v>
@@ -14535,11 +14535,11 @@
       <c r="H144" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I144" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J144" s="2" t="s">
-        <v>44</v>
+      <c r="I144" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>44</v>
@@ -14624,11 +14624,11 @@
       <c r="H145" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I145" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J145" s="2" t="s">
-        <v>44</v>
+      <c r="I145" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>44</v>
@@ -14891,11 +14891,11 @@
       <c r="H148" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I148" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J148" s="2" t="s">
-        <v>44</v>
+      <c r="I148" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>44</v>
@@ -14962,11 +14962,11 @@
       <c r="B149" t="s">
         <v>479</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>44</v>
+      <c r="C149" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>44</v>
@@ -15069,11 +15069,11 @@
       <c r="H150" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I150" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J150" s="2" t="s">
-        <v>44</v>
+      <c r="I150" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>45</v>
@@ -15354,11 +15354,11 @@
       <c r="N153" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O153" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P153" s="1" t="s">
-        <v>45</v>
+      <c r="O153" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P153" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q153" s="1" t="s">
         <v>45</v>
@@ -15443,11 +15443,11 @@
       <c r="N154" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O154" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P154" s="1" t="s">
-        <v>45</v>
+      <c r="O154" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P154" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q154" s="1" t="s">
         <v>45</v>
@@ -15532,11 +15532,11 @@
       <c r="N155" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O155" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P155" s="1" t="s">
-        <v>45</v>
+      <c r="O155" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P155" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q155" s="1" t="s">
         <v>45</v>
@@ -15621,11 +15621,11 @@
       <c r="N156" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O156" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P156" s="1" t="s">
-        <v>45</v>
+      <c r="O156" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P156" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="Q156" s="1" t="s">
         <v>45</v>
@@ -15959,11 +15959,11 @@
       <c r="H160" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I160" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J160" s="2" t="s">
-        <v>44</v>
+      <c r="I160" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>45</v>
@@ -16137,11 +16137,11 @@
       <c r="H162" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I162" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J162" s="1" t="s">
-        <v>45</v>
+      <c r="I162" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J162" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>44</v>
@@ -16226,11 +16226,11 @@
       <c r="H163" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I163" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J163" s="2" t="s">
-        <v>44</v>
+      <c r="I163" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>45</v>
@@ -16297,11 +16297,11 @@
       <c r="B164" t="s">
         <v>28</v>
       </c>
-      <c r="C164" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>45</v>
+      <c r="C164" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>44</v>
@@ -16392,11 +16392,11 @@
       <c r="D165" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E165" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>45</v>
+      <c r="E165" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
#4461 implementation of review comments
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4981" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4981" uniqueCount="534">
   <si>
     <t>User Right</t>
   </si>
@@ -24,1567 +24,1570 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>National User</t>
-  </si>
-  <si>
-    <t>Surveillance Supervisor</t>
-  </si>
-  <si>
-    <t>Admin Surveillance Supervisor</t>
-  </si>
-  <si>
-    <t>Surveillance Officer</t>
-  </si>
-  <si>
-    <t>Hospital Informant</t>
-  </si>
-  <si>
-    <t>Community Officer</t>
-  </si>
-  <si>
-    <t>Community Informant</t>
-  </si>
-  <si>
-    <t>Clinician</t>
-  </si>
-  <si>
-    <t>Case Officer</t>
-  </si>
-  <si>
-    <t>Contact Supervisor</t>
-  </si>
-  <si>
-    <t>Contact Officer</t>
-  </si>
-  <si>
-    <t>Event Officer</t>
-  </si>
-  <si>
-    <t>Lab Officer</t>
-  </si>
-  <si>
-    <t>External Lab Officer</t>
-  </si>
-  <si>
-    <t>National Observer</t>
-  </si>
-  <si>
-    <t>Region Observer</t>
-  </si>
-  <si>
-    <t>District Observer</t>
-  </si>
-  <si>
-    <t>National Clinician</t>
-  </si>
-  <si>
-    <t>POE Informant</t>
-  </si>
-  <si>
-    <t>POE Supervisor</t>
-  </si>
-  <si>
-    <t>POE National User</t>
-  </si>
-  <si>
-    <t>Import User</t>
-  </si>
-  <si>
-    <t>External Visits User</t>
-  </si>
-  <si>
-    <t>ReST User</t>
+    <t>de.symeda.sormas.api.user.UserRoleDto@3e0fcccd</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@3dff5cbb</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@50f0fbb6</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@945b91d2</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@2e755b7e</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@ada82ce5</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@49166699</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@5c4685c9</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@73406cd2</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@1b26af75</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@749ee487</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@7055444f</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@43772529</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@c97a495b</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@1fcf9a6c</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@9e69804d</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@33a6c500</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@82eb2d81</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@598f9824</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@b77cd212</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@d588dfe6</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@37d680e7</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@1d0251b1</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@b58af9f9</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@7e620215</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@df15b86d</t>
+  </si>
+  <si>
+    <t>de.symeda.sormas.api.user.UserRoleDto@46843f7b</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Jurisdiction of role</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Nation</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>EXTERNAL_LABORATORY</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Point of entry</t>
+  </si>
+  <si>
+    <t>CASE_CREATE</t>
+  </si>
+  <si>
+    <t>Create new cases</t>
+  </si>
+  <si>
+    <t>Able to create new cases</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>CASE_VIEW</t>
+  </si>
+  <si>
+    <t>View existing cases</t>
+  </si>
+  <si>
+    <t>Able to view existing cases</t>
+  </si>
+  <si>
+    <t>CASE_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing cases</t>
+  </si>
+  <si>
+    <t>Able to edit existing cases</t>
+  </si>
+  <si>
+    <t>CASE_TRANSFER</t>
+  </si>
+  <si>
+    <t>Transfer cases to another region/district/facility</t>
+  </si>
+  <si>
+    <t>Able to transfer cases to another region/district/facility</t>
+  </si>
+  <si>
+    <t>CASE_REFER_FROM_POE</t>
+  </si>
+  <si>
+    <t>Refer case from point of entry</t>
+  </si>
+  <si>
+    <t>Able to refer case from point of entry</t>
+  </si>
+  <si>
+    <t>CASE_INVESTIGATE</t>
+  </si>
+  <si>
+    <t>Edit case investigation status</t>
+  </si>
+  <si>
+    <t>Able to edit case investigation status</t>
+  </si>
+  <si>
+    <t>CASE_CLASSIFY</t>
+  </si>
+  <si>
+    <t>Edit case classification and outcome</t>
+  </si>
+  <si>
+    <t>Able to edit case classification and outcome</t>
+  </si>
+  <si>
+    <t>CASE_CHANGE_DISEASE</t>
+  </si>
+  <si>
+    <t>Edit case disease</t>
+  </si>
+  <si>
+    <t>Able to edit case disease</t>
+  </si>
+  <si>
+    <t>CASE_CHANGE_EPID_NUMBER</t>
+  </si>
+  <si>
+    <t>Edit case epid number</t>
+  </si>
+  <si>
+    <t>Able to edit case epid number</t>
+  </si>
+  <si>
+    <t>CASE_DELETE</t>
+  </si>
+  <si>
+    <t>Delete cases from the system</t>
+  </si>
+  <si>
+    <t>Able to delete cases from the system</t>
+  </si>
+  <si>
+    <t>CASE_IMPORT</t>
+  </si>
+  <si>
+    <t>Import cases into SORMAS</t>
+  </si>
+  <si>
+    <t>Able to import cases into SORMAS</t>
+  </si>
+  <si>
+    <t>CASE_EXPORT</t>
+  </si>
+  <si>
+    <t>Export cases from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export cases from SORMAS</t>
+  </si>
+  <si>
+    <t>CASE_SHARE</t>
+  </si>
+  <si>
+    <t>Share cases with the whole country</t>
+  </si>
+  <si>
+    <t>Able to share cases with the whole country</t>
+  </si>
+  <si>
+    <t>CASE_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive cases</t>
+  </si>
+  <si>
+    <t>Able to archive cases</t>
+  </si>
+  <si>
+    <t>CASE_MERGE</t>
+  </si>
+  <si>
+    <t>Merge cases</t>
+  </si>
+  <si>
+    <t>Able to merge cases</t>
+  </si>
+  <si>
+    <t>CASE_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>Can be responsible for a case</t>
+  </si>
+  <si>
+    <t>IMMUNIZATION_VIEW</t>
+  </si>
+  <si>
+    <t>View existing immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>Able to view existing immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>IMMUNIZATION_CREATE</t>
+  </si>
+  <si>
+    <t>Create new immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>Able to create new immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>IMMUNIZATION_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>Able to edit existing immunizations and vaccinations</t>
+  </si>
+  <si>
+    <t>IMMUNIZATION_DELETE</t>
+  </si>
+  <si>
+    <t>Delete immunizations and vaccinations from the system</t>
+  </si>
+  <si>
+    <t>Able to delete immunizations and vaccinations from the system</t>
+  </si>
+  <si>
+    <t>IMMUNIZATION_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive immunizations</t>
+  </si>
+  <si>
+    <t>Able to archive immunizations</t>
+  </si>
+  <si>
+    <t>PERSON_VIEW</t>
+  </si>
+  <si>
+    <t>View existing persons</t>
+  </si>
+  <si>
+    <t>Able to view existing persons</t>
+  </si>
+  <si>
+    <t>PERSON_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing persons</t>
+  </si>
+  <si>
+    <t>Able to edit existing persons</t>
+  </si>
+  <si>
+    <t>PERSON_DELETE</t>
+  </si>
+  <si>
+    <t>Delete persons from the system</t>
+  </si>
+  <si>
+    <t>Able to delete persons from the system</t>
+  </si>
+  <si>
+    <t>PERSON_CONTACT_DETAILS_DELETE</t>
+  </si>
+  <si>
+    <t>Delete person contact details</t>
+  </si>
+  <si>
+    <t>Able to delete person contact details</t>
+  </si>
+  <si>
+    <t>PERSON_EXPORT</t>
+  </si>
+  <si>
+    <t>Export persons</t>
+  </si>
+  <si>
+    <t>Able to export persons</t>
+  </si>
+  <si>
+    <t>SAMPLE_CREATE</t>
+  </si>
+  <si>
+    <t>Create new samples</t>
+  </si>
+  <si>
+    <t>Able to create new samples</t>
+  </si>
+  <si>
+    <t>SAMPLE_VIEW</t>
+  </si>
+  <si>
+    <t>View existing samples</t>
+  </si>
+  <si>
+    <t>Able to view existing samples</t>
+  </si>
+  <si>
+    <t>SAMPLE_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing samples</t>
+  </si>
+  <si>
+    <t>Able to edit existing samples</t>
+  </si>
+  <si>
+    <t>SAMPLE_EDIT_NOT_OWNED</t>
+  </si>
+  <si>
+    <t>Edit samples reported by other users</t>
+  </si>
+  <si>
+    <t>Able to edit samples reported by other users</t>
+  </si>
+  <si>
+    <t>SAMPLE_DELETE</t>
+  </si>
+  <si>
+    <t>Delete samples from the system</t>
+  </si>
+  <si>
+    <t>Able to delete samples from the system</t>
+  </si>
+  <si>
+    <t>SAMPLE_TRANSFER</t>
+  </si>
+  <si>
+    <t>Transfer samples to another lab</t>
+  </si>
+  <si>
+    <t>Able to transfer samples to another lab</t>
+  </si>
+  <si>
+    <t>SAMPLE_EXPORT</t>
+  </si>
+  <si>
+    <t>Export samples from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export samples from SORMAS</t>
+  </si>
+  <si>
+    <t>PATHOGEN_TEST_CREATE</t>
+  </si>
+  <si>
+    <t>Create new pathogen tests</t>
+  </si>
+  <si>
+    <t>Able to create new pathogen tests</t>
+  </si>
+  <si>
+    <t>PATHOGEN_TEST_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing pathogen tests</t>
+  </si>
+  <si>
+    <t>Able to edit existing pathogen tests</t>
+  </si>
+  <si>
+    <t>PATHOGEN_TEST_DELETE</t>
+  </si>
+  <si>
+    <t>Delete pathogen tests from the system</t>
+  </si>
+  <si>
+    <t>Able to delete pathogen tests from the system</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_TEST_VIEW</t>
+  </si>
+  <si>
+    <t>View existing additional tests</t>
+  </si>
+  <si>
+    <t>Able to view existing additional tests</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_TEST_CREATE</t>
+  </si>
+  <si>
+    <t>Create new additional tests</t>
+  </si>
+  <si>
+    <t>Able to create new additional tests</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_TEST_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing additional tests</t>
+  </si>
+  <si>
+    <t>Able to edit existing additional tests</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_TEST_DELETE</t>
+  </si>
+  <si>
+    <t>Delete additional tests from the system</t>
+  </si>
+  <si>
+    <t>Able to delete additional tests from the system</t>
+  </si>
+  <si>
+    <t>CONTACT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new contacts</t>
+  </si>
+  <si>
+    <t>Able to create new contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_IMPORT</t>
+  </si>
+  <si>
+    <t>Import contacts</t>
+  </si>
+  <si>
+    <t>Able to import contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_VIEW</t>
+  </si>
+  <si>
+    <t>View existing contacts</t>
+  </si>
+  <si>
+    <t>Able to view existing contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive contacts</t>
+  </si>
+  <si>
+    <t>Able to archive contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_ASSIGN</t>
+  </si>
+  <si>
+    <t>Assign contacts to officers</t>
+  </si>
+  <si>
+    <t>Able to assign contacts to officers</t>
+  </si>
+  <si>
+    <t>CONTACT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing contacts</t>
+  </si>
+  <si>
+    <t>Able to edit existing contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete contacts from the system</t>
+  </si>
+  <si>
+    <t>Able to delete contacts from the system</t>
+  </si>
+  <si>
+    <t>CONTACT_CLASSIFY</t>
+  </si>
+  <si>
+    <t>Edit contact classification</t>
+  </si>
+  <si>
+    <t>Able to edit contact classification</t>
+  </si>
+  <si>
+    <t>CONTACT_CONVERT</t>
+  </si>
+  <si>
+    <t>Create resulting cases from contacts</t>
+  </si>
+  <si>
+    <t>Able to create resulting cases from contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_EXPORT</t>
+  </si>
+  <si>
+    <t>Export contacts from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export contacts from SORMAS</t>
+  </si>
+  <si>
+    <t>CONTACT_REASSIGN_CASE</t>
+  </si>
+  <si>
+    <t>Reassign the source case of contacts</t>
+  </si>
+  <si>
+    <t>Able to reassign the source case of contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_MERGE</t>
+  </si>
+  <si>
+    <t>Merge contacts</t>
+  </si>
+  <si>
+    <t>Able to merge contacts</t>
+  </si>
+  <si>
+    <t>CONTACT_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>Can be responsible for a contact</t>
+  </si>
+  <si>
+    <t>MANAGE_EXTERNAL_SYMPTOM_JOURNAL</t>
+  </si>
+  <si>
+    <t>Manage external symptom journal</t>
+  </si>
+  <si>
+    <t>Able to manage external symptom journal</t>
+  </si>
+  <si>
+    <t>VISIT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new visits</t>
+  </si>
+  <si>
+    <t>Able to create new visits</t>
+  </si>
+  <si>
+    <t>VISIT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing visits</t>
+  </si>
+  <si>
+    <t>Able to edit existing visits</t>
+  </si>
+  <si>
+    <t>VISIT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete visits from the system</t>
+  </si>
+  <si>
+    <t>Able to delete visits from the system</t>
+  </si>
+  <si>
+    <t>VISIT_EXPORT</t>
+  </si>
+  <si>
+    <t>Export visits from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export visits from SORMAS</t>
+  </si>
+  <si>
+    <t>TASK_CREATE</t>
+  </si>
+  <si>
+    <t>Create new tasks</t>
+  </si>
+  <si>
+    <t>Able to create new tasks</t>
+  </si>
+  <si>
+    <t>TASK_VIEW</t>
+  </si>
+  <si>
+    <t>View existing tasks</t>
+  </si>
+  <si>
+    <t>Able to view existing tasks</t>
+  </si>
+  <si>
+    <t>TASK_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing tasks</t>
+  </si>
+  <si>
+    <t>Able to edit existing tasks</t>
+  </si>
+  <si>
+    <t>TASK_ASSIGN</t>
+  </si>
+  <si>
+    <t>Assign tasks to users</t>
+  </si>
+  <si>
+    <t>Able to assign tasks to users</t>
+  </si>
+  <si>
+    <t>TASK_DELETE</t>
+  </si>
+  <si>
+    <t>Delete tasks from the system</t>
+  </si>
+  <si>
+    <t>Able to delete tasks from the system</t>
+  </si>
+  <si>
+    <t>TASK_EXPORT</t>
+  </si>
+  <si>
+    <t>Export tasks from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export tasks from SORMAS</t>
+  </si>
+  <si>
+    <t>ACTION_CREATE</t>
+  </si>
+  <si>
+    <t>Create new actions</t>
+  </si>
+  <si>
+    <t>Able to create new actions</t>
+  </si>
+  <si>
+    <t>ACTION_DELETE</t>
+  </si>
+  <si>
+    <t>Delete actions from the system</t>
+  </si>
+  <si>
+    <t>Able to delete actions from the system</t>
+  </si>
+  <si>
+    <t>ACTION_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing actions</t>
+  </si>
+  <si>
+    <t>Able to edit existing actions</t>
+  </si>
+  <si>
+    <t>EVENT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new events</t>
+  </si>
+  <si>
+    <t>Able to create new events</t>
+  </si>
+  <si>
+    <t>EVENT_VIEW</t>
+  </si>
+  <si>
+    <t>View existing events</t>
+  </si>
+  <si>
+    <t>Able to view existing events</t>
+  </si>
+  <si>
+    <t>EVENT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing events</t>
+  </si>
+  <si>
+    <t>Able to edit existing events</t>
+  </si>
+  <si>
+    <t>EVENT_IMPORT</t>
+  </si>
+  <si>
+    <t>Import events</t>
+  </si>
+  <si>
+    <t>Able to import events</t>
+  </si>
+  <si>
+    <t>EVENT_EXPORT</t>
+  </si>
+  <si>
+    <t>Export events from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export events from SORMAS</t>
+  </si>
+  <si>
+    <t>EVENT_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive events</t>
+  </si>
+  <si>
+    <t>Able to archive events</t>
+  </si>
+  <si>
+    <t>EVENT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete events from the system</t>
+  </si>
+  <si>
+    <t>Able to delete events from the system</t>
+  </si>
+  <si>
+    <t>EVENT_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>Can be responsible for an event</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Event participant archive</t>
+  </si>
+  <si>
+    <t>Able to archive event participants</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new event participants</t>
+  </si>
+  <si>
+    <t>Able to create new event participants</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing event participants</t>
+  </si>
+  <si>
+    <t>Able to edit existing event participants</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete event participants from the system</t>
+  </si>
+  <si>
+    <t>Able to delete event participants from the system</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_IMPORT</t>
+  </si>
+  <si>
+    <t>Import event participants</t>
+  </si>
+  <si>
+    <t>Able to import event participants</t>
+  </si>
+  <si>
+    <t>EVENTPARTICIPANT_VIEW</t>
+  </si>
+  <si>
+    <t>View existing event participants</t>
+  </si>
+  <si>
+    <t>Able to view existing event participants</t>
+  </si>
+  <si>
+    <t>EVENTGROUP_CREATE</t>
+  </si>
+  <si>
+    <t>Create new event groups</t>
+  </si>
+  <si>
+    <t>Able to create new event groups</t>
+  </si>
+  <si>
+    <t>EVENTGROUP_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing event groups</t>
+  </si>
+  <si>
+    <t>Able to edit existing event groups</t>
+  </si>
+  <si>
+    <t>EVENTGROUP_LINK</t>
+  </si>
+  <si>
+    <t>Link events to event groups</t>
+  </si>
+  <si>
+    <t>Able to link events to event groups</t>
+  </si>
+  <si>
+    <t>EVENTGROUP_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive event groups</t>
+  </si>
+  <si>
+    <t>Able to archive event groups</t>
+  </si>
+  <si>
+    <t>EVENTGROUP_DELETE</t>
+  </si>
+  <si>
+    <t>Delete event groups from the system</t>
+  </si>
+  <si>
+    <t>Able to delete event groups from the system</t>
+  </si>
+  <si>
+    <t>WEEKLYREPORT_CREATE</t>
+  </si>
+  <si>
+    <t>Create weekly reports</t>
+  </si>
+  <si>
+    <t>Able to create weekly reports</t>
+  </si>
+  <si>
+    <t>WEEKLYREPORT_VIEW</t>
+  </si>
+  <si>
+    <t>View weekly reports</t>
+  </si>
+  <si>
+    <t>Able to view weekly reports</t>
+  </si>
+  <si>
+    <t>USER_CREATE</t>
+  </si>
+  <si>
+    <t>Create new users</t>
+  </si>
+  <si>
+    <t>Able to create new users</t>
+  </si>
+  <si>
+    <t>USER_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing users</t>
+  </si>
+  <si>
+    <t>Able to edit existing users</t>
+  </si>
+  <si>
+    <t>USER_VIEW</t>
+  </si>
+  <si>
+    <t>View existing users</t>
+  </si>
+  <si>
+    <t>Able to view existing users</t>
+  </si>
+  <si>
+    <t>SEND_MANUAL_EXTERNAL_MESSAGES</t>
+  </si>
+  <si>
+    <t>Send manual external messages</t>
+  </si>
+  <si>
+    <t>Able to send manual external messages</t>
+  </si>
+  <si>
+    <t>STATISTICS_ACCESS</t>
+  </si>
+  <si>
+    <t>Access statistics</t>
+  </si>
+  <si>
+    <t>Able to access statistics</t>
+  </si>
+  <si>
+    <t>STATISTICS_EXPORT</t>
+  </si>
+  <si>
+    <t>Export detailed statistics from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export detailed statistics from SORMAS</t>
+  </si>
+  <si>
+    <t>DATABASE_EXPORT_ACCESS</t>
+  </si>
+  <si>
+    <t>Export the whole database</t>
+  </si>
+  <si>
+    <t>Able to export the whole database</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS</t>
+  </si>
+  <si>
+    <t>Perform bulk operations in lists</t>
+  </si>
+  <si>
+    <t>Able to perform bulk operations in lists</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS_EVENT</t>
+  </si>
+  <si>
+    <t>Perform bulk operations in the event directory</t>
+  </si>
+  <si>
+    <t>Able to perform bulk operations in the event directory</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS_EVENTPARTICIPANT</t>
+  </si>
+  <si>
+    <t>Perform bulk operations in the event participants directory</t>
+  </si>
+  <si>
+    <t>Able to perform bulk operations in the event participants directory</t>
+  </si>
+  <si>
+    <t>MANAGE_PUBLIC_EXPORT_CONFIGURATION</t>
+  </si>
+  <si>
+    <t>Manage public export configurations</t>
+  </si>
+  <si>
+    <t>Able to manage public export configurations</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS_CASE_SAMPLES</t>
+  </si>
+  <si>
+    <t>Perform bulk operations on case samples</t>
+  </si>
+  <si>
+    <t>Able to perform bulk operations on case samples</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS_PSEUDONYM</t>
+  </si>
+  <si>
+    <t>Perform bulk pseudonomization</t>
+  </si>
+  <si>
+    <t>Able to perform bulk pseudonomization</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_CREATE</t>
+  </si>
+  <si>
+    <t>Create new regions/districts/communities/facilities</t>
+  </si>
+  <si>
+    <t>Able to create new regions/districts/communities/facilities</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_EDIT</t>
+  </si>
+  <si>
+    <t>Edit regions/districts/communities/facilities</t>
+  </si>
+  <si>
+    <t>Able to edit regions/districts/communities/facilities</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_VIEW</t>
+  </si>
+  <si>
+    <t>View regions/districts/communities/facilities in the system</t>
+  </si>
+  <si>
+    <t>Able to view regions/districts/communities/facilities in the system</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_EXPORT</t>
+  </si>
+  <si>
+    <t>Export infrastructure data from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export infrastructure data from SORMAS</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_IMPORT</t>
+  </si>
+  <si>
+    <t>Import infrastructure data</t>
+  </si>
+  <si>
+    <t>Able to import infrastructure data</t>
+  </si>
+  <si>
+    <t>INFRASTRUCTURE_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive infrastructure data</t>
+  </si>
+  <si>
+    <t>Able to archive infrastructure data</t>
+  </si>
+  <si>
+    <t>DASHBOARD_SURVEILLANCE_VIEW</t>
+  </si>
+  <si>
+    <t>Access the surveillance supervisor dashboard</t>
+  </si>
+  <si>
+    <t>Able to access the surveillance supervisor dashboard</t>
+  </si>
+  <si>
+    <t>DASHBOARD_CONTACT_VIEW</t>
+  </si>
+  <si>
+    <t>Access the contact supervisor dashboard</t>
+  </si>
+  <si>
+    <t>Able to access the contact supervisor dashboard</t>
+  </si>
+  <si>
+    <t>DASHBOARD_CONTACT_VIEW_TRANSMISSION_CHAINS</t>
+  </si>
+  <si>
+    <t>View contact transmission chains on the dashboard</t>
+  </si>
+  <si>
+    <t>Able to view contact transmission chains on the dashboard</t>
+  </si>
+  <si>
+    <t>DASHBOARD_CAMPAIGNS_VIEW</t>
+  </si>
+  <si>
+    <t>Access campaigns dashboard</t>
+  </si>
+  <si>
+    <t>Able to access campaigns dashboard</t>
+  </si>
+  <si>
+    <t>CASE_CLINICIAN_VIEW</t>
+  </si>
+  <si>
+    <t>Access case sections concerned with clinician</t>
+  </si>
+  <si>
+    <t>Able to access case sections concerned with clinician</t>
+  </si>
+  <si>
+    <t>THERAPY_VIEW</t>
+  </si>
+  <si>
+    <t>View existing therapies</t>
+  </si>
+  <si>
+    <t>Able to view existing therapies</t>
+  </si>
+  <si>
+    <t>PRESCRIPTION_CREATE</t>
+  </si>
+  <si>
+    <t>Create new prescriptions</t>
+  </si>
+  <si>
+    <t>Able to create new prescriptions</t>
+  </si>
+  <si>
+    <t>PRESCRIPTION_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing prescriptions</t>
+  </si>
+  <si>
+    <t>Able to edit existing prescriptions</t>
+  </si>
+  <si>
+    <t>PRESCRIPTION_DELETE</t>
+  </si>
+  <si>
+    <t>Delete prescriptions from the system</t>
+  </si>
+  <si>
+    <t>Able to delete prescriptions from the system</t>
+  </si>
+  <si>
+    <t>TREATMENT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new treatments</t>
+  </si>
+  <si>
+    <t>Able to create new treatments</t>
+  </si>
+  <si>
+    <t>TREATMENT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing treatments</t>
+  </si>
+  <si>
+    <t>Able to edit existing treatments</t>
+  </si>
+  <si>
+    <t>TREATMENT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete treatments from the system</t>
+  </si>
+  <si>
+    <t>Able to delete treatments from the system</t>
+  </si>
+  <si>
+    <t>CLINICAL_COURSE_VIEW</t>
+  </si>
+  <si>
+    <t>View the clinical course of cases</t>
+  </si>
+  <si>
+    <t>Able to view the clinical course of cases</t>
+  </si>
+  <si>
+    <t>CLINICAL_COURSE_EDIT</t>
+  </si>
+  <si>
+    <t>Edit the clinical course of cases</t>
+  </si>
+  <si>
+    <t>Able to edit the clinical course of cases</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_CREATE</t>
+  </si>
+  <si>
+    <t>Create new clinical visits</t>
+  </si>
+  <si>
+    <t>Able to create new clinical visits</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing clinical visits</t>
+  </si>
+  <si>
+    <t>Able to edit existing clinical visits</t>
+  </si>
+  <si>
+    <t>CLINICAL_VISIT_DELETE</t>
+  </si>
+  <si>
+    <t>Delete clinical visits from the system</t>
+  </si>
+  <si>
+    <t>Able to delete clinical visits from the system</t>
+  </si>
+  <si>
+    <t>PORT_HEALTH_INFO_VIEW</t>
+  </si>
+  <si>
+    <t>View port health info</t>
+  </si>
+  <si>
+    <t>Able to view port health info</t>
+  </si>
+  <si>
+    <t>PORT_HEALTH_INFO_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing port health info</t>
+  </si>
+  <si>
+    <t>Able to edit existing port health info</t>
+  </si>
+  <si>
+    <t>POPULATION_MANAGE</t>
+  </si>
+  <si>
+    <t>Manage population data</t>
+  </si>
+  <si>
+    <t>Able to manage population data</t>
+  </si>
+  <si>
+    <t>DOCUMENT_TEMPLATE_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Manage document templates</t>
+  </si>
+  <si>
+    <t>Able to manage document templates</t>
+  </si>
+  <si>
+    <t>QUARANTINE_ORDER_CREATE</t>
+  </si>
+  <si>
+    <t>Create new quarantine orders</t>
+  </si>
+  <si>
+    <t>Able to create new quarantine orders</t>
+  </si>
+  <si>
+    <t>LINE_LISTING_CONFIGURE</t>
+  </si>
+  <si>
+    <t>Configure line listing</t>
+  </si>
+  <si>
+    <t>Able to configure line listing</t>
+  </si>
+  <si>
+    <t>AGGREGATE_REPORT_VIEW</t>
+  </si>
+  <si>
+    <t>Create new aggregate reports</t>
+  </si>
+  <si>
+    <t>Able to create new aggregate reports</t>
+  </si>
+  <si>
+    <t>AGGREGATE_REPORT_EXPORT</t>
+  </si>
+  <si>
+    <t>Export aggregate reports from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export aggregate reports from SORMAS</t>
+  </si>
+  <si>
+    <t>AGGREGATE_REPORT_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing aggregate reports</t>
+  </si>
+  <si>
+    <t>Able to edit existing aggregate reports</t>
+  </si>
+  <si>
+    <t>SEE_PERSONAL_DATA_IN_JURISDICTION</t>
+  </si>
+  <si>
+    <t>See personal data in jurisdiction</t>
+  </si>
+  <si>
+    <t>Able to see personal data in jurisdiction</t>
+  </si>
+  <si>
+    <t>SEE_PERSONAL_DATA_OUTSIDE_JURISDICTION</t>
+  </si>
+  <si>
+    <t>See personal data outside jurisdiction</t>
+  </si>
+  <si>
+    <t>Able to see personal data outside jurisdiction</t>
+  </si>
+  <si>
+    <t>SEE_SENSITIVE_DATA_IN_JURISDICTION</t>
+  </si>
+  <si>
+    <t>See sensitive data in jurisdiction</t>
+  </si>
+  <si>
+    <t>Able to see sensitive data in jurisdiction</t>
+  </si>
+  <si>
+    <t>SEE_SENSITIVE_DATA_OUTSIDE_JURISDICTION</t>
+  </si>
+  <si>
+    <t>See sensitive data outside jurisdiction</t>
+  </si>
+  <si>
+    <t>Able to see sensitive data outside jurisdiction</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_VIEW</t>
+  </si>
+  <si>
+    <t>View existing campaigns</t>
+  </si>
+  <si>
+    <t>Able to view existing campaigns</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing campaigns</t>
+  </si>
+  <si>
+    <t>Able to edit existing campaigns</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive campaigns</t>
+  </si>
+  <si>
+    <t>Able to archive campaigns</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_DELETE</t>
+  </si>
+  <si>
+    <t>Delete campaigns from the system</t>
+  </si>
+  <si>
+    <t>Able to delete campaigns from the system</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_FORM_DATA_VIEW</t>
+  </si>
+  <si>
+    <t>View existing campaign form data</t>
+  </si>
+  <si>
+    <t>Able to view existing campaign form data</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_FORM_DATA_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing campaign form data</t>
+  </si>
+  <si>
+    <t>Able to edit existing campaign form data</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_FORM_DATA_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive campaign form data</t>
+  </si>
+  <si>
+    <t>Able to archive campaign form data</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_FORM_DATA_DELETE</t>
+  </si>
+  <si>
+    <t>Delete campaign form data from the system</t>
+  </si>
+  <si>
+    <t>Able to delete campaign form data from the system</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_FORM_DATA_EXPORT</t>
+  </si>
+  <si>
+    <t>Export campaign form data from SORMAS</t>
+  </si>
+  <si>
+    <t>Able to export campaign form data from SORMAS</t>
+  </si>
+  <si>
+    <t>BAG_EXPORT</t>
+  </si>
+  <si>
+    <t>Perform BAG export</t>
+  </si>
+  <si>
+    <t>Able to perform BAG export</t>
+  </si>
+  <si>
+    <t>SORMAS_TO_SORMAS_SHARE</t>
+  </si>
+  <si>
+    <t>Share data from one SORMAS instance to another</t>
+  </si>
+  <si>
+    <t>Able to share data from one SORMAS instance to another</t>
+  </si>
+  <si>
+    <t>LAB_MESSAGES</t>
+  </si>
+  <si>
+    <t>Manage lab messages</t>
+  </si>
+  <si>
+    <t>Able to manage lab messages</t>
+  </si>
+  <si>
+    <t>PERFORM_BULK_OPERATIONS_LAB_MESSAGES</t>
+  </si>
+  <si>
+    <t>Perform bulk operations in lab messages list</t>
+  </si>
+  <si>
+    <t>Able to perform bulk operations in lab messages list</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
+  </si>
+  <si>
+    <t>Access the travel entry directory</t>
+  </si>
+  <si>
+    <t>Able to access the travel entry directory</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_VIEW</t>
+  </si>
+  <si>
+    <t>View existing travel entries</t>
+  </si>
+  <si>
+    <t>Able to view existing travel entries</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_CREATE</t>
+  </si>
+  <si>
+    <t>Create new travel entries</t>
+  </si>
+  <si>
+    <t>Able to create new travel entries</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_EDIT</t>
+  </si>
+  <si>
+    <t>Edit existing travel entries</t>
+  </si>
+  <si>
+    <t>Able to edit existing travel entries</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_DELETE</t>
+  </si>
+  <si>
+    <t>Delete travel entries from the system</t>
+  </si>
+  <si>
+    <t>Able to delete travel entries from the system</t>
+  </si>
+  <si>
+    <t>TRAVEL_ENTRY_ARCHIVE</t>
+  </si>
+  <si>
+    <t>Archive travel entries</t>
+  </si>
+  <si>
+    <t>Able to archive travel entries</t>
+  </si>
+  <si>
+    <t>EXPORT_DATA_PROTECTION_DATA</t>
+  </si>
+  <si>
+    <t>Export data protection data</t>
+  </si>
+  <si>
+    <t>Able to export data protection data</t>
+  </si>
+  <si>
+    <t>OUTBREAK_VIEW</t>
+  </si>
+  <si>
+    <t>View outbreaks</t>
+  </si>
+  <si>
+    <t>Able to view outbreaks</t>
+  </si>
+  <si>
+    <t>OUTBREAK_EDIT</t>
+  </si>
+  <si>
+    <t>Edit outbreaks</t>
+  </si>
+  <si>
+    <t>Able to edit outbreaks</t>
+  </si>
+  <si>
+    <t>SORMAS_REST</t>
+  </si>
+  <si>
+    <t>Access Sormas REST</t>
+  </si>
+  <si>
+    <t>Able to access the SORMAS REST interface</t>
+  </si>
+  <si>
+    <t>SORMAS_UI</t>
+  </si>
+  <si>
+    <t>Access Sormas UI</t>
+  </si>
+  <si>
+    <t>Able to access the SORMAS graphical user interface</t>
+  </si>
+  <si>
+    <t>SORMAS_TO_SORMAS_CLIENT</t>
   </si>
   <si>
     <t>Sormas to Sormas Client</t>
-  </si>
-  <si>
-    <t>BAG User</t>
-  </si>
-  <si>
-    <t>Jurisdiction</t>
-  </si>
-  <si>
-    <t>Jurisdiction of role</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Nation</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>Laboratory</t>
-  </si>
-  <si>
-    <t>EXTERNAL_LABORATORY</t>
-  </si>
-  <si>
-    <t>Point of entry</t>
-  </si>
-  <si>
-    <t>CASE_CREATE</t>
-  </si>
-  <si>
-    <t>Create new cases</t>
-  </si>
-  <si>
-    <t>Able to create new cases</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>CASE_VIEW</t>
-  </si>
-  <si>
-    <t>View existing cases</t>
-  </si>
-  <si>
-    <t>Able to view existing cases</t>
-  </si>
-  <si>
-    <t>CASE_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing cases</t>
-  </si>
-  <si>
-    <t>Able to edit existing cases</t>
-  </si>
-  <si>
-    <t>CASE_TRANSFER</t>
-  </si>
-  <si>
-    <t>Transfer cases to another region/district/facility</t>
-  </si>
-  <si>
-    <t>Able to transfer cases to another region/district/facility</t>
-  </si>
-  <si>
-    <t>CASE_REFER_FROM_POE</t>
-  </si>
-  <si>
-    <t>Refer case from point of entry</t>
-  </si>
-  <si>
-    <t>Able to refer case from point of entry</t>
-  </si>
-  <si>
-    <t>CASE_INVESTIGATE</t>
-  </si>
-  <si>
-    <t>Edit case investigation status</t>
-  </si>
-  <si>
-    <t>Able to edit case investigation status</t>
-  </si>
-  <si>
-    <t>CASE_CLASSIFY</t>
-  </si>
-  <si>
-    <t>Edit case classification and outcome</t>
-  </si>
-  <si>
-    <t>Able to edit case classification and outcome</t>
-  </si>
-  <si>
-    <t>CASE_CHANGE_DISEASE</t>
-  </si>
-  <si>
-    <t>Edit case disease</t>
-  </si>
-  <si>
-    <t>Able to edit case disease</t>
-  </si>
-  <si>
-    <t>CASE_CHANGE_EPID_NUMBER</t>
-  </si>
-  <si>
-    <t>Edit case epid number</t>
-  </si>
-  <si>
-    <t>Able to edit case epid number</t>
-  </si>
-  <si>
-    <t>CASE_DELETE</t>
-  </si>
-  <si>
-    <t>Delete cases from the system</t>
-  </si>
-  <si>
-    <t>Able to delete cases from the system</t>
-  </si>
-  <si>
-    <t>CASE_IMPORT</t>
-  </si>
-  <si>
-    <t>Import cases into SORMAS</t>
-  </si>
-  <si>
-    <t>Able to import cases into SORMAS</t>
-  </si>
-  <si>
-    <t>CASE_EXPORT</t>
-  </si>
-  <si>
-    <t>Export cases from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export cases from SORMAS</t>
-  </si>
-  <si>
-    <t>CASE_SHARE</t>
-  </si>
-  <si>
-    <t>Share cases with the whole country</t>
-  </si>
-  <si>
-    <t>Able to share cases with the whole country</t>
-  </si>
-  <si>
-    <t>CASE_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive cases</t>
-  </si>
-  <si>
-    <t>Able to archive cases</t>
-  </si>
-  <si>
-    <t>CASE_MERGE</t>
-  </si>
-  <si>
-    <t>Merge cases</t>
-  </si>
-  <si>
-    <t>Able to merge cases</t>
-  </si>
-  <si>
-    <t>CASE_RESPONSIBLE</t>
-  </si>
-  <si>
-    <t>Can be responsible for a case</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION_VIEW</t>
-  </si>
-  <si>
-    <t>View existing immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>Able to view existing immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION_CREATE</t>
-  </si>
-  <si>
-    <t>Create new immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>Able to create new immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>Able to edit existing immunizations and vaccinations</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION_DELETE</t>
-  </si>
-  <si>
-    <t>Delete immunizations and vaccinations from the system</t>
-  </si>
-  <si>
-    <t>Able to delete immunizations and vaccinations from the system</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive immunizations</t>
-  </si>
-  <si>
-    <t>Able to archive immunizations</t>
-  </si>
-  <si>
-    <t>PERSON_VIEW</t>
-  </si>
-  <si>
-    <t>View existing persons</t>
-  </si>
-  <si>
-    <t>Able to view existing persons</t>
-  </si>
-  <si>
-    <t>PERSON_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing persons</t>
-  </si>
-  <si>
-    <t>Able to edit existing persons</t>
-  </si>
-  <si>
-    <t>PERSON_DELETE</t>
-  </si>
-  <si>
-    <t>Delete persons from the system</t>
-  </si>
-  <si>
-    <t>Able to delete persons from the system</t>
-  </si>
-  <si>
-    <t>PERSON_CONTACT_DETAILS_DELETE</t>
-  </si>
-  <si>
-    <t>Delete person contact details</t>
-  </si>
-  <si>
-    <t>Able to delete person contact details</t>
-  </si>
-  <si>
-    <t>PERSON_EXPORT</t>
-  </si>
-  <si>
-    <t>Export persons</t>
-  </si>
-  <si>
-    <t>Able to export persons</t>
-  </si>
-  <si>
-    <t>SAMPLE_CREATE</t>
-  </si>
-  <si>
-    <t>Create new samples</t>
-  </si>
-  <si>
-    <t>Able to create new samples</t>
-  </si>
-  <si>
-    <t>SAMPLE_VIEW</t>
-  </si>
-  <si>
-    <t>View existing samples</t>
-  </si>
-  <si>
-    <t>Able to view existing samples</t>
-  </si>
-  <si>
-    <t>SAMPLE_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing samples</t>
-  </si>
-  <si>
-    <t>Able to edit existing samples</t>
-  </si>
-  <si>
-    <t>SAMPLE_EDIT_NOT_OWNED</t>
-  </si>
-  <si>
-    <t>Edit samples reported by other users</t>
-  </si>
-  <si>
-    <t>Able to edit samples reported by other users</t>
-  </si>
-  <si>
-    <t>SAMPLE_DELETE</t>
-  </si>
-  <si>
-    <t>Delete samples from the system</t>
-  </si>
-  <si>
-    <t>Able to delete samples from the system</t>
-  </si>
-  <si>
-    <t>SAMPLE_TRANSFER</t>
-  </si>
-  <si>
-    <t>Transfer samples to another lab</t>
-  </si>
-  <si>
-    <t>Able to transfer samples to another lab</t>
-  </si>
-  <si>
-    <t>SAMPLE_EXPORT</t>
-  </si>
-  <si>
-    <t>Export samples from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export samples from SORMAS</t>
-  </si>
-  <si>
-    <t>PATHOGEN_TEST_CREATE</t>
-  </si>
-  <si>
-    <t>Create new pathogen tests</t>
-  </si>
-  <si>
-    <t>Able to create new pathogen tests</t>
-  </si>
-  <si>
-    <t>PATHOGEN_TEST_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing pathogen tests</t>
-  </si>
-  <si>
-    <t>Able to edit existing pathogen tests</t>
-  </si>
-  <si>
-    <t>PATHOGEN_TEST_DELETE</t>
-  </si>
-  <si>
-    <t>Delete pathogen tests from the system</t>
-  </si>
-  <si>
-    <t>Able to delete pathogen tests from the system</t>
-  </si>
-  <si>
-    <t>ADDITIONAL_TEST_VIEW</t>
-  </si>
-  <si>
-    <t>View existing additional tests</t>
-  </si>
-  <si>
-    <t>Able to view existing additional tests</t>
-  </si>
-  <si>
-    <t>ADDITIONAL_TEST_CREATE</t>
-  </si>
-  <si>
-    <t>Create new additional tests</t>
-  </si>
-  <si>
-    <t>Able to create new additional tests</t>
-  </si>
-  <si>
-    <t>ADDITIONAL_TEST_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing additional tests</t>
-  </si>
-  <si>
-    <t>Able to edit existing additional tests</t>
-  </si>
-  <si>
-    <t>ADDITIONAL_TEST_DELETE</t>
-  </si>
-  <si>
-    <t>Delete additional tests from the system</t>
-  </si>
-  <si>
-    <t>Able to delete additional tests from the system</t>
-  </si>
-  <si>
-    <t>CONTACT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new contacts</t>
-  </si>
-  <si>
-    <t>Able to create new contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_IMPORT</t>
-  </si>
-  <si>
-    <t>Import contacts</t>
-  </si>
-  <si>
-    <t>Able to import contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_VIEW</t>
-  </si>
-  <si>
-    <t>View existing contacts</t>
-  </si>
-  <si>
-    <t>Able to view existing contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive contacts</t>
-  </si>
-  <si>
-    <t>Able to archive contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_ASSIGN</t>
-  </si>
-  <si>
-    <t>Assign contacts to officers</t>
-  </si>
-  <si>
-    <t>Able to assign contacts to officers</t>
-  </si>
-  <si>
-    <t>CONTACT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing contacts</t>
-  </si>
-  <si>
-    <t>Able to edit existing contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete contacts from the system</t>
-  </si>
-  <si>
-    <t>Able to delete contacts from the system</t>
-  </si>
-  <si>
-    <t>CONTACT_CLASSIFY</t>
-  </si>
-  <si>
-    <t>Edit contact classification</t>
-  </si>
-  <si>
-    <t>Able to edit contact classification</t>
-  </si>
-  <si>
-    <t>CONTACT_CONVERT</t>
-  </si>
-  <si>
-    <t>Create resulting cases from contacts</t>
-  </si>
-  <si>
-    <t>Able to create resulting cases from contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_EXPORT</t>
-  </si>
-  <si>
-    <t>Export contacts from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export contacts from SORMAS</t>
-  </si>
-  <si>
-    <t>CONTACT_REASSIGN_CASE</t>
-  </si>
-  <si>
-    <t>Reassign the source case of contacts</t>
-  </si>
-  <si>
-    <t>Able to reassign the source case of contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_MERGE</t>
-  </si>
-  <si>
-    <t>Merge contacts</t>
-  </si>
-  <si>
-    <t>Able to merge contacts</t>
-  </si>
-  <si>
-    <t>CONTACT_RESPONSIBLE</t>
-  </si>
-  <si>
-    <t>Can be responsible for a contact</t>
-  </si>
-  <si>
-    <t>MANAGE_EXTERNAL_SYMPTOM_JOURNAL</t>
-  </si>
-  <si>
-    <t>Manage external symptom journal</t>
-  </si>
-  <si>
-    <t>Able to manage external symptom journal</t>
-  </si>
-  <si>
-    <t>VISIT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new visits</t>
-  </si>
-  <si>
-    <t>Able to create new visits</t>
-  </si>
-  <si>
-    <t>VISIT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing visits</t>
-  </si>
-  <si>
-    <t>Able to edit existing visits</t>
-  </si>
-  <si>
-    <t>VISIT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete visits from the system</t>
-  </si>
-  <si>
-    <t>Able to delete visits from the system</t>
-  </si>
-  <si>
-    <t>VISIT_EXPORT</t>
-  </si>
-  <si>
-    <t>Export visits from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export visits from SORMAS</t>
-  </si>
-  <si>
-    <t>TASK_CREATE</t>
-  </si>
-  <si>
-    <t>Create new tasks</t>
-  </si>
-  <si>
-    <t>Able to create new tasks</t>
-  </si>
-  <si>
-    <t>TASK_VIEW</t>
-  </si>
-  <si>
-    <t>View existing tasks</t>
-  </si>
-  <si>
-    <t>Able to view existing tasks</t>
-  </si>
-  <si>
-    <t>TASK_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing tasks</t>
-  </si>
-  <si>
-    <t>Able to edit existing tasks</t>
-  </si>
-  <si>
-    <t>TASK_ASSIGN</t>
-  </si>
-  <si>
-    <t>Assign tasks to users</t>
-  </si>
-  <si>
-    <t>Able to assign tasks to users</t>
-  </si>
-  <si>
-    <t>TASK_DELETE</t>
-  </si>
-  <si>
-    <t>Delete tasks from the system</t>
-  </si>
-  <si>
-    <t>Able to delete tasks from the system</t>
-  </si>
-  <si>
-    <t>TASK_EXPORT</t>
-  </si>
-  <si>
-    <t>Export tasks from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export tasks from SORMAS</t>
-  </si>
-  <si>
-    <t>ACTION_CREATE</t>
-  </si>
-  <si>
-    <t>Create new actions</t>
-  </si>
-  <si>
-    <t>Able to create new actions</t>
-  </si>
-  <si>
-    <t>ACTION_DELETE</t>
-  </si>
-  <si>
-    <t>Delete actions from the system</t>
-  </si>
-  <si>
-    <t>Able to delete actions from the system</t>
-  </si>
-  <si>
-    <t>ACTION_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing actions</t>
-  </si>
-  <si>
-    <t>Able to edit existing actions</t>
-  </si>
-  <si>
-    <t>EVENT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new events</t>
-  </si>
-  <si>
-    <t>Able to create new events</t>
-  </si>
-  <si>
-    <t>EVENT_VIEW</t>
-  </si>
-  <si>
-    <t>View existing events</t>
-  </si>
-  <si>
-    <t>Able to view existing events</t>
-  </si>
-  <si>
-    <t>EVENT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing events</t>
-  </si>
-  <si>
-    <t>Able to edit existing events</t>
-  </si>
-  <si>
-    <t>EVENT_IMPORT</t>
-  </si>
-  <si>
-    <t>Import events</t>
-  </si>
-  <si>
-    <t>Able to import events</t>
-  </si>
-  <si>
-    <t>EVENT_EXPORT</t>
-  </si>
-  <si>
-    <t>Export events from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export events from SORMAS</t>
-  </si>
-  <si>
-    <t>EVENT_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive events</t>
-  </si>
-  <si>
-    <t>Able to archive events</t>
-  </si>
-  <si>
-    <t>EVENT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete events from the system</t>
-  </si>
-  <si>
-    <t>Able to delete events from the system</t>
-  </si>
-  <si>
-    <t>EVENT_RESPONSIBLE</t>
-  </si>
-  <si>
-    <t>Can be responsible for an event</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Event participant archive</t>
-  </si>
-  <si>
-    <t>Able to archive event participants</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new event participants</t>
-  </si>
-  <si>
-    <t>Able to create new event participants</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing event participants</t>
-  </si>
-  <si>
-    <t>Able to edit existing event participants</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete event participants from the system</t>
-  </si>
-  <si>
-    <t>Able to delete event participants from the system</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_IMPORT</t>
-  </si>
-  <si>
-    <t>Import event participants</t>
-  </si>
-  <si>
-    <t>Able to import event participants</t>
-  </si>
-  <si>
-    <t>EVENTPARTICIPANT_VIEW</t>
-  </si>
-  <si>
-    <t>View existing event participants</t>
-  </si>
-  <si>
-    <t>Able to view existing event participants</t>
-  </si>
-  <si>
-    <t>EVENTGROUP_CREATE</t>
-  </si>
-  <si>
-    <t>Create new event groups</t>
-  </si>
-  <si>
-    <t>Able to create new event groups</t>
-  </si>
-  <si>
-    <t>EVENTGROUP_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing event groups</t>
-  </si>
-  <si>
-    <t>Able to edit existing event groups</t>
-  </si>
-  <si>
-    <t>EVENTGROUP_LINK</t>
-  </si>
-  <si>
-    <t>Link events to event groups</t>
-  </si>
-  <si>
-    <t>Able to link events to event groups</t>
-  </si>
-  <si>
-    <t>EVENTGROUP_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive event groups</t>
-  </si>
-  <si>
-    <t>Able to archive event groups</t>
-  </si>
-  <si>
-    <t>EVENTGROUP_DELETE</t>
-  </si>
-  <si>
-    <t>Delete event groups from the system</t>
-  </si>
-  <si>
-    <t>Able to delete event groups from the system</t>
-  </si>
-  <si>
-    <t>WEEKLYREPORT_CREATE</t>
-  </si>
-  <si>
-    <t>Create weekly reports</t>
-  </si>
-  <si>
-    <t>Able to create weekly reports</t>
-  </si>
-  <si>
-    <t>WEEKLYREPORT_VIEW</t>
-  </si>
-  <si>
-    <t>View weekly reports</t>
-  </si>
-  <si>
-    <t>Able to view weekly reports</t>
-  </si>
-  <si>
-    <t>USER_CREATE</t>
-  </si>
-  <si>
-    <t>Create new users</t>
-  </si>
-  <si>
-    <t>Able to create new users</t>
-  </si>
-  <si>
-    <t>USER_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing users</t>
-  </si>
-  <si>
-    <t>Able to edit existing users</t>
-  </si>
-  <si>
-    <t>USER_VIEW</t>
-  </si>
-  <si>
-    <t>View existing users</t>
-  </si>
-  <si>
-    <t>Able to view existing users</t>
-  </si>
-  <si>
-    <t>SEND_MANUAL_EXTERNAL_MESSAGES</t>
-  </si>
-  <si>
-    <t>Send manual external messages</t>
-  </si>
-  <si>
-    <t>Able to send manual external messages</t>
-  </si>
-  <si>
-    <t>STATISTICS_ACCESS</t>
-  </si>
-  <si>
-    <t>Access statistics</t>
-  </si>
-  <si>
-    <t>Able to access statistics</t>
-  </si>
-  <si>
-    <t>STATISTICS_EXPORT</t>
-  </si>
-  <si>
-    <t>Export detailed statistics from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export detailed statistics from SORMAS</t>
-  </si>
-  <si>
-    <t>DATABASE_EXPORT_ACCESS</t>
-  </si>
-  <si>
-    <t>Export the whole database</t>
-  </si>
-  <si>
-    <t>Able to export the whole database</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS</t>
-  </si>
-  <si>
-    <t>Perform bulk operations in lists</t>
-  </si>
-  <si>
-    <t>Able to perform bulk operations in lists</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS_EVENT</t>
-  </si>
-  <si>
-    <t>Perform bulk operations in the event directory</t>
-  </si>
-  <si>
-    <t>Able to perform bulk operations in the event directory</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS_EVENTPARTICIPANT</t>
-  </si>
-  <si>
-    <t>Perform bulk operations in the event participants directory</t>
-  </si>
-  <si>
-    <t>Able to perform bulk operations in the event participants directory</t>
-  </si>
-  <si>
-    <t>MANAGE_PUBLIC_EXPORT_CONFIGURATION</t>
-  </si>
-  <si>
-    <t>Manage public export configurations</t>
-  </si>
-  <si>
-    <t>Able to manage public export configurations</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS_CASE_SAMPLES</t>
-  </si>
-  <si>
-    <t>Perform bulk operations on case samples</t>
-  </si>
-  <si>
-    <t>Able to perform bulk operations on case samples</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS_PSEUDONYM</t>
-  </si>
-  <si>
-    <t>Perform bulk pseudonomization</t>
-  </si>
-  <si>
-    <t>Able to perform bulk pseudonomization</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_CREATE</t>
-  </si>
-  <si>
-    <t>Create new regions/districts/communities/facilities</t>
-  </si>
-  <si>
-    <t>Able to create new regions/districts/communities/facilities</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_EDIT</t>
-  </si>
-  <si>
-    <t>Edit regions/districts/communities/facilities</t>
-  </si>
-  <si>
-    <t>Able to edit regions/districts/communities/facilities</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_VIEW</t>
-  </si>
-  <si>
-    <t>View regions/districts/communities/facilities in the system</t>
-  </si>
-  <si>
-    <t>Able to view regions/districts/communities/facilities in the system</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_EXPORT</t>
-  </si>
-  <si>
-    <t>Export infrastructure data from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export infrastructure data from SORMAS</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_IMPORT</t>
-  </si>
-  <si>
-    <t>Import infrastructure data</t>
-  </si>
-  <si>
-    <t>Able to import infrastructure data</t>
-  </si>
-  <si>
-    <t>INFRASTRUCTURE_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive infrastructure data</t>
-  </si>
-  <si>
-    <t>Able to archive infrastructure data</t>
-  </si>
-  <si>
-    <t>DASHBOARD_SURVEILLANCE_VIEW</t>
-  </si>
-  <si>
-    <t>Access the surveillance supervisor dashboard</t>
-  </si>
-  <si>
-    <t>Able to access the surveillance supervisor dashboard</t>
-  </si>
-  <si>
-    <t>DASHBOARD_CONTACT_VIEW</t>
-  </si>
-  <si>
-    <t>Access the contact supervisor dashboard</t>
-  </si>
-  <si>
-    <t>Able to access the contact supervisor dashboard</t>
-  </si>
-  <si>
-    <t>DASHBOARD_CONTACT_VIEW_TRANSMISSION_CHAINS</t>
-  </si>
-  <si>
-    <t>View contact transmission chains on the dashboard</t>
-  </si>
-  <si>
-    <t>Able to view contact transmission chains on the dashboard</t>
-  </si>
-  <si>
-    <t>DASHBOARD_CAMPAIGNS_VIEW</t>
-  </si>
-  <si>
-    <t>Access campaigns dashboard</t>
-  </si>
-  <si>
-    <t>Able to access campaigns dashboard</t>
-  </si>
-  <si>
-    <t>CASE_CLINICIAN_VIEW</t>
-  </si>
-  <si>
-    <t>Access case sections concerned with clinician</t>
-  </si>
-  <si>
-    <t>Able to access case sections concerned with clinician</t>
-  </si>
-  <si>
-    <t>THERAPY_VIEW</t>
-  </si>
-  <si>
-    <t>View existing therapies</t>
-  </si>
-  <si>
-    <t>Able to view existing therapies</t>
-  </si>
-  <si>
-    <t>PRESCRIPTION_CREATE</t>
-  </si>
-  <si>
-    <t>Create new prescriptions</t>
-  </si>
-  <si>
-    <t>Able to create new prescriptions</t>
-  </si>
-  <si>
-    <t>PRESCRIPTION_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing prescriptions</t>
-  </si>
-  <si>
-    <t>Able to edit existing prescriptions</t>
-  </si>
-  <si>
-    <t>PRESCRIPTION_DELETE</t>
-  </si>
-  <si>
-    <t>Delete prescriptions from the system</t>
-  </si>
-  <si>
-    <t>Able to delete prescriptions from the system</t>
-  </si>
-  <si>
-    <t>TREATMENT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new treatments</t>
-  </si>
-  <si>
-    <t>Able to create new treatments</t>
-  </si>
-  <si>
-    <t>TREATMENT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing treatments</t>
-  </si>
-  <si>
-    <t>Able to edit existing treatments</t>
-  </si>
-  <si>
-    <t>TREATMENT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete treatments from the system</t>
-  </si>
-  <si>
-    <t>Able to delete treatments from the system</t>
-  </si>
-  <si>
-    <t>CLINICAL_COURSE_VIEW</t>
-  </si>
-  <si>
-    <t>View the clinical course of cases</t>
-  </si>
-  <si>
-    <t>Able to view the clinical course of cases</t>
-  </si>
-  <si>
-    <t>CLINICAL_COURSE_EDIT</t>
-  </si>
-  <si>
-    <t>Edit the clinical course of cases</t>
-  </si>
-  <si>
-    <t>Able to edit the clinical course of cases</t>
-  </si>
-  <si>
-    <t>CLINICAL_VISIT_CREATE</t>
-  </si>
-  <si>
-    <t>Create new clinical visits</t>
-  </si>
-  <si>
-    <t>Able to create new clinical visits</t>
-  </si>
-  <si>
-    <t>CLINICAL_VISIT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing clinical visits</t>
-  </si>
-  <si>
-    <t>Able to edit existing clinical visits</t>
-  </si>
-  <si>
-    <t>CLINICAL_VISIT_DELETE</t>
-  </si>
-  <si>
-    <t>Delete clinical visits from the system</t>
-  </si>
-  <si>
-    <t>Able to delete clinical visits from the system</t>
-  </si>
-  <si>
-    <t>PORT_HEALTH_INFO_VIEW</t>
-  </si>
-  <si>
-    <t>View port health info</t>
-  </si>
-  <si>
-    <t>Able to view port health info</t>
-  </si>
-  <si>
-    <t>PORT_HEALTH_INFO_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing port health info</t>
-  </si>
-  <si>
-    <t>Able to edit existing port health info</t>
-  </si>
-  <si>
-    <t>POPULATION_MANAGE</t>
-  </si>
-  <si>
-    <t>Manage population data</t>
-  </si>
-  <si>
-    <t>Able to manage population data</t>
-  </si>
-  <si>
-    <t>DOCUMENT_TEMPLATE_MANAGEMENT</t>
-  </si>
-  <si>
-    <t>Manage document templates</t>
-  </si>
-  <si>
-    <t>Able to manage document templates</t>
-  </si>
-  <si>
-    <t>QUARANTINE_ORDER_CREATE</t>
-  </si>
-  <si>
-    <t>Create new quarantine orders</t>
-  </si>
-  <si>
-    <t>Able to create new quarantine orders</t>
-  </si>
-  <si>
-    <t>LINE_LISTING_CONFIGURE</t>
-  </si>
-  <si>
-    <t>Configure line listing</t>
-  </si>
-  <si>
-    <t>Able to configure line listing</t>
-  </si>
-  <si>
-    <t>AGGREGATE_REPORT_VIEW</t>
-  </si>
-  <si>
-    <t>Create new aggregate reports</t>
-  </si>
-  <si>
-    <t>Able to create new aggregate reports</t>
-  </si>
-  <si>
-    <t>AGGREGATE_REPORT_EXPORT</t>
-  </si>
-  <si>
-    <t>Export aggregate reports from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export aggregate reports from SORMAS</t>
-  </si>
-  <si>
-    <t>AGGREGATE_REPORT_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing aggregate reports</t>
-  </si>
-  <si>
-    <t>Able to edit existing aggregate reports</t>
-  </si>
-  <si>
-    <t>SEE_PERSONAL_DATA_IN_JURISDICTION</t>
-  </si>
-  <si>
-    <t>See personal data in jurisdiction</t>
-  </si>
-  <si>
-    <t>Able to see personal data in jurisdiction</t>
-  </si>
-  <si>
-    <t>SEE_PERSONAL_DATA_OUTSIDE_JURISDICTION</t>
-  </si>
-  <si>
-    <t>See personal data outside jurisdiction</t>
-  </si>
-  <si>
-    <t>Able to see personal data outside jurisdiction</t>
-  </si>
-  <si>
-    <t>SEE_SENSITIVE_DATA_IN_JURISDICTION</t>
-  </si>
-  <si>
-    <t>See sensitive data in jurisdiction</t>
-  </si>
-  <si>
-    <t>Able to see sensitive data in jurisdiction</t>
-  </si>
-  <si>
-    <t>SEE_SENSITIVE_DATA_OUTSIDE_JURISDICTION</t>
-  </si>
-  <si>
-    <t>See sensitive data outside jurisdiction</t>
-  </si>
-  <si>
-    <t>Able to see sensitive data outside jurisdiction</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_VIEW</t>
-  </si>
-  <si>
-    <t>View existing campaigns</t>
-  </si>
-  <si>
-    <t>Able to view existing campaigns</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing campaigns</t>
-  </si>
-  <si>
-    <t>Able to edit existing campaigns</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive campaigns</t>
-  </si>
-  <si>
-    <t>Able to archive campaigns</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_DELETE</t>
-  </si>
-  <si>
-    <t>Delete campaigns from the system</t>
-  </si>
-  <si>
-    <t>Able to delete campaigns from the system</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_FORM_DATA_VIEW</t>
-  </si>
-  <si>
-    <t>View existing campaign form data</t>
-  </si>
-  <si>
-    <t>Able to view existing campaign form data</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_FORM_DATA_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing campaign form data</t>
-  </si>
-  <si>
-    <t>Able to edit existing campaign form data</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_FORM_DATA_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive campaign form data</t>
-  </si>
-  <si>
-    <t>Able to archive campaign form data</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_FORM_DATA_DELETE</t>
-  </si>
-  <si>
-    <t>Delete campaign form data from the system</t>
-  </si>
-  <si>
-    <t>Able to delete campaign form data from the system</t>
-  </si>
-  <si>
-    <t>CAMPAIGN_FORM_DATA_EXPORT</t>
-  </si>
-  <si>
-    <t>Export campaign form data from SORMAS</t>
-  </si>
-  <si>
-    <t>Able to export campaign form data from SORMAS</t>
-  </si>
-  <si>
-    <t>BAG_EXPORT</t>
-  </si>
-  <si>
-    <t>Perform BAG export</t>
-  </si>
-  <si>
-    <t>Able to perform BAG export</t>
-  </si>
-  <si>
-    <t>SORMAS_TO_SORMAS_SHARE</t>
-  </si>
-  <si>
-    <t>Share data from one SORMAS instance to another</t>
-  </si>
-  <si>
-    <t>Able to share data from one SORMAS instance to another</t>
-  </si>
-  <si>
-    <t>LAB_MESSAGES</t>
-  </si>
-  <si>
-    <t>Manage lab messages</t>
-  </si>
-  <si>
-    <t>Able to manage lab messages</t>
-  </si>
-  <si>
-    <t>PERFORM_BULK_OPERATIONS_LAB_MESSAGES</t>
-  </si>
-  <si>
-    <t>Perform bulk operations in lab messages list</t>
-  </si>
-  <si>
-    <t>Able to perform bulk operations in lab messages list</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_MANAGEMENT_ACCESS</t>
-  </si>
-  <si>
-    <t>Access the travel entry directory</t>
-  </si>
-  <si>
-    <t>Able to access the travel entry directory</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_VIEW</t>
-  </si>
-  <si>
-    <t>View existing travel entries</t>
-  </si>
-  <si>
-    <t>Able to view existing travel entries</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_CREATE</t>
-  </si>
-  <si>
-    <t>Create new travel entries</t>
-  </si>
-  <si>
-    <t>Able to create new travel entries</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_EDIT</t>
-  </si>
-  <si>
-    <t>Edit existing travel entries</t>
-  </si>
-  <si>
-    <t>Able to edit existing travel entries</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_DELETE</t>
-  </si>
-  <si>
-    <t>Delete travel entries from the system</t>
-  </si>
-  <si>
-    <t>Able to delete travel entries from the system</t>
-  </si>
-  <si>
-    <t>TRAVEL_ENTRY_ARCHIVE</t>
-  </si>
-  <si>
-    <t>Archive travel entries</t>
-  </si>
-  <si>
-    <t>Able to archive travel entries</t>
-  </si>
-  <si>
-    <t>EXPORT_DATA_PROTECTION_DATA</t>
-  </si>
-  <si>
-    <t>Export data protection data</t>
-  </si>
-  <si>
-    <t>Able to export data protection data</t>
-  </si>
-  <si>
-    <t>OUTBREAK_VIEW</t>
-  </si>
-  <si>
-    <t>View outbreaks</t>
-  </si>
-  <si>
-    <t>Able to view outbreaks</t>
-  </si>
-  <si>
-    <t>OUTBREAK_EDIT</t>
-  </si>
-  <si>
-    <t>Edit outbreaks</t>
-  </si>
-  <si>
-    <t>Able to edit outbreaks</t>
-  </si>
-  <si>
-    <t>SORMAS_REST</t>
-  </si>
-  <si>
-    <t>Access Sormas REST</t>
-  </si>
-  <si>
-    <t>Able to access the SORMAS REST interface</t>
-  </si>
-  <si>
-    <t>SORMAS_UI</t>
-  </si>
-  <si>
-    <t>Access Sormas UI</t>
-  </si>
-  <si>
-    <t>Able to access the SORMAS graphical user interface</t>
-  </si>
-  <si>
-    <t>SORMAS_TO_SORMAS_CLIENT</t>
   </si>
   <si>
     <t>Techincal user right for the SORMAS to SORMAS interface</t>
@@ -1886,79 +1889,79 @@
         <v>33</v>
       </c>
       <c r="F2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s" s="3">
         <v>34</v>
       </c>
-      <c r="G2" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s" s="3">
+      <c r="I2" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="J2" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s" s="3">
         <v>36</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="N2" t="s" s="3">
         <v>37</v>
       </c>
-      <c r="K2" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="N2" t="s" s="3">
-        <v>34</v>
-      </c>
       <c r="O2" t="s" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P2" t="s" s="3">
         <v>34</v>
       </c>
       <c r="Q2" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s" s="3">
         <v>38</v>
       </c>
-      <c r="R2" t="s" s="3">
+      <c r="X2" t="s" s="3">
         <v>39</v>
-      </c>
-      <c r="S2" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="T2" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="V2" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="W2" t="s" s="3">
-        <v>40</v>
-      </c>
-      <c r="X2" t="s" s="3">
-        <v>34</v>
       </c>
       <c r="Y2" t="s" s="3">
         <v>33</v>
       </c>
       <c r="Z2" t="s" s="3">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AA2" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AB2" t="s" s="3">
         <v>33</v>
       </c>
       <c r="AC2" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD2" t="s" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
@@ -2004,11 +2007,11 @@
       <c r="N3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>44</v>
+      <c r="O3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>45</v>
@@ -2057,11 +2060,11 @@
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>44</v>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>44</v>
@@ -2093,11 +2096,11 @@
       <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>44</v>
+      <c r="O4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>45</v>
@@ -2182,11 +2185,11 @@
       <c r="N5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>44</v>
+      <c r="O5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>45</v>
@@ -2342,11 +2345,11 @@
       <c r="H7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>45</v>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>45</v>
@@ -2538,11 +2541,11 @@
       <c r="N9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>44</v>
+      <c r="O9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>44</v>
@@ -2716,11 +2719,11 @@
       <c r="N11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>44</v>
+      <c r="O11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>45</v>
@@ -2965,11 +2968,11 @@
       <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>45</v>
+      <c r="I14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>45</v>
@@ -2983,11 +2986,11 @@
       <c r="N14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>44</v>
+      <c r="O14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>44</v>
@@ -3054,11 +3057,11 @@
       <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>45</v>
+      <c r="I15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>45</v>
@@ -3428,11 +3431,11 @@
       <c r="N19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>44</v>
+      <c r="O19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>45</v>
@@ -3517,11 +3520,11 @@
       <c r="N20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>44</v>
+      <c r="O20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>45</v>
@@ -3606,11 +3609,11 @@
       <c r="N21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>44</v>
+      <c r="O21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>45</v>
@@ -3873,11 +3876,11 @@
       <c r="N24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>44</v>
+      <c r="O24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>45</v>
@@ -3962,11 +3965,11 @@
       <c r="N25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>44</v>
+      <c r="O25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>45</v>
@@ -4318,11 +4321,11 @@
       <c r="N29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>44</v>
+      <c r="O29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>45</v>
@@ -4852,11 +4855,11 @@
       <c r="N35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>44</v>
+      <c r="O35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>44</v>
@@ -5742,11 +5745,11 @@
       <c r="N45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>44</v>
+      <c r="O45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>45</v>
@@ -6009,11 +6012,11 @@
       <c r="N48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>44</v>
+      <c r="O48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>44</v>
@@ -6365,11 +6368,11 @@
       <c r="N52" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>44</v>
+      <c r="O52" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>44</v>
@@ -7077,11 +7080,11 @@
       <c r="N60" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O60" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P60" s="2" t="s">
-        <v>44</v>
+      <c r="O60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q60" s="2" t="s">
         <v>44</v>
@@ -7148,11 +7151,11 @@
       <c r="H61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>45</v>
+      <c r="I61" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>45</v>
@@ -7166,11 +7169,11 @@
       <c r="N61" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P61" s="2" t="s">
-        <v>44</v>
+      <c r="O61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q61" s="2" t="s">
         <v>44</v>
@@ -7415,11 +7418,11 @@
       <c r="H64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>45</v>
+      <c r="I64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>45</v>
@@ -7433,11 +7436,11 @@
       <c r="N64" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O64" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P64" s="2" t="s">
-        <v>44</v>
+      <c r="O64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q64" s="2" t="s">
         <v>44</v>
@@ -8056,11 +8059,11 @@
       <c r="N71" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O71" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P71" s="2" t="s">
-        <v>44</v>
+      <c r="O71" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q71" s="1" t="s">
         <v>45</v>
@@ -8305,11 +8308,11 @@
       <c r="H74" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I74" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>45</v>
+      <c r="I74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>45</v>
@@ -8323,11 +8326,11 @@
       <c r="N74" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>44</v>
+      <c r="O74" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q74" s="2" t="s">
         <v>44</v>
@@ -8857,11 +8860,11 @@
       <c r="N80" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O80" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P80" s="2" t="s">
-        <v>44</v>
+      <c r="O80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q80" s="1" t="s">
         <v>45</v>
@@ -9124,11 +9127,11 @@
       <c r="N83" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O83" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P83" s="2" t="s">
-        <v>44</v>
+      <c r="O83" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q83" s="1" t="s">
         <v>45</v>
@@ -10174,11 +10177,11 @@
       <c r="H95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I95" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>45</v>
+      <c r="I95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>45</v>
@@ -10192,11 +10195,11 @@
       <c r="N95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O95" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P95" s="2" t="s">
-        <v>44</v>
+      <c r="O95" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q95" s="2" t="s">
         <v>44</v>
@@ -10263,11 +10266,11 @@
       <c r="H96" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I96" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>45</v>
+      <c r="I96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>45</v>
@@ -10281,11 +10284,11 @@
       <c r="N96" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O96" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P96" s="2" t="s">
-        <v>44</v>
+      <c r="O96" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q96" s="2" t="s">
         <v>44</v>
@@ -11153,11 +11156,11 @@
       <c r="H106" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I106" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J106" s="1" t="s">
-        <v>45</v>
+      <c r="I106" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>45</v>
@@ -11242,11 +11245,11 @@
       <c r="H107" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I107" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>45</v>
+      <c r="I107" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>45</v>
@@ -11509,11 +11512,11 @@
       <c r="H110" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I110" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>45</v>
+      <c r="I110" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>45</v>
@@ -11527,11 +11530,11 @@
       <c r="N110" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O110" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P110" s="2" t="s">
-        <v>44</v>
+      <c r="O110" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P110" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q110" s="1" t="s">
         <v>45</v>
@@ -11776,11 +11779,11 @@
       <c r="H113" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I113" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J113" s="1" t="s">
-        <v>45</v>
+      <c r="I113" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>44</v>
@@ -11883,11 +11886,11 @@
       <c r="N114" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O114" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P114" s="2" t="s">
-        <v>44</v>
+      <c r="O114" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q114" s="2" t="s">
         <v>44</v>
@@ -13040,11 +13043,11 @@
       <c r="N127" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O127" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P127" s="2" t="s">
-        <v>44</v>
+      <c r="O127" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q127" s="1" t="s">
         <v>45</v>
@@ -13645,11 +13648,11 @@
       <c r="H134" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I134" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J134" s="1" t="s">
-        <v>45</v>
+      <c r="I134" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>45</v>
@@ -13805,17 +13808,17 @@
       <c r="B136" t="s">
         <v>440</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>44</v>
+      <c r="C136" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>44</v>
@@ -13841,11 +13844,11 @@
       <c r="N136" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O136" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P136" s="2" t="s">
-        <v>44</v>
+      <c r="O136" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q136" s="1" t="s">
         <v>45</v>
@@ -13894,17 +13897,17 @@
       <c r="B137" t="s">
         <v>443</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>44</v>
+      <c r="C137" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>44</v>
@@ -13983,17 +13986,17 @@
       <c r="B138" t="s">
         <v>446</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>44</v>
+      <c r="C138" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>44</v>
@@ -14019,11 +14022,11 @@
       <c r="N138" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O138" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P138" s="2" t="s">
-        <v>44</v>
+      <c r="O138" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q138" s="1" t="s">
         <v>45</v>
@@ -14072,17 +14075,17 @@
       <c r="B139" t="s">
         <v>449</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>44</v>
+      <c r="C139" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>44</v>
@@ -14179,11 +14182,11 @@
       <c r="H140" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I140" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J140" s="1" t="s">
-        <v>45</v>
+      <c r="I140" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J140" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>44</v>
@@ -14535,11 +14538,11 @@
       <c r="H144" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I144" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J144" s="1" t="s">
-        <v>45</v>
+      <c r="I144" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J144" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>44</v>
@@ -14624,11 +14627,11 @@
       <c r="H145" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I145" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J145" s="1" t="s">
-        <v>45</v>
+      <c r="I145" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>44</v>
@@ -14891,11 +14894,11 @@
       <c r="H148" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I148" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J148" s="1" t="s">
-        <v>45</v>
+      <c r="I148" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J148" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>44</v>
@@ -14962,11 +14965,11 @@
       <c r="B149" t="s">
         <v>479</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>45</v>
+      <c r="C149" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>44</v>
@@ -15069,11 +15072,11 @@
       <c r="H150" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I150" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J150" s="1" t="s">
-        <v>45</v>
+      <c r="I150" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J150" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>45</v>
@@ -15354,11 +15357,11 @@
       <c r="N153" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O153" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P153" s="2" t="s">
-        <v>44</v>
+      <c r="O153" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P153" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q153" s="1" t="s">
         <v>45</v>
@@ -15443,11 +15446,11 @@
       <c r="N154" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O154" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P154" s="2" t="s">
-        <v>44</v>
+      <c r="O154" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P154" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q154" s="1" t="s">
         <v>45</v>
@@ -15532,11 +15535,11 @@
       <c r="N155" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O155" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P155" s="2" t="s">
-        <v>44</v>
+      <c r="O155" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q155" s="1" t="s">
         <v>45</v>
@@ -15621,11 +15624,11 @@
       <c r="N156" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O156" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P156" s="2" t="s">
-        <v>44</v>
+      <c r="O156" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P156" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="Q156" s="1" t="s">
         <v>45</v>
@@ -15959,11 +15962,11 @@
       <c r="H160" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I160" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J160" s="1" t="s">
-        <v>45</v>
+      <c r="I160" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J160" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>45</v>
@@ -16137,11 +16140,11 @@
       <c r="H162" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I162" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J162" s="2" t="s">
-        <v>44</v>
+      <c r="I162" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>44</v>
@@ -16226,11 +16229,11 @@
       <c r="H163" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I163" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J163" s="1" t="s">
-        <v>45</v>
+      <c r="I163" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J163" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>45</v>
@@ -16295,13 +16298,13 @@
         <v>523</v>
       </c>
       <c r="B164" t="s">
-        <v>28</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>44</v>
+        <v>524</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>44</v>
@@ -16381,10 +16384,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="3">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B165" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>44</v>
@@ -16392,11 +16395,11 @@
       <c r="D165" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E165" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>44</v>
+      <c r="E165" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>44</v>
@@ -16470,10 +16473,10 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="3">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B166" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>44</v>
@@ -16572,12 +16575,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>